<commit_message>
refactor: refactored the code
</commit_message>
<xml_diff>
--- a/inputs/Health-RI-Metadata_CoreGenericHealth_v2-0-0.xlsx
+++ b/inputs/Health-RI-Metadata_CoreGenericHealth_v2-0-0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10810"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexanderharms/Documents/Projects/Metadata automation/metadata-automation/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33085A69-C88B-E841-B58B-FC616A8A244B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E40607F6-6B97-5648-A910-3B152AE7BABC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="20960" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36000" yWindow="-4920" windowWidth="34360" windowHeight="20540" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="14" r:id="rId1"/>
@@ -37,7 +37,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Agent!$A$1:$J$9</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">Catalogue!$A$1:$J$24</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">DataService!$A$1:$J$23</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Dataset!$A$1:$J$53</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Dataset!$A$1:$J$49</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">DatasetSeries!$A$1:$L$15</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">Distribution!$A$1:$J$23</definedName>
   </definedNames>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1885" uniqueCount="674">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2071" uniqueCount="727">
   <si>
     <t>Property label</t>
   </si>
@@ -2174,9 +2174,6 @@
     <t>dcat</t>
   </si>
   <si>
-    <t>dcterms</t>
-  </si>
-  <si>
     <t>xsd</t>
   </si>
   <si>
@@ -2349,6 +2346,168 @@
   </si>
   <si>
     <t>import_classes</t>
+  </si>
+  <si>
+    <t>dct</t>
+  </si>
+  <si>
+    <t>spdx</t>
+  </si>
+  <si>
+    <t>http://spdx.org/rdf/terms#</t>
+  </si>
+  <si>
+    <t>owl</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/2002/07/owl#</t>
+  </si>
+  <si>
+    <t>disco</t>
+  </si>
+  <si>
+    <t>skosthes</t>
+  </si>
+  <si>
+    <t>rdfs</t>
+  </si>
+  <si>
+    <t>qb</t>
+  </si>
+  <si>
+    <t>healthdcatap</t>
+  </si>
+  <si>
+    <t>doap</t>
+  </si>
+  <si>
+    <t>sh</t>
+  </si>
+  <si>
+    <t>euvoc</t>
+  </si>
+  <si>
+    <t>hri</t>
+  </si>
+  <si>
+    <t>dcatap</t>
+  </si>
+  <si>
+    <t>org</t>
+  </si>
+  <si>
+    <t>skosxl</t>
+  </si>
+  <si>
+    <t>dc</t>
+  </si>
+  <si>
+    <t>rdf</t>
+  </si>
+  <si>
+    <t>http://rdf-vocabulary.ddialliance.org/discovery#</t>
+  </si>
+  <si>
+    <t>http://purl.org/iso25964/skos-thes#</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/2004/02/skos/core#</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/2000/01/rdf-schema#</t>
+  </si>
+  <si>
+    <t>http://purl.org/linked-data/cube#</t>
+  </si>
+  <si>
+    <t>http://healthdataportal.eu/ns/health#</t>
+  </si>
+  <si>
+    <t>http://usefulinc.com/ns/doap#</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/ns/shacl#</t>
+  </si>
+  <si>
+    <t>http://publications.europa.eu/ontology/euvoc#</t>
+  </si>
+  <si>
+    <t>http://data.health-ri.nl/core/p2/</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/r5r/</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/ns/org#</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/2008/05/skos-xl#</t>
+  </si>
+  <si>
+    <t>http://www.w3.org/1999/02/22-rdf-syntax-ns#</t>
+  </si>
+  <si>
+    <t>http://purl.org/dc/elements/1.1/</t>
+  </si>
+  <si>
+    <t>skos</t>
+  </si>
+  <si>
+    <t>hri:Agent</t>
+  </si>
+  <si>
+    <t>target_ontology_name</t>
+  </si>
+  <si>
+    <t>hri:Kind</t>
+  </si>
+  <si>
+    <t>Dataset</t>
+  </si>
+  <si>
+    <t>hri:Dataset</t>
+  </si>
+  <si>
+    <t>dash:EnumSelectEditor</t>
+  </si>
+  <si>
+    <t>dash:BlankNodeEditor</t>
+  </si>
+  <si>
+    <t>dash:DetailsViewer</t>
+  </si>
+  <si>
+    <t>dash:TextFieldEditor</t>
+  </si>
+  <si>
+    <t>dash:DateTimePickerEditor</t>
+  </si>
+  <si>
+    <t>dash:LabelViewer</t>
+  </si>
+  <si>
+    <t>HRIKind</t>
+  </si>
+  <si>
+    <t>HRIAgent</t>
+  </si>
+  <si>
+    <t>HRIIdentifier</t>
+  </si>
+  <si>
+    <t>HRIAttribution</t>
+  </si>
+  <si>
+    <t>HRIRelation</t>
+  </si>
+  <si>
+    <t>HRIQualityCertificate</t>
+  </si>
+  <si>
+    <t>HRIPeriodOfTime</t>
+  </si>
+  <si>
+    <t>hri:Kind,hri:Agent</t>
   </si>
 </sst>
 </file>
@@ -2783,7 +2942,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="51" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="232">
+  <cellXfs count="234">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -3415,48 +3574,54 @@
     <xf numFmtId="0" fontId="50" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="51" fillId="12" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -8605,7 +8770,7 @@
       <c r="I6" s="224" t="s">
         <v>19</v>
       </c>
-      <c r="J6" s="217" t="s">
+      <c r="J6" s="219" t="s">
         <v>30</v>
       </c>
       <c r="K6" s="225" t="s">
@@ -8625,7 +8790,7 @@
       <c r="G7" s="226"/>
       <c r="H7" s="226"/>
       <c r="I7" s="224"/>
-      <c r="J7" s="217"/>
+      <c r="J7" s="219"/>
       <c r="K7" s="225"/>
       <c r="L7" s="224"/>
     </row>
@@ -8641,7 +8806,7 @@
       <c r="G8" s="226"/>
       <c r="H8" s="226"/>
       <c r="I8" s="224"/>
-      <c r="J8" s="217"/>
+      <c r="J8" s="219"/>
       <c r="K8" s="225"/>
       <c r="L8" s="224"/>
     </row>
@@ -8657,7 +8822,7 @@
       <c r="G9" s="226"/>
       <c r="H9" s="226"/>
       <c r="I9" s="224"/>
-      <c r="J9" s="217"/>
+      <c r="J9" s="219"/>
       <c r="K9" s="225"/>
       <c r="L9" s="224"/>
     </row>
@@ -8673,7 +8838,7 @@
       <c r="G10" s="226"/>
       <c r="H10" s="226"/>
       <c r="I10" s="224"/>
-      <c r="J10" s="217"/>
+      <c r="J10" s="219"/>
       <c r="K10" s="225"/>
       <c r="L10" s="224"/>
     </row>
@@ -13228,10 +13393,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F1189FF-E617-AB44-8E2D-7CBBF26DD393}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13248,96 +13413,240 @@
       <c r="A2" t="s">
         <v>613</v>
       </c>
-      <c r="B2" s="230" t="s">
-        <v>625</v>
+      <c r="B2" s="217" t="s">
+        <v>624</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>614</v>
       </c>
-      <c r="B3" s="230" t="s">
-        <v>626</v>
+      <c r="B3" s="217" t="s">
+        <v>625</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>615</v>
-      </c>
-      <c r="B4" s="230" t="s">
-        <v>627</v>
+        <v>673</v>
+      </c>
+      <c r="B4" s="217" t="s">
+        <v>626</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>616</v>
-      </c>
-      <c r="B5" s="230" t="s">
-        <v>628</v>
+        <v>615</v>
+      </c>
+      <c r="B5" s="217" t="s">
+        <v>627</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>617</v>
-      </c>
-      <c r="B6" s="230" t="s">
-        <v>629</v>
+        <v>616</v>
+      </c>
+      <c r="B6" s="217" t="s">
+        <v>628</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>618</v>
-      </c>
-      <c r="B7" s="230" t="s">
-        <v>630</v>
+        <v>617</v>
+      </c>
+      <c r="B7" s="217" t="s">
+        <v>629</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>619</v>
-      </c>
-      <c r="B8" s="230" t="s">
-        <v>631</v>
+        <v>618</v>
+      </c>
+      <c r="B8" s="217" t="s">
+        <v>630</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>620</v>
-      </c>
-      <c r="B9" s="230" t="s">
-        <v>632</v>
+        <v>619</v>
+      </c>
+      <c r="B9" s="217" t="s">
+        <v>631</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>621</v>
-      </c>
-      <c r="B10" s="230" t="s">
-        <v>633</v>
+        <v>620</v>
+      </c>
+      <c r="B10" s="217" t="s">
+        <v>632</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>622</v>
-      </c>
-      <c r="B11" s="230" t="s">
-        <v>634</v>
+        <v>621</v>
+      </c>
+      <c r="B11" s="217" t="s">
+        <v>633</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>623</v>
-      </c>
-      <c r="B12" s="230" t="s">
-        <v>635</v>
+        <v>622</v>
+      </c>
+      <c r="B12" s="217" t="s">
+        <v>634</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>624</v>
-      </c>
-      <c r="B13" s="230" t="s">
-        <v>636</v>
+        <v>623</v>
+      </c>
+      <c r="B13" s="217" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>674</v>
+      </c>
+      <c r="B14" s="217" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>676</v>
+      </c>
+      <c r="B15" s="217" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>678</v>
+      </c>
+      <c r="B16" s="217" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>615</v>
+      </c>
+      <c r="B17" s="217" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>679</v>
+      </c>
+      <c r="B18" s="217" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>707</v>
+      </c>
+      <c r="B19" s="217" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>680</v>
+      </c>
+      <c r="B20" s="217" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>681</v>
+      </c>
+      <c r="B21" s="217" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>682</v>
+      </c>
+      <c r="B22" s="217" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>683</v>
+      </c>
+      <c r="B23" s="217" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>684</v>
+      </c>
+      <c r="B24" s="217" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>685</v>
+      </c>
+      <c r="B25" s="217" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>686</v>
+      </c>
+      <c r="B26" s="217" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>687</v>
+      </c>
+      <c r="B27" s="217" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>688</v>
+      </c>
+      <c r="B28" s="217" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>689</v>
+      </c>
+      <c r="B29" s="217" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>691</v>
+      </c>
+      <c r="B30" s="217" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>690</v>
+      </c>
+      <c r="B31" s="217" t="s">
+        <v>706</v>
       </c>
     </row>
   </sheetData>
@@ -13354,6 +13663,24 @@
     <hyperlink ref="B11" r:id="rId10" xr:uid="{EAE8384A-D39A-8945-973B-48344CF01E00}"/>
     <hyperlink ref="B12" r:id="rId11" xr:uid="{B8A8D85F-33A0-0C4B-9A89-DE7DE905FE65}"/>
     <hyperlink ref="B13" r:id="rId12" xr:uid="{8478CF07-8EE7-F944-8BB6-EE594885E3D7}"/>
+    <hyperlink ref="B14" r:id="rId13" xr:uid="{71E575CD-2D8C-0749-8D65-87F5B775A661}"/>
+    <hyperlink ref="B15" r:id="rId14" xr:uid="{1435ED8E-5FED-7448-B02E-5DE2EF1297F2}"/>
+    <hyperlink ref="B16" r:id="rId15" xr:uid="{B96FA7C6-52C3-C942-8C65-D6DC2CDC9F1B}"/>
+    <hyperlink ref="B17" r:id="rId16" xr:uid="{DE43ED45-C3E1-9148-A0DD-DF15569B21E6}"/>
+    <hyperlink ref="B18" r:id="rId17" xr:uid="{2EEE5FF0-8463-BE4E-839E-5A245CDB1620}"/>
+    <hyperlink ref="B19" r:id="rId18" xr:uid="{65ECF204-BE44-3D45-A5C0-4067DD603080}"/>
+    <hyperlink ref="B20" r:id="rId19" xr:uid="{9AE022BA-CF35-4A40-9985-944F0B5C363C}"/>
+    <hyperlink ref="B21" r:id="rId20" xr:uid="{662A6D97-5C21-2C49-9C05-60E4375F45AF}"/>
+    <hyperlink ref="B22" r:id="rId21" xr:uid="{86415B6A-25F8-A148-A14B-42AC5F1CF2F6}"/>
+    <hyperlink ref="B23" r:id="rId22" xr:uid="{B75239CC-836A-B648-BDAF-15856A345C5A}"/>
+    <hyperlink ref="B24" r:id="rId23" xr:uid="{5F291806-1D6E-8E41-9037-771C74CC1018}"/>
+    <hyperlink ref="B25" r:id="rId24" xr:uid="{C2681AE1-A1B0-6947-A48C-7E5980CFB909}"/>
+    <hyperlink ref="B26" r:id="rId25" xr:uid="{934E76D2-8B57-0545-98A1-87978EE40126}"/>
+    <hyperlink ref="B27" r:id="rId26" xr:uid="{147C3E47-EB40-B14A-8B4E-54ADC4B536E9}"/>
+    <hyperlink ref="B28" r:id="rId27" xr:uid="{67DED638-26EF-1F46-9FCA-AFFCEE447A8C}"/>
+    <hyperlink ref="B29" r:id="rId28" xr:uid="{7679A33F-D9A8-1E4D-9794-A6F18E87CD85}"/>
+    <hyperlink ref="B30" r:id="rId29" xr:uid="{5E4D6351-641B-DB46-B485-B03E357151B3}"/>
+    <hyperlink ref="B31" r:id="rId30" xr:uid="{03F5C7D9-B7B1-B849-B1A8-C69532B79FD4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13361,19 +13688,23 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD28D2AD-F644-014B-AA60-BBFA3B19D155}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="13.83203125" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" customWidth="1"/>
+    <col min="4" max="4" width="15.5" customWidth="1"/>
     <col min="6" max="6" width="20.33203125" customWidth="1"/>
+    <col min="7" max="7" width="12.5" customWidth="1"/>
+    <col min="8" max="8" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>610</v>
       </c>
@@ -13384,44 +13715,67 @@
         <v>612</v>
       </c>
       <c r="D1" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="E1" t="s">
         <v>71</v>
       </c>
       <c r="F1" t="s">
+        <v>656</v>
+      </c>
+      <c r="G1" t="s">
         <v>657</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>637</v>
+      </c>
+      <c r="B2" t="s">
+        <v>710</v>
+      </c>
+      <c r="F2" s="217" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>638</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="G2" t="s">
+        <v>659</v>
+      </c>
+      <c r="H2" t="s">
         <v>60</v>
       </c>
-      <c r="F2" s="230" t="s">
-        <v>659</v>
-      </c>
-      <c r="G2" t="s">
-        <v>660</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="B3" t="s">
+        <v>708</v>
+      </c>
+      <c r="F3" s="217" t="s">
+        <v>670</v>
+      </c>
+      <c r="G3" t="s">
+        <v>671</v>
+      </c>
+      <c r="H3" t="s">
         <v>68</v>
       </c>
-      <c r="F3" s="230" t="s">
-        <v>671</v>
-      </c>
-      <c r="G3" t="s">
-        <v>672</v>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>711</v>
+      </c>
+      <c r="B4" t="s">
+        <v>712</v>
+      </c>
+      <c r="D4" t="s">
+        <v>726</v>
+      </c>
+      <c r="H4" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -13440,9 +13794,9 @@
   </sheetPr>
   <dimension ref="A1:R57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
+      <selection pane="bottomLeft" activeCell="M1" sqref="M1:R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13500,23 +13854,23 @@
       <c r="L1" s="108" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="231" t="s">
+      <c r="M1" s="218" t="s">
+        <v>638</v>
+      </c>
+      <c r="N1" s="218" t="s">
         <v>639</v>
       </c>
-      <c r="N1" s="231" t="s">
+      <c r="O1" s="218" t="s">
         <v>640</v>
       </c>
-      <c r="O1" s="231" t="s">
+      <c r="P1" s="218" t="s">
         <v>641</v>
       </c>
-      <c r="P1" s="231" t="s">
+      <c r="Q1" s="218" t="s">
         <v>642</v>
       </c>
-      <c r="Q1" s="231" t="s">
+      <c r="R1" s="218" t="s">
         <v>643</v>
-      </c>
-      <c r="R1" s="231" t="s">
-        <v>644</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="32" x14ac:dyDescent="0.2">
@@ -13551,22 +13905,22 @@
       <c r="K2" s="164"/>
       <c r="L2" s="107"/>
       <c r="M2" s="137" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="N2" s="137" t="s">
         <v>608</v>
       </c>
       <c r="O2" s="137" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="P2" s="137" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="Q2" s="137" t="s">
         <v>608</v>
       </c>
       <c r="R2" s="137" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="96" x14ac:dyDescent="0.2">
@@ -13605,22 +13959,22 @@
       </c>
       <c r="L3" s="130"/>
       <c r="M3" s="137" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="N3" s="137" t="s">
         <v>608</v>
       </c>
       <c r="O3" s="137" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="P3" s="137" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="Q3" s="137" t="s">
         <v>608</v>
       </c>
       <c r="R3" s="137" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="112" x14ac:dyDescent="0.2">
@@ -13659,22 +14013,22 @@
       </c>
       <c r="L4" s="107"/>
       <c r="M4" s="137" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="N4" s="137" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="O4" s="137" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="P4" s="137" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="Q4" s="137" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="R4" s="137" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="48" x14ac:dyDescent="0.2">
@@ -13713,22 +14067,22 @@
       </c>
       <c r="L5" s="130"/>
       <c r="M5" s="137" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="N5" s="137" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="O5" s="137" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="P5" s="137" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="Q5" s="137" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="R5" s="137" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="80" x14ac:dyDescent="0.2">
@@ -13765,22 +14119,22 @@
       <c r="K6" s="164"/>
       <c r="L6" s="107"/>
       <c r="M6" s="137" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="N6" s="137" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="O6" s="137" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="P6" s="137" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="Q6" s="137" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="R6" s="137" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="128" x14ac:dyDescent="0.2">
@@ -13817,22 +14171,22 @@
       <c r="K7" s="164"/>
       <c r="L7" s="130"/>
       <c r="M7" s="137" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="N7" s="137" t="s">
         <v>608</v>
       </c>
       <c r="O7" s="137" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="P7" s="137" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="Q7" s="137" t="s">
         <v>608</v>
       </c>
       <c r="R7" s="137" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="32" x14ac:dyDescent="0.2">
@@ -13871,22 +14225,22 @@
       </c>
       <c r="L8" s="107"/>
       <c r="M8" s="137" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="N8" s="137" t="s">
         <v>608</v>
       </c>
       <c r="O8" s="137" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="P8" s="137" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="Q8" s="137" t="s">
         <v>608</v>
       </c>
       <c r="R8" s="137" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="48" x14ac:dyDescent="0.2">
@@ -13925,22 +14279,22 @@
       </c>
       <c r="L9" s="130"/>
       <c r="M9" s="137" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="N9" s="137" t="s">
         <v>608</v>
       </c>
       <c r="O9" s="137" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="P9" s="137" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="Q9" s="137" t="s">
         <v>608</v>
       </c>
       <c r="R9" s="137" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
@@ -14619,9 +14973,9 @@
   </sheetPr>
   <dimension ref="A1:R56"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M1" sqref="M1:R1"/>
+      <selection pane="bottomLeft" activeCell="O1" sqref="O1:Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14684,23 +15038,23 @@
       <c r="L1" s="108" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="231" t="s">
+      <c r="M1" s="218" t="s">
+        <v>638</v>
+      </c>
+      <c r="N1" s="218" t="s">
         <v>639</v>
       </c>
-      <c r="N1" s="231" t="s">
+      <c r="O1" s="218" t="s">
         <v>640</v>
       </c>
-      <c r="O1" s="231" t="s">
+      <c r="P1" s="218" t="s">
         <v>641</v>
       </c>
-      <c r="P1" s="231" t="s">
+      <c r="Q1" s="218" t="s">
         <v>642</v>
       </c>
-      <c r="Q1" s="231" t="s">
+      <c r="R1" s="218" t="s">
         <v>643</v>
-      </c>
-      <c r="R1" s="231" t="s">
-        <v>644</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="64.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -14739,22 +15093,22 @@
       </c>
       <c r="L2" s="137"/>
       <c r="M2" s="84" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="N2" s="84" t="s">
         <v>608</v>
       </c>
       <c r="O2" s="84" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="P2" s="84" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="Q2" s="84" t="s">
         <v>608</v>
       </c>
       <c r="R2" s="84" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="112" x14ac:dyDescent="0.2">
@@ -14793,22 +15147,22 @@
       </c>
       <c r="L3" s="137"/>
       <c r="M3" s="84" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="N3" s="84" t="s">
         <v>608</v>
       </c>
       <c r="O3" s="84" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="P3" s="84" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="Q3" s="84" t="s">
         <v>608</v>
       </c>
       <c r="R3" s="84" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="32" x14ac:dyDescent="0.2">
@@ -14847,22 +15201,22 @@
       </c>
       <c r="L4" s="137"/>
       <c r="M4" s="84" t="s">
+        <v>646</v>
+      </c>
+      <c r="N4" s="84" t="s">
         <v>647</v>
       </c>
-      <c r="N4" s="84" t="s">
-        <v>648</v>
-      </c>
       <c r="O4" s="84" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="P4" s="84" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="Q4" s="84" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="R4" s="84" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
@@ -15605,27 +15959,27 @@
       <c r="L1" s="108" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="231" t="s">
+      <c r="M1" s="218" t="s">
+        <v>638</v>
+      </c>
+      <c r="N1" s="218" t="s">
         <v>639</v>
       </c>
-      <c r="N1" s="231" t="s">
+      <c r="O1" s="218" t="s">
         <v>640</v>
       </c>
-      <c r="O1" s="231" t="s">
+      <c r="P1" s="218" t="s">
         <v>641</v>
       </c>
-      <c r="P1" s="231" t="s">
+      <c r="Q1" s="218" t="s">
         <v>642</v>
       </c>
-      <c r="Q1" s="231" t="s">
+      <c r="R1" s="218" t="s">
         <v>643</v>
       </c>
-      <c r="R1" s="231" t="s">
-        <v>644</v>
-      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="H1:I1 F1">
+  <conditionalFormatting sqref="F1 H1:I1">
     <cfRule type="cellIs" dxfId="178" priority="5" operator="equal">
       <formula>"Optional"</formula>
     </cfRule>
@@ -15669,11 +16023,11 @@
     <tabColor rgb="FFC00000"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L53"/>
+  <dimension ref="A1:R49"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q49" sqref="Q49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15683,17 +16037,22 @@
     <col min="3" max="3" width="28.83203125" style="41" customWidth="1"/>
     <col min="4" max="4" width="22.33203125" style="34" customWidth="1"/>
     <col min="5" max="5" width="68.83203125" style="34" customWidth="1"/>
-    <col min="6" max="6" width="18.33203125" style="32" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.83203125" style="32" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" style="32" customWidth="1"/>
+    <col min="7" max="7" width="22.83203125" style="32" customWidth="1"/>
     <col min="8" max="8" width="13.6640625" style="32" customWidth="1"/>
     <col min="9" max="9" width="17.1640625" style="32" customWidth="1"/>
     <col min="10" max="10" width="24.33203125" style="32" customWidth="1"/>
     <col min="11" max="11" width="23.6640625" style="32" customWidth="1"/>
     <col min="12" max="12" width="31.6640625" style="32" customWidth="1"/>
-    <col min="13" max="16384" width="9.1640625" style="32"/>
+    <col min="13" max="13" width="11" style="32" customWidth="1"/>
+    <col min="14" max="14" width="11.33203125" style="32" customWidth="1"/>
+    <col min="15" max="15" width="18.83203125" style="32" customWidth="1"/>
+    <col min="16" max="16" width="21.33203125" style="32" customWidth="1"/>
+    <col min="17" max="17" width="22" style="32" customWidth="1"/>
+    <col min="18" max="16384" width="9.1640625" style="32"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="202" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" s="202" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A1" s="91" t="s">
         <v>0</v>
       </c>
@@ -15730,8 +16089,26 @@
       <c r="L1" s="108" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="209.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M1" s="218" t="s">
+        <v>638</v>
+      </c>
+      <c r="N1" s="218" t="s">
+        <v>639</v>
+      </c>
+      <c r="O1" s="218" t="s">
+        <v>640</v>
+      </c>
+      <c r="P1" s="218" t="s">
+        <v>641</v>
+      </c>
+      <c r="Q1" s="218" t="s">
+        <v>642</v>
+      </c>
+      <c r="R1" s="218" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="209.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="122" t="s">
         <v>12</v>
       </c>
@@ -15766,8 +16143,17 @@
         <v>21</v>
       </c>
       <c r="L2" s="107"/>
-    </row>
-    <row r="3" spans="1:12" ht="80" x14ac:dyDescent="0.2">
+      <c r="O2" s="32" t="s">
+        <v>648</v>
+      </c>
+      <c r="P2" s="32" t="s">
+        <v>713</v>
+      </c>
+      <c r="Q2" s="32" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="80" x14ac:dyDescent="0.2">
       <c r="A3" s="126" t="s">
         <v>22</v>
       </c>
@@ -15802,8 +16188,17 @@
         <v>31</v>
       </c>
       <c r="L3" s="130"/>
-    </row>
-    <row r="4" spans="1:12" s="118" customFormat="1" ht="144" x14ac:dyDescent="0.2">
+      <c r="O3" s="32" t="s">
+        <v>648</v>
+      </c>
+      <c r="P3" s="32" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q3" s="32" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" s="118" customFormat="1" ht="144" x14ac:dyDescent="0.2">
       <c r="A4" s="132" t="s">
         <v>32</v>
       </c>
@@ -15838,8 +16233,17 @@
         <v>38</v>
       </c>
       <c r="L4" s="107"/>
-    </row>
-    <row r="5" spans="1:12" ht="64" x14ac:dyDescent="0.2">
+      <c r="O4" s="118" t="s">
+        <v>648</v>
+      </c>
+      <c r="P4" s="118" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q4" s="118" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="64" x14ac:dyDescent="0.2">
       <c r="A5" s="126" t="s">
         <v>39</v>
       </c>
@@ -15874,8 +16278,17 @@
         <v>44</v>
       </c>
       <c r="L5" s="130"/>
-    </row>
-    <row r="6" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="O5" s="32" t="s">
+        <v>648</v>
+      </c>
+      <c r="P5" s="32" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q5" s="32" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="122" t="s">
         <v>45</v>
       </c>
@@ -15910,8 +16323,17 @@
         <v>50</v>
       </c>
       <c r="L6" s="107"/>
-    </row>
-    <row r="7" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+      <c r="O6" s="32" t="s">
+        <v>648</v>
+      </c>
+      <c r="P6" s="32" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q6" s="32" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="48" x14ac:dyDescent="0.2">
       <c r="A7" s="126" t="s">
         <v>51</v>
       </c>
@@ -15946,8 +16368,17 @@
         <v>55</v>
       </c>
       <c r="L7" s="130"/>
-    </row>
-    <row r="8" spans="1:12" ht="123.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O7" s="32" t="s">
+        <v>648</v>
+      </c>
+      <c r="P7" s="32" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q7" s="32" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="123.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="122" t="s">
         <v>56</v>
       </c>
@@ -15982,8 +16413,17 @@
         <v>63</v>
       </c>
       <c r="L8" s="107"/>
-    </row>
-    <row r="9" spans="1:12" ht="64" x14ac:dyDescent="0.2">
+      <c r="O8" s="32" t="s">
+        <v>648</v>
+      </c>
+      <c r="P8" s="32" t="s">
+        <v>714</v>
+      </c>
+      <c r="Q8" s="32" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="64" x14ac:dyDescent="0.2">
       <c r="A9" s="126" t="s">
         <v>64</v>
       </c>
@@ -16018,8 +16458,17 @@
         <v>70</v>
       </c>
       <c r="L9" s="130"/>
-    </row>
-    <row r="10" spans="1:12" ht="64" x14ac:dyDescent="0.2">
+      <c r="O9" s="32" t="s">
+        <v>715</v>
+      </c>
+      <c r="P9" s="32" t="s">
+        <v>714</v>
+      </c>
+      <c r="Q9" s="32" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="64" x14ac:dyDescent="0.2">
       <c r="A10" s="122" t="s">
         <v>71</v>
       </c>
@@ -16054,8 +16503,17 @@
         <v>77</v>
       </c>
       <c r="L10" s="107"/>
-    </row>
-    <row r="11" spans="1:12" s="210" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="O10" s="32" t="s">
+        <v>649</v>
+      </c>
+      <c r="P10" s="32" t="s">
+        <v>716</v>
+      </c>
+      <c r="Q10" s="32" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" s="210" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="126" t="s">
         <v>78</v>
       </c>
@@ -16088,8 +16546,17 @@
       </c>
       <c r="K11" s="131"/>
       <c r="L11" s="130"/>
-    </row>
-    <row r="12" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="O11" s="210" t="s">
+        <v>648</v>
+      </c>
+      <c r="P11" s="210" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q11" s="210" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="122" t="s">
         <v>82</v>
       </c>
@@ -16124,8 +16591,17 @@
         <v>87</v>
       </c>
       <c r="L12" s="107"/>
-    </row>
-    <row r="13" spans="1:12" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O12" s="32" t="s">
+        <v>648</v>
+      </c>
+      <c r="P12" s="32" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q12" s="32" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="126" t="s">
         <v>88</v>
       </c>
@@ -16160,126 +16636,258 @@
         <v>94</v>
       </c>
       <c r="L13" s="130"/>
-    </row>
-    <row r="14" spans="1:12" ht="32" x14ac:dyDescent="0.2">
-      <c r="A14" s="220" t="s">
+      <c r="O13" s="32" t="s">
+        <v>648</v>
+      </c>
+      <c r="P13" s="32" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q13" s="32" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="230" t="s">
         <v>95</v>
       </c>
-      <c r="B14" s="221" t="s">
+      <c r="B14" s="231" t="s">
         <v>96</v>
       </c>
-      <c r="C14" s="220" t="s">
+      <c r="C14" s="230" t="s">
         <v>97</v>
       </c>
       <c r="D14" s="154" t="s">
         <v>98</v>
       </c>
-      <c r="E14" s="222" t="s">
+      <c r="E14" s="232" t="s">
         <v>99</v>
       </c>
-      <c r="F14" s="219" t="s">
+      <c r="F14" s="230" t="s">
         <v>27</v>
       </c>
-      <c r="G14" s="219" t="s">
+      <c r="G14" s="230" t="s">
         <v>100</v>
       </c>
-      <c r="H14" s="219" t="s">
+      <c r="H14" s="230" t="s">
         <v>29</v>
       </c>
-      <c r="I14" s="217" t="s">
+      <c r="I14" s="233" t="s">
         <v>19</v>
       </c>
-      <c r="J14" s="217" t="s">
+      <c r="J14" s="233" t="s">
         <v>30</v>
       </c>
-      <c r="K14" s="218"/>
-      <c r="L14" s="217"/>
-    </row>
-    <row r="15" spans="1:12" ht="32" x14ac:dyDescent="0.2">
-      <c r="A15" s="220"/>
-      <c r="B15" s="221"/>
-      <c r="C15" s="220"/>
-      <c r="D15" s="155" t="s">
-        <v>101</v>
-      </c>
-      <c r="E15" s="222"/>
-      <c r="F15" s="219"/>
-      <c r="G15" s="219"/>
-      <c r="H15" s="219"/>
-      <c r="I15" s="217"/>
-      <c r="J15" s="217"/>
-      <c r="K15" s="218"/>
-      <c r="L15" s="217"/>
-    </row>
-    <row r="16" spans="1:12" ht="32" x14ac:dyDescent="0.2">
-      <c r="A16" s="220"/>
-      <c r="B16" s="221"/>
-      <c r="C16" s="220"/>
-      <c r="D16" s="155" t="s">
-        <v>102</v>
-      </c>
-      <c r="E16" s="222"/>
-      <c r="F16" s="219"/>
-      <c r="G16" s="219"/>
-      <c r="H16" s="219"/>
-      <c r="I16" s="217"/>
-      <c r="J16" s="217"/>
-      <c r="K16" s="218"/>
-      <c r="L16" s="217"/>
-    </row>
-    <row r="17" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="220"/>
-      <c r="B17" s="221"/>
-      <c r="C17" s="220"/>
-      <c r="D17" s="155" t="s">
-        <v>103</v>
-      </c>
-      <c r="E17" s="222"/>
-      <c r="F17" s="219"/>
-      <c r="G17" s="219"/>
-      <c r="H17" s="219"/>
-      <c r="I17" s="217"/>
-      <c r="J17" s="217"/>
-      <c r="K17" s="218"/>
-      <c r="L17" s="217"/>
-    </row>
-    <row r="18" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="220"/>
-      <c r="B18" s="221"/>
-      <c r="C18" s="220"/>
-      <c r="D18" s="155" t="s">
-        <v>104</v>
-      </c>
-      <c r="E18" s="222"/>
-      <c r="F18" s="219"/>
-      <c r="G18" s="219"/>
-      <c r="H18" s="219"/>
-      <c r="I18" s="217"/>
-      <c r="J18" s="217"/>
-      <c r="K18" s="218"/>
-      <c r="L18" s="217"/>
-    </row>
-    <row r="19" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="K14" s="158"/>
+      <c r="L14" s="233"/>
+      <c r="O14" s="32" t="s">
+        <v>648</v>
+      </c>
+      <c r="P14" s="32" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q14" s="32" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+      <c r="A15" s="126" t="s">
+        <v>105</v>
+      </c>
+      <c r="B15" s="74" t="s">
+        <v>106</v>
+      </c>
+      <c r="C15" s="126" t="s">
+        <v>107</v>
+      </c>
+      <c r="D15" s="127" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="80" t="s">
+        <v>108</v>
+      </c>
+      <c r="F15" s="128" t="s">
+        <v>27</v>
+      </c>
+      <c r="G15" s="128" t="s">
+        <v>109</v>
+      </c>
+      <c r="H15" s="128" t="s">
+        <v>29</v>
+      </c>
+      <c r="I15" s="130" t="s">
+        <v>19</v>
+      </c>
+      <c r="J15" s="130" t="s">
+        <v>76</v>
+      </c>
+      <c r="K15" s="211" t="s">
+        <v>110</v>
+      </c>
+      <c r="L15" s="130"/>
+      <c r="O15" s="32" t="s">
+        <v>648</v>
+      </c>
+      <c r="P15" s="32" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q15" s="32" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="96" x14ac:dyDescent="0.2">
+      <c r="A16" s="122" t="s">
+        <v>111</v>
+      </c>
+      <c r="B16" s="35" t="s">
+        <v>112</v>
+      </c>
+      <c r="C16" s="122" t="s">
+        <v>113</v>
+      </c>
+      <c r="D16" s="133" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="79" t="s">
+        <v>114</v>
+      </c>
+      <c r="F16" s="125" t="s">
+        <v>27</v>
+      </c>
+      <c r="G16" s="125" t="s">
+        <v>43</v>
+      </c>
+      <c r="H16" s="125" t="s">
+        <v>29</v>
+      </c>
+      <c r="I16" s="107" t="s">
+        <v>19</v>
+      </c>
+      <c r="J16" s="107" t="s">
+        <v>30</v>
+      </c>
+      <c r="K16" s="106" t="s">
+        <v>115</v>
+      </c>
+      <c r="L16" s="107"/>
+      <c r="O16" s="32" t="s">
+        <v>648</v>
+      </c>
+      <c r="P16" s="32" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q16" s="32" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="96" x14ac:dyDescent="0.2">
+      <c r="A17" s="126" t="s">
+        <v>116</v>
+      </c>
+      <c r="B17" s="74" t="s">
+        <v>117</v>
+      </c>
+      <c r="C17" s="126" t="s">
+        <v>118</v>
+      </c>
+      <c r="D17" s="127" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="212" t="s">
+        <v>119</v>
+      </c>
+      <c r="F17" s="128" t="s">
+        <v>17</v>
+      </c>
+      <c r="G17" s="128" t="s">
+        <v>75</v>
+      </c>
+      <c r="H17" s="128">
+        <v>1</v>
+      </c>
+      <c r="I17" s="130" t="s">
+        <v>69</v>
+      </c>
+      <c r="J17" s="130" t="s">
+        <v>62</v>
+      </c>
+      <c r="K17" s="131" t="s">
+        <v>120</v>
+      </c>
+      <c r="L17" s="130"/>
+      <c r="O17" s="32" t="s">
+        <v>649</v>
+      </c>
+      <c r="P17" s="32" t="s">
+        <v>716</v>
+      </c>
+      <c r="Q17" s="32" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="122" t="s">
+        <v>121</v>
+      </c>
+      <c r="B18" s="35" t="s">
+        <v>122</v>
+      </c>
+      <c r="C18" s="122" t="s">
+        <v>123</v>
+      </c>
+      <c r="D18" s="133" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" s="133" t="s">
+        <v>124</v>
+      </c>
+      <c r="F18" s="125" t="s">
+        <v>27</v>
+      </c>
+      <c r="G18" s="125" t="s">
+        <v>125</v>
+      </c>
+      <c r="H18" s="125" t="s">
+        <v>29</v>
+      </c>
+      <c r="I18" s="107" t="s">
+        <v>69</v>
+      </c>
+      <c r="J18" s="107" t="s">
+        <v>76</v>
+      </c>
+      <c r="K18" s="106"/>
+      <c r="L18" s="107"/>
+      <c r="O18" s="32" t="s">
+        <v>648</v>
+      </c>
+      <c r="P18" s="32" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q18" s="32" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="126" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="B19" s="74" t="s">
-        <v>106</v>
+        <v>127</v>
       </c>
       <c r="C19" s="126" t="s">
-        <v>107</v>
+        <v>128</v>
       </c>
       <c r="D19" s="127" t="s">
         <v>25</v>
       </c>
-      <c r="E19" s="80" t="s">
-        <v>108</v>
+      <c r="E19" s="74" t="s">
+        <v>129</v>
       </c>
       <c r="F19" s="128" t="s">
         <v>27</v>
       </c>
       <c r="G19" s="128" t="s">
-        <v>109</v>
+        <v>130</v>
       </c>
       <c r="H19" s="128" t="s">
         <v>29</v>
@@ -16291,248 +16899,313 @@
         <v>76</v>
       </c>
       <c r="K19" s="211" t="s">
-        <v>110</v>
+        <v>131</v>
       </c>
       <c r="L19" s="130"/>
-    </row>
-    <row r="20" spans="1:12" ht="96" x14ac:dyDescent="0.2">
+      <c r="O19" s="32" t="s">
+        <v>648</v>
+      </c>
+      <c r="P19" s="32" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q19" s="32" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A20" s="122" t="s">
-        <v>111</v>
+        <v>132</v>
       </c>
       <c r="B20" s="35" t="s">
-        <v>112</v>
-      </c>
-      <c r="C20" s="122" t="s">
-        <v>113</v>
+        <v>133</v>
+      </c>
+      <c r="C20" s="143" t="s">
+        <v>134</v>
       </c>
       <c r="D20" s="133" t="s">
         <v>25</v>
       </c>
-      <c r="E20" s="79" t="s">
-        <v>114</v>
+      <c r="E20" s="71" t="s">
+        <v>135</v>
       </c>
       <c r="F20" s="125" t="s">
+        <v>17</v>
+      </c>
+      <c r="G20" s="125" t="s">
+        <v>75</v>
+      </c>
+      <c r="H20" s="125" t="s">
+        <v>37</v>
+      </c>
+      <c r="I20" s="107" t="s">
+        <v>61</v>
+      </c>
+      <c r="J20" s="107" t="s">
+        <v>76</v>
+      </c>
+      <c r="K20" s="106" t="s">
+        <v>136</v>
+      </c>
+      <c r="L20" s="107"/>
+      <c r="O20" s="32" t="s">
+        <v>649</v>
+      </c>
+      <c r="P20" s="32" t="s">
+        <v>716</v>
+      </c>
+      <c r="Q20" s="32" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" ht="48" x14ac:dyDescent="0.2">
+      <c r="A21" s="126" t="s">
+        <v>137</v>
+      </c>
+      <c r="B21" s="74" t="s">
+        <v>138</v>
+      </c>
+      <c r="C21" s="135" t="s">
+        <v>139</v>
+      </c>
+      <c r="D21" s="144" t="s">
+        <v>140</v>
+      </c>
+      <c r="E21" s="127" t="s">
+        <v>141</v>
+      </c>
+      <c r="F21" s="128" t="s">
         <v>27</v>
       </c>
-      <c r="G20" s="125" t="s">
-        <v>43</v>
-      </c>
-      <c r="H20" s="125" t="s">
+      <c r="G21" s="128" t="s">
+        <v>142</v>
+      </c>
+      <c r="H21" s="128" t="s">
         <v>29</v>
       </c>
-      <c r="I20" s="107" t="s">
+      <c r="I21" s="130" t="s">
         <v>19</v>
       </c>
-      <c r="J20" s="107" t="s">
-        <v>30</v>
-      </c>
-      <c r="K20" s="106" t="s">
-        <v>115</v>
-      </c>
-      <c r="L20" s="107"/>
-    </row>
-    <row r="21" spans="1:12" ht="96" x14ac:dyDescent="0.2">
-      <c r="A21" s="126" t="s">
-        <v>116</v>
-      </c>
-      <c r="B21" s="74" t="s">
-        <v>117</v>
-      </c>
-      <c r="C21" s="126" t="s">
-        <v>118</v>
-      </c>
-      <c r="D21" s="127" t="s">
-        <v>25</v>
-      </c>
-      <c r="E21" s="212" t="s">
-        <v>119</v>
-      </c>
-      <c r="F21" s="128" t="s">
-        <v>17</v>
-      </c>
-      <c r="G21" s="128" t="s">
-        <v>75</v>
-      </c>
-      <c r="H21" s="128">
-        <v>1</v>
-      </c>
-      <c r="I21" s="130" t="s">
-        <v>69</v>
-      </c>
       <c r="J21" s="130" t="s">
-        <v>62</v>
-      </c>
-      <c r="K21" s="131" t="s">
-        <v>120</v>
+        <v>76</v>
+      </c>
+      <c r="K21" s="213" t="s">
+        <v>143</v>
       </c>
       <c r="L21" s="130"/>
-    </row>
-    <row r="22" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="O21" s="32" t="s">
+        <v>648</v>
+      </c>
+      <c r="P21" s="32" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q21" s="32" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" ht="128" x14ac:dyDescent="0.2">
       <c r="A22" s="122" t="s">
-        <v>121</v>
+        <v>144</v>
       </c>
       <c r="B22" s="35" t="s">
-        <v>122</v>
-      </c>
-      <c r="C22" s="122" t="s">
-        <v>123</v>
-      </c>
-      <c r="D22" s="133" t="s">
-        <v>25</v>
+        <v>145</v>
+      </c>
+      <c r="C22" s="143" t="s">
+        <v>146</v>
+      </c>
+      <c r="D22" s="123" t="s">
+        <v>147</v>
       </c>
       <c r="E22" s="133" t="s">
-        <v>124</v>
+        <v>148</v>
       </c>
       <c r="F22" s="125" t="s">
         <v>27</v>
       </c>
       <c r="G22" s="125" t="s">
-        <v>125</v>
+        <v>149</v>
       </c>
       <c r="H22" s="125" t="s">
         <v>29</v>
       </c>
       <c r="I22" s="107" t="s">
-        <v>69</v>
+        <v>19</v>
       </c>
       <c r="J22" s="107" t="s">
-        <v>76</v>
-      </c>
-      <c r="K22" s="106"/>
+        <v>30</v>
+      </c>
+      <c r="K22" s="106" t="s">
+        <v>150</v>
+      </c>
       <c r="L22" s="107"/>
-    </row>
-    <row r="23" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="O22" s="32" t="s">
+        <v>648</v>
+      </c>
+      <c r="P22" s="32" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q22" s="32" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="126" t="s">
-        <v>126</v>
+        <v>151</v>
       </c>
       <c r="B23" s="74" t="s">
-        <v>127</v>
+        <v>152</v>
       </c>
       <c r="C23" s="126" t="s">
-        <v>128</v>
+        <v>153</v>
       </c>
       <c r="D23" s="127" t="s">
         <v>25</v>
       </c>
-      <c r="E23" s="74" t="s">
-        <v>129</v>
+      <c r="E23" s="127" t="s">
+        <v>154</v>
       </c>
       <c r="F23" s="128" t="s">
         <v>27</v>
       </c>
       <c r="G23" s="128" t="s">
-        <v>130</v>
+        <v>155</v>
       </c>
       <c r="H23" s="128" t="s">
-        <v>29</v>
+        <v>93</v>
       </c>
       <c r="I23" s="130" t="s">
         <v>19</v>
       </c>
       <c r="J23" s="130" t="s">
-        <v>76</v>
-      </c>
-      <c r="K23" s="211" t="s">
-        <v>131</v>
+        <v>30</v>
+      </c>
+      <c r="K23" s="131" t="s">
+        <v>156</v>
       </c>
       <c r="L23" s="130"/>
-    </row>
-    <row r="24" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+      <c r="O23" s="32" t="s">
+        <v>649</v>
+      </c>
+      <c r="P23" s="32" t="s">
+        <v>716</v>
+      </c>
+      <c r="Q23" s="32" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="122" t="s">
-        <v>132</v>
+        <v>157</v>
       </c>
       <c r="B24" s="35" t="s">
-        <v>133</v>
+        <v>158</v>
       </c>
       <c r="C24" s="143" t="s">
-        <v>134</v>
+        <v>159</v>
       </c>
       <c r="D24" s="133" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="71" t="s">
-        <v>135</v>
+      <c r="E24" s="133" t="s">
+        <v>160</v>
       </c>
       <c r="F24" s="125" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="G24" s="125" t="s">
-        <v>75</v>
+        <v>155</v>
       </c>
       <c r="H24" s="125" t="s">
-        <v>37</v>
+        <v>93</v>
       </c>
       <c r="I24" s="107" t="s">
-        <v>61</v>
+        <v>19</v>
       </c>
       <c r="J24" s="107" t="s">
-        <v>76</v>
+        <v>30</v>
       </c>
       <c r="K24" s="106" t="s">
-        <v>136</v>
+        <v>161</v>
       </c>
       <c r="L24" s="107"/>
-    </row>
-    <row r="25" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+      <c r="O24" s="32" t="s">
+        <v>649</v>
+      </c>
+      <c r="P24" s="32" t="s">
+        <v>716</v>
+      </c>
+      <c r="Q24" s="32" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A25" s="126" t="s">
-        <v>137</v>
+        <v>162</v>
       </c>
       <c r="B25" s="74" t="s">
-        <v>138</v>
-      </c>
-      <c r="C25" s="135" t="s">
-        <v>139</v>
-      </c>
-      <c r="D25" s="144" t="s">
-        <v>140</v>
-      </c>
-      <c r="E25" s="127" t="s">
-        <v>141</v>
+        <v>163</v>
+      </c>
+      <c r="C25" s="126" t="s">
+        <v>164</v>
+      </c>
+      <c r="D25" s="127" t="s">
+        <v>25</v>
+      </c>
+      <c r="E25" s="74" t="s">
+        <v>165</v>
       </c>
       <c r="F25" s="128" t="s">
         <v>27</v>
       </c>
       <c r="G25" s="128" t="s">
-        <v>142</v>
+        <v>166</v>
       </c>
       <c r="H25" s="128" t="s">
-        <v>29</v>
+        <v>93</v>
       </c>
       <c r="I25" s="130" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="J25" s="130" t="s">
         <v>76</v>
       </c>
-      <c r="K25" s="213" t="s">
-        <v>143</v>
+      <c r="K25" s="131" t="s">
+        <v>167</v>
       </c>
       <c r="L25" s="130"/>
-    </row>
-    <row r="26" spans="1:12" ht="128" x14ac:dyDescent="0.2">
+      <c r="O25" s="32" t="s">
+        <v>649</v>
+      </c>
+      <c r="P25" s="32" t="s">
+        <v>717</v>
+      </c>
+      <c r="Q25" s="32" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="122" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="B26" s="35" t="s">
-        <v>145</v>
-      </c>
-      <c r="C26" s="143" t="s">
-        <v>146</v>
-      </c>
-      <c r="D26" s="123" t="s">
-        <v>147</v>
+        <v>169</v>
+      </c>
+      <c r="C26" s="122" t="s">
+        <v>170</v>
+      </c>
+      <c r="D26" s="133" t="s">
+        <v>25</v>
       </c>
       <c r="E26" s="133" t="s">
-        <v>148</v>
+        <v>171</v>
       </c>
       <c r="F26" s="125" t="s">
         <v>27</v>
       </c>
       <c r="G26" s="125" t="s">
-        <v>149</v>
+        <v>172</v>
       </c>
       <c r="H26" s="125" t="s">
-        <v>29</v>
+        <v>93</v>
       </c>
       <c r="I26" s="107" t="s">
         <v>19</v>
@@ -16541,31 +17214,40 @@
         <v>30</v>
       </c>
       <c r="K26" s="106" t="s">
-        <v>150</v>
+        <v>173</v>
       </c>
       <c r="L26" s="107"/>
-    </row>
-    <row r="27" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="O26" s="32" t="s">
+        <v>649</v>
+      </c>
+      <c r="P26" s="32" t="s">
+        <v>716</v>
+      </c>
+      <c r="Q26" s="32" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="126" t="s">
-        <v>151</v>
+        <v>174</v>
       </c>
       <c r="B27" s="74" t="s">
-        <v>152</v>
+        <v>175</v>
       </c>
       <c r="C27" s="126" t="s">
-        <v>153</v>
+        <v>176</v>
       </c>
       <c r="D27" s="127" t="s">
         <v>25</v>
       </c>
-      <c r="E27" s="127" t="s">
-        <v>154</v>
+      <c r="E27" s="74" t="s">
+        <v>177</v>
       </c>
       <c r="F27" s="128" t="s">
         <v>27</v>
       </c>
       <c r="G27" s="128" t="s">
-        <v>155</v>
+        <v>172</v>
       </c>
       <c r="H27" s="128" t="s">
         <v>93</v>
@@ -16577,106 +17259,133 @@
         <v>30</v>
       </c>
       <c r="K27" s="131" t="s">
-        <v>156</v>
+        <v>178</v>
       </c>
       <c r="L27" s="130"/>
-    </row>
-    <row r="28" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="O27" s="32" t="s">
+        <v>649</v>
+      </c>
+      <c r="P27" s="32" t="s">
+        <v>716</v>
+      </c>
+      <c r="Q27" s="32" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A28" s="122" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="B28" s="35" t="s">
-        <v>158</v>
-      </c>
-      <c r="C28" s="143" t="s">
-        <v>159</v>
+        <v>180</v>
+      </c>
+      <c r="C28" s="122" t="s">
+        <v>181</v>
       </c>
       <c r="D28" s="133" t="s">
         <v>25</v>
       </c>
       <c r="E28" s="133" t="s">
-        <v>160</v>
+        <v>182</v>
       </c>
       <c r="F28" s="125" t="s">
         <v>27</v>
       </c>
       <c r="G28" s="125" t="s">
-        <v>155</v>
+        <v>183</v>
       </c>
       <c r="H28" s="125" t="s">
-        <v>93</v>
+        <v>29</v>
       </c>
       <c r="I28" s="107" t="s">
         <v>19</v>
       </c>
       <c r="J28" s="107" t="s">
-        <v>30</v>
+        <v>76</v>
       </c>
       <c r="K28" s="106" t="s">
-        <v>161</v>
+        <v>184</v>
       </c>
       <c r="L28" s="107"/>
-    </row>
-    <row r="29" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+      <c r="O28" s="32" t="s">
+        <v>715</v>
+      </c>
+      <c r="P28" s="32" t="s">
+        <v>714</v>
+      </c>
+      <c r="Q28" s="32" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" ht="64" x14ac:dyDescent="0.2">
       <c r="A29" s="126" t="s">
-        <v>162</v>
+        <v>185</v>
       </c>
       <c r="B29" s="74" t="s">
-        <v>163</v>
+        <v>186</v>
       </c>
       <c r="C29" s="126" t="s">
-        <v>164</v>
-      </c>
-      <c r="D29" s="127" t="s">
-        <v>25</v>
-      </c>
-      <c r="E29" s="74" t="s">
-        <v>165</v>
+        <v>187</v>
+      </c>
+      <c r="D29" s="144" t="s">
+        <v>188</v>
+      </c>
+      <c r="E29" s="80" t="s">
+        <v>189</v>
       </c>
       <c r="F29" s="128" t="s">
         <v>27</v>
       </c>
       <c r="G29" s="128" t="s">
-        <v>166</v>
+        <v>190</v>
       </c>
       <c r="H29" s="128" t="s">
-        <v>93</v>
+        <v>29</v>
       </c>
       <c r="I29" s="130" t="s">
-        <v>61</v>
+        <v>19</v>
       </c>
       <c r="J29" s="130" t="s">
-        <v>76</v>
+        <v>30</v>
       </c>
       <c r="K29" s="131" t="s">
-        <v>167</v>
+        <v>191</v>
       </c>
       <c r="L29" s="130"/>
-    </row>
-    <row r="30" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="O29" s="32" t="s">
+        <v>718</v>
+      </c>
+      <c r="P29" s="32" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q29" s="32" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A30" s="122" t="s">
-        <v>168</v>
+        <v>192</v>
       </c>
       <c r="B30" s="35" t="s">
-        <v>169</v>
+        <v>193</v>
       </c>
       <c r="C30" s="122" t="s">
-        <v>170</v>
+        <v>194</v>
       </c>
       <c r="D30" s="133" t="s">
         <v>25</v>
       </c>
       <c r="E30" s="133" t="s">
-        <v>171</v>
+        <v>195</v>
       </c>
       <c r="F30" s="125" t="s">
         <v>27</v>
       </c>
       <c r="G30" s="125" t="s">
-        <v>172</v>
+        <v>75</v>
       </c>
       <c r="H30" s="125" t="s">
-        <v>93</v>
+        <v>29</v>
       </c>
       <c r="I30" s="107" t="s">
         <v>19</v>
@@ -16685,67 +17394,85 @@
         <v>30</v>
       </c>
       <c r="K30" s="106" t="s">
-        <v>173</v>
+        <v>196</v>
       </c>
       <c r="L30" s="107"/>
-    </row>
-    <row r="31" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="O30" s="32" t="s">
+        <v>649</v>
+      </c>
+      <c r="P30" s="32" t="s">
+        <v>716</v>
+      </c>
+      <c r="Q30" s="32" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" ht="112" x14ac:dyDescent="0.2">
       <c r="A31" s="126" t="s">
-        <v>174</v>
+        <v>197</v>
       </c>
       <c r="B31" s="74" t="s">
-        <v>175</v>
+        <v>198</v>
       </c>
       <c r="C31" s="126" t="s">
-        <v>176</v>
+        <v>199</v>
       </c>
       <c r="D31" s="127" t="s">
         <v>25</v>
       </c>
-      <c r="E31" s="74" t="s">
-        <v>177</v>
+      <c r="E31" s="208" t="s">
+        <v>200</v>
       </c>
       <c r="F31" s="128" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="G31" s="128" t="s">
-        <v>172</v>
-      </c>
-      <c r="H31" s="128" t="s">
-        <v>93</v>
+        <v>68</v>
+      </c>
+      <c r="H31" s="128">
+        <v>1</v>
       </c>
       <c r="I31" s="130" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="J31" s="130" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="K31" s="131" t="s">
-        <v>178</v>
+        <v>201</v>
       </c>
       <c r="L31" s="130"/>
-    </row>
-    <row r="32" spans="1:12" ht="64" x14ac:dyDescent="0.2">
+      <c r="O31" s="32" t="s">
+        <v>715</v>
+      </c>
+      <c r="P31" s="32" t="s">
+        <v>714</v>
+      </c>
+      <c r="Q31" s="32" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A32" s="122" t="s">
-        <v>179</v>
+        <v>202</v>
       </c>
       <c r="B32" s="35" t="s">
-        <v>180</v>
+        <v>203</v>
       </c>
       <c r="C32" s="122" t="s">
-        <v>181</v>
-      </c>
-      <c r="D32" s="133" t="s">
-        <v>25</v>
-      </c>
-      <c r="E32" s="133" t="s">
-        <v>182</v>
+        <v>204</v>
+      </c>
+      <c r="D32" s="123" t="s">
+        <v>205</v>
+      </c>
+      <c r="E32" s="139" t="s">
+        <v>206</v>
       </c>
       <c r="F32" s="125" t="s">
         <v>27</v>
       </c>
       <c r="G32" s="125" t="s">
-        <v>183</v>
+        <v>207</v>
       </c>
       <c r="H32" s="125" t="s">
         <v>29</v>
@@ -16754,34 +17481,43 @@
         <v>19</v>
       </c>
       <c r="J32" s="107" t="s">
-        <v>76</v>
+        <v>30</v>
       </c>
       <c r="K32" s="106" t="s">
-        <v>184</v>
+        <v>208</v>
       </c>
       <c r="L32" s="107"/>
-    </row>
-    <row r="33" spans="1:12" ht="64" x14ac:dyDescent="0.2">
+      <c r="O32" s="32" t="s">
+        <v>718</v>
+      </c>
+      <c r="P32" s="32" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q32" s="32" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" ht="192" x14ac:dyDescent="0.2">
       <c r="A33" s="126" t="s">
-        <v>185</v>
+        <v>209</v>
       </c>
       <c r="B33" s="74" t="s">
-        <v>186</v>
-      </c>
-      <c r="C33" s="126" t="s">
-        <v>187</v>
-      </c>
-      <c r="D33" s="144" t="s">
-        <v>188</v>
-      </c>
-      <c r="E33" s="80" t="s">
-        <v>189</v>
+        <v>210</v>
+      </c>
+      <c r="C33" s="135" t="s">
+        <v>211</v>
+      </c>
+      <c r="D33" s="127" t="s">
+        <v>25</v>
+      </c>
+      <c r="E33" s="127" t="s">
+        <v>212</v>
       </c>
       <c r="F33" s="128" t="s">
         <v>27</v>
       </c>
       <c r="G33" s="128" t="s">
-        <v>190</v>
+        <v>213</v>
       </c>
       <c r="H33" s="128" t="s">
         <v>29</v>
@@ -16792,32 +17528,39 @@
       <c r="J33" s="130" t="s">
         <v>30</v>
       </c>
-      <c r="K33" s="131" t="s">
-        <v>191</v>
-      </c>
+      <c r="K33" s="131"/>
       <c r="L33" s="130"/>
-    </row>
-    <row r="34" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+      <c r="O33" s="32" t="s">
+        <v>715</v>
+      </c>
+      <c r="P33" s="32" t="s">
+        <v>714</v>
+      </c>
+      <c r="Q33" s="32" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A34" s="122" t="s">
-        <v>192</v>
+        <v>214</v>
       </c>
       <c r="B34" s="35" t="s">
-        <v>193</v>
+        <v>215</v>
       </c>
       <c r="C34" s="122" t="s">
-        <v>194</v>
+        <v>216</v>
       </c>
       <c r="D34" s="133" t="s">
         <v>25</v>
       </c>
       <c r="E34" s="133" t="s">
-        <v>195</v>
+        <v>217</v>
       </c>
       <c r="F34" s="125" t="s">
         <v>27</v>
       </c>
       <c r="G34" s="125" t="s">
-        <v>75</v>
+        <v>218</v>
       </c>
       <c r="H34" s="125" t="s">
         <v>29</v>
@@ -16826,109 +17569,134 @@
         <v>19</v>
       </c>
       <c r="J34" s="107" t="s">
-        <v>30</v>
+        <v>76</v>
       </c>
       <c r="K34" s="106" t="s">
-        <v>196</v>
+        <v>219</v>
       </c>
       <c r="L34" s="107"/>
-    </row>
-    <row r="35" spans="1:12" ht="112" x14ac:dyDescent="0.2">
+      <c r="O34" s="32" t="s">
+        <v>715</v>
+      </c>
+      <c r="P34" s="32" t="s">
+        <v>714</v>
+      </c>
+      <c r="Q34" s="32" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A35" s="126" t="s">
-        <v>197</v>
+        <v>220</v>
       </c>
       <c r="B35" s="74" t="s">
-        <v>198</v>
+        <v>221</v>
       </c>
       <c r="C35" s="126" t="s">
-        <v>199</v>
+        <v>222</v>
       </c>
       <c r="D35" s="127" t="s">
         <v>25</v>
       </c>
-      <c r="E35" s="208" t="s">
-        <v>200</v>
+      <c r="E35" s="127" t="s">
+        <v>223</v>
       </c>
       <c r="F35" s="128" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="G35" s="128" t="s">
-        <v>68</v>
-      </c>
-      <c r="H35" s="128">
-        <v>1</v>
+        <v>224</v>
+      </c>
+      <c r="H35" s="128" t="s">
+        <v>29</v>
       </c>
       <c r="I35" s="130" t="s">
-        <v>61</v>
+        <v>19</v>
       </c>
       <c r="J35" s="130" t="s">
-        <v>20</v>
-      </c>
-      <c r="K35" s="131" t="s">
-        <v>201</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="K35" s="131"/>
       <c r="L35" s="130"/>
-    </row>
-    <row r="36" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+      <c r="O35" s="32" t="s">
+        <v>715</v>
+      </c>
+      <c r="P35" s="32" t="s">
+        <v>714</v>
+      </c>
+      <c r="Q35" s="32" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A36" s="122" t="s">
-        <v>202</v>
+        <v>225</v>
       </c>
       <c r="B36" s="35" t="s">
-        <v>203</v>
+        <v>226</v>
       </c>
       <c r="C36" s="122" t="s">
-        <v>204</v>
-      </c>
-      <c r="D36" s="123" t="s">
-        <v>205</v>
-      </c>
-      <c r="E36" s="139" t="s">
-        <v>206</v>
+        <v>227</v>
+      </c>
+      <c r="D36" s="133" t="s">
+        <v>25</v>
+      </c>
+      <c r="E36" s="133" t="s">
+        <v>228</v>
       </c>
       <c r="F36" s="125" t="s">
         <v>27</v>
       </c>
       <c r="G36" s="125" t="s">
-        <v>207</v>
+        <v>166</v>
       </c>
       <c r="H36" s="125" t="s">
-        <v>29</v>
+        <v>93</v>
       </c>
       <c r="I36" s="107" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="J36" s="107" t="s">
-        <v>30</v>
+        <v>76</v>
       </c>
       <c r="K36" s="106" t="s">
-        <v>208</v>
+        <v>229</v>
       </c>
       <c r="L36" s="107"/>
-    </row>
-    <row r="37" spans="1:12" ht="192" x14ac:dyDescent="0.2">
+      <c r="O36" s="32" t="s">
+        <v>649</v>
+      </c>
+      <c r="P36" s="32" t="s">
+        <v>717</v>
+      </c>
+      <c r="Q36" s="32" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A37" s="126" t="s">
-        <v>209</v>
+        <v>230</v>
       </c>
       <c r="B37" s="74" t="s">
-        <v>210</v>
-      </c>
-      <c r="C37" s="135" t="s">
-        <v>211</v>
+        <v>231</v>
+      </c>
+      <c r="C37" s="126" t="s">
+        <v>232</v>
       </c>
       <c r="D37" s="127" t="s">
         <v>25</v>
       </c>
-      <c r="E37" s="127" t="s">
-        <v>212</v>
+      <c r="E37" s="74" t="s">
+        <v>233</v>
       </c>
       <c r="F37" s="128" t="s">
         <v>27</v>
       </c>
       <c r="G37" s="128" t="s">
-        <v>213</v>
+        <v>234</v>
       </c>
       <c r="H37" s="128" t="s">
-        <v>29</v>
+        <v>93</v>
       </c>
       <c r="I37" s="130" t="s">
         <v>19</v>
@@ -16936,30 +17704,41 @@
       <c r="J37" s="130" t="s">
         <v>30</v>
       </c>
-      <c r="K37" s="131"/>
+      <c r="K37" s="131" t="s">
+        <v>235</v>
+      </c>
       <c r="L37" s="130"/>
-    </row>
-    <row r="38" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+      <c r="O37" s="32" t="s">
+        <v>715</v>
+      </c>
+      <c r="P37" s="32" t="s">
+        <v>714</v>
+      </c>
+      <c r="Q37" s="32" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" ht="64" x14ac:dyDescent="0.2">
       <c r="A38" s="122" t="s">
-        <v>214</v>
+        <v>236</v>
       </c>
       <c r="B38" s="35" t="s">
-        <v>215</v>
+        <v>237</v>
       </c>
       <c r="C38" s="122" t="s">
-        <v>216</v>
+        <v>238</v>
       </c>
       <c r="D38" s="133" t="s">
         <v>25</v>
       </c>
       <c r="E38" s="133" t="s">
-        <v>217</v>
+        <v>239</v>
       </c>
       <c r="F38" s="125" t="s">
         <v>27</v>
       </c>
       <c r="G38" s="125" t="s">
-        <v>218</v>
+        <v>28</v>
       </c>
       <c r="H38" s="125" t="s">
         <v>29</v>
@@ -16968,34 +17747,43 @@
         <v>19</v>
       </c>
       <c r="J38" s="107" t="s">
-        <v>76</v>
+        <v>30</v>
       </c>
       <c r="K38" s="106" t="s">
-        <v>219</v>
+        <v>240</v>
       </c>
       <c r="L38" s="107"/>
-    </row>
-    <row r="39" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+      <c r="O38" s="32" t="s">
+        <v>648</v>
+      </c>
+      <c r="P38" s="32" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q38" s="32" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A39" s="126" t="s">
-        <v>220</v>
+        <v>241</v>
       </c>
       <c r="B39" s="74" t="s">
-        <v>221</v>
+        <v>242</v>
       </c>
       <c r="C39" s="126" t="s">
-        <v>222</v>
+        <v>243</v>
       </c>
       <c r="D39" s="127" t="s">
         <v>25</v>
       </c>
-      <c r="E39" s="127" t="s">
-        <v>223</v>
+      <c r="E39" s="80" t="s">
+        <v>244</v>
       </c>
       <c r="F39" s="128" t="s">
         <v>27</v>
       </c>
       <c r="G39" s="128" t="s">
-        <v>224</v>
+        <v>109</v>
       </c>
       <c r="H39" s="128" t="s">
         <v>29</v>
@@ -17004,62 +17792,82 @@
         <v>19</v>
       </c>
       <c r="J39" s="130" t="s">
-        <v>30</v>
-      </c>
-      <c r="K39" s="131"/>
+        <v>76</v>
+      </c>
+      <c r="K39" s="131" t="s">
+        <v>245</v>
+      </c>
       <c r="L39" s="130"/>
-    </row>
-    <row r="40" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="O39" s="32" t="s">
+        <v>648</v>
+      </c>
+      <c r="P39" s="32" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q39" s="32" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" ht="64" x14ac:dyDescent="0.2">
       <c r="A40" s="122" t="s">
-        <v>225</v>
+        <v>246</v>
       </c>
       <c r="B40" s="35" t="s">
-        <v>226</v>
+        <v>247</v>
       </c>
       <c r="C40" s="122" t="s">
-        <v>227</v>
-      </c>
-      <c r="D40" s="133" t="s">
-        <v>25</v>
+        <v>248</v>
+      </c>
+      <c r="D40" s="184" t="s">
+        <v>249</v>
       </c>
       <c r="E40" s="133" t="s">
-        <v>228</v>
+        <v>250</v>
       </c>
       <c r="F40" s="125" t="s">
         <v>27</v>
       </c>
       <c r="G40" s="125" t="s">
-        <v>166</v>
+        <v>43</v>
       </c>
       <c r="H40" s="125" t="s">
         <v>93</v>
       </c>
       <c r="I40" s="107" t="s">
-        <v>61</v>
+        <v>19</v>
       </c>
       <c r="J40" s="107" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="K40" s="106" t="s">
-        <v>229</v>
+        <v>251</v>
       </c>
       <c r="L40" s="107"/>
-    </row>
-    <row r="41" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="O40" s="32" t="s">
+        <v>648</v>
+      </c>
+      <c r="P40" s="32" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q40" s="32" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A41" s="126" t="s">
-        <v>230</v>
+        <v>252</v>
       </c>
       <c r="B41" s="74" t="s">
-        <v>231</v>
+        <v>253</v>
       </c>
       <c r="C41" s="126" t="s">
-        <v>232</v>
+        <v>254</v>
       </c>
       <c r="D41" s="127" t="s">
         <v>25</v>
       </c>
       <c r="E41" s="74" t="s">
-        <v>233</v>
+        <v>255</v>
       </c>
       <c r="F41" s="128" t="s">
         <v>27</v>
@@ -17068,449 +17876,364 @@
         <v>234</v>
       </c>
       <c r="H41" s="128" t="s">
-        <v>93</v>
+        <v>29</v>
       </c>
       <c r="I41" s="130" t="s">
         <v>19</v>
       </c>
       <c r="J41" s="130" t="s">
-        <v>30</v>
+        <v>76</v>
       </c>
       <c r="K41" s="131" t="s">
-        <v>235</v>
+        <v>256</v>
       </c>
       <c r="L41" s="130"/>
-    </row>
-    <row r="42" spans="1:12" ht="64" x14ac:dyDescent="0.2">
+      <c r="O41" s="32" t="s">
+        <v>715</v>
+      </c>
+      <c r="P41" s="32" t="s">
+        <v>714</v>
+      </c>
+      <c r="Q41" s="32" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A42" s="122" t="s">
-        <v>236</v>
+        <v>257</v>
       </c>
       <c r="B42" s="35" t="s">
-        <v>237</v>
-      </c>
-      <c r="C42" s="122" t="s">
-        <v>238</v>
+        <v>258</v>
+      </c>
+      <c r="C42" s="143" t="s">
+        <v>259</v>
       </c>
       <c r="D42" s="133" t="s">
         <v>25</v>
       </c>
       <c r="E42" s="133" t="s">
-        <v>239</v>
+        <v>260</v>
       </c>
       <c r="F42" s="125" t="s">
         <v>27</v>
       </c>
       <c r="G42" s="125" t="s">
-        <v>28</v>
+        <v>261</v>
       </c>
       <c r="H42" s="125" t="s">
-        <v>29</v>
+        <v>93</v>
       </c>
       <c r="I42" s="107" t="s">
         <v>19</v>
       </c>
       <c r="J42" s="107" t="s">
+        <v>62</v>
+      </c>
+      <c r="K42" s="106" t="s">
+        <v>262</v>
+      </c>
+      <c r="L42" s="107"/>
+      <c r="O42" s="32" t="s">
+        <v>649</v>
+      </c>
+      <c r="P42" s="32" t="s">
+        <v>716</v>
+      </c>
+      <c r="Q42" s="32" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="126" t="s">
+        <v>263</v>
+      </c>
+      <c r="B43" s="74" t="s">
+        <v>264</v>
+      </c>
+      <c r="C43" s="126" t="s">
+        <v>265</v>
+      </c>
+      <c r="D43" s="144" t="s">
+        <v>266</v>
+      </c>
+      <c r="E43" s="74" t="s">
+        <v>267</v>
+      </c>
+      <c r="F43" s="128" t="s">
+        <v>17</v>
+      </c>
+      <c r="G43" s="128" t="s">
+        <v>43</v>
+      </c>
+      <c r="H43" s="128" t="s">
+        <v>37</v>
+      </c>
+      <c r="I43" s="130" t="s">
+        <v>69</v>
+      </c>
+      <c r="J43" s="130" t="s">
         <v>30</v>
       </c>
-      <c r="K42" s="106" t="s">
-        <v>240</v>
-      </c>
-      <c r="L42" s="107"/>
-    </row>
-    <row r="43" spans="1:12" ht="32" x14ac:dyDescent="0.2">
-      <c r="A43" s="126" t="s">
-        <v>241</v>
-      </c>
-      <c r="B43" s="74" t="s">
-        <v>242</v>
-      </c>
-      <c r="C43" s="126" t="s">
-        <v>243</v>
-      </c>
-      <c r="D43" s="127" t="s">
+      <c r="K43" s="131" t="s">
+        <v>268</v>
+      </c>
+      <c r="L43" s="130"/>
+      <c r="O43" s="32" t="s">
+        <v>648</v>
+      </c>
+      <c r="P43" s="32" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q43" s="32" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+      <c r="A44" s="122" t="s">
+        <v>269</v>
+      </c>
+      <c r="B44" s="35" t="s">
+        <v>270</v>
+      </c>
+      <c r="C44" s="122" t="s">
+        <v>271</v>
+      </c>
+      <c r="D44" s="133" t="s">
         <v>25</v>
       </c>
-      <c r="E43" s="80" t="s">
-        <v>244</v>
-      </c>
-      <c r="F43" s="128" t="s">
-        <v>27</v>
-      </c>
-      <c r="G43" s="128" t="s">
-        <v>109</v>
-      </c>
-      <c r="H43" s="128" t="s">
-        <v>29</v>
-      </c>
-      <c r="I43" s="130" t="s">
-        <v>19</v>
-      </c>
-      <c r="J43" s="130" t="s">
+      <c r="E44" s="133" t="s">
+        <v>272</v>
+      </c>
+      <c r="F44" s="125" t="s">
+        <v>17</v>
+      </c>
+      <c r="G44" s="125" t="s">
+        <v>75</v>
+      </c>
+      <c r="H44" s="125" t="s">
+        <v>37</v>
+      </c>
+      <c r="I44" s="107" t="s">
+        <v>69</v>
+      </c>
+      <c r="J44" s="107" t="s">
         <v>76</v>
       </c>
-      <c r="K43" s="131" t="s">
-        <v>245</v>
-      </c>
-      <c r="L43" s="130"/>
-    </row>
-    <row r="44" spans="1:12" ht="64" x14ac:dyDescent="0.2">
-      <c r="A44" s="122" t="s">
-        <v>246</v>
-      </c>
-      <c r="B44" s="35" t="s">
-        <v>247</v>
-      </c>
-      <c r="C44" s="122" t="s">
-        <v>248</v>
-      </c>
-      <c r="D44" s="184" t="s">
-        <v>249</v>
-      </c>
-      <c r="E44" s="133" t="s">
-        <v>250</v>
-      </c>
-      <c r="F44" s="125" t="s">
-        <v>27</v>
-      </c>
-      <c r="G44" s="125" t="s">
-        <v>43</v>
-      </c>
-      <c r="H44" s="125" t="s">
-        <v>93</v>
-      </c>
-      <c r="I44" s="107" t="s">
-        <v>19</v>
-      </c>
-      <c r="J44" s="107" t="s">
-        <v>62</v>
-      </c>
       <c r="K44" s="106" t="s">
-        <v>251</v>
+        <v>269</v>
       </c>
       <c r="L44" s="107"/>
-    </row>
-    <row r="45" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="O44" s="32" t="s">
+        <v>649</v>
+      </c>
+      <c r="P44" s="32" t="s">
+        <v>716</v>
+      </c>
+      <c r="Q44" s="32" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" ht="64" x14ac:dyDescent="0.2">
       <c r="A45" s="126" t="s">
-        <v>252</v>
+        <v>273</v>
       </c>
       <c r="B45" s="74" t="s">
-        <v>253</v>
+        <v>274</v>
       </c>
       <c r="C45" s="126" t="s">
-        <v>254</v>
-      </c>
-      <c r="D45" s="127" t="s">
-        <v>25</v>
-      </c>
-      <c r="E45" s="74" t="s">
-        <v>255</v>
+        <v>275</v>
+      </c>
+      <c r="D45" s="188" t="s">
+        <v>276</v>
+      </c>
+      <c r="E45" s="83" t="s">
+        <v>277</v>
       </c>
       <c r="F45" s="128" t="s">
         <v>27</v>
       </c>
       <c r="G45" s="128" t="s">
-        <v>234</v>
+        <v>43</v>
       </c>
       <c r="H45" s="128" t="s">
         <v>29</v>
       </c>
       <c r="I45" s="130" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="J45" s="130" t="s">
-        <v>76</v>
+        <v>30</v>
       </c>
       <c r="K45" s="131" t="s">
-        <v>256</v>
+        <v>278</v>
       </c>
       <c r="L45" s="130"/>
-    </row>
-    <row r="46" spans="1:12" ht="64" x14ac:dyDescent="0.2">
+      <c r="O45" s="32" t="s">
+        <v>648</v>
+      </c>
+      <c r="P45" s="32" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q45" s="32" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A46" s="122" t="s">
-        <v>257</v>
+        <v>279</v>
       </c>
       <c r="B46" s="35" t="s">
-        <v>258</v>
-      </c>
-      <c r="C46" s="143" t="s">
-        <v>259</v>
+        <v>280</v>
+      </c>
+      <c r="C46" s="122" t="s">
+        <v>281</v>
       </c>
       <c r="D46" s="133" t="s">
         <v>25</v>
       </c>
       <c r="E46" s="133" t="s">
-        <v>260</v>
+        <v>282</v>
       </c>
       <c r="F46" s="125" t="s">
         <v>27</v>
       </c>
       <c r="G46" s="125" t="s">
-        <v>261</v>
+        <v>75</v>
       </c>
       <c r="H46" s="125" t="s">
         <v>93</v>
       </c>
       <c r="I46" s="107" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="J46" s="107" t="s">
         <v>62</v>
       </c>
       <c r="K46" s="106" t="s">
-        <v>262</v>
+        <v>283</v>
       </c>
       <c r="L46" s="107"/>
-    </row>
-    <row r="47" spans="1:12" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O46" s="32" t="s">
+        <v>649</v>
+      </c>
+      <c r="P46" s="32" t="s">
+        <v>716</v>
+      </c>
+      <c r="Q46" s="32" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A47" s="126" t="s">
-        <v>263</v>
+        <v>284</v>
       </c>
       <c r="B47" s="74" t="s">
-        <v>264</v>
+        <v>285</v>
       </c>
       <c r="C47" s="126" t="s">
-        <v>265</v>
-      </c>
-      <c r="D47" s="144" t="s">
-        <v>266</v>
+        <v>286</v>
+      </c>
+      <c r="D47" s="127" t="s">
+        <v>25</v>
       </c>
       <c r="E47" s="74" t="s">
-        <v>267</v>
+        <v>287</v>
       </c>
       <c r="F47" s="128" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="G47" s="128" t="s">
-        <v>43</v>
+        <v>75</v>
       </c>
       <c r="H47" s="128" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="I47" s="130" t="s">
-        <v>69</v>
+        <v>19</v>
       </c>
       <c r="J47" s="130" t="s">
-        <v>30</v>
+        <v>76</v>
       </c>
       <c r="K47" s="131" t="s">
-        <v>268</v>
+        <v>288</v>
       </c>
       <c r="L47" s="130"/>
-    </row>
-    <row r="48" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="O47" s="32" t="s">
+        <v>649</v>
+      </c>
+      <c r="P47" s="32" t="s">
+        <v>716</v>
+      </c>
+      <c r="Q47" s="32" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" ht="84.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="122" t="s">
-        <v>269</v>
+        <v>289</v>
       </c>
       <c r="B48" s="35" t="s">
-        <v>270</v>
+        <v>290</v>
       </c>
       <c r="C48" s="122" t="s">
-        <v>271</v>
+        <v>291</v>
       </c>
       <c r="D48" s="133" t="s">
         <v>25</v>
       </c>
-      <c r="E48" s="133" t="s">
-        <v>272</v>
-      </c>
+      <c r="E48" s="133"/>
       <c r="F48" s="125" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="G48" s="125" t="s">
-        <v>75</v>
+        <v>292</v>
       </c>
       <c r="H48" s="125" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="I48" s="107" t="s">
-        <v>69</v>
+        <v>19</v>
       </c>
       <c r="J48" s="107" t="s">
         <v>76</v>
       </c>
-      <c r="K48" s="106" t="s">
-        <v>269</v>
-      </c>
+      <c r="K48" s="106"/>
       <c r="L48" s="107"/>
-    </row>
-    <row r="49" spans="1:12" ht="64" x14ac:dyDescent="0.2">
-      <c r="A49" s="126" t="s">
-        <v>273</v>
-      </c>
-      <c r="B49" s="74" t="s">
-        <v>274</v>
-      </c>
-      <c r="C49" s="126" t="s">
-        <v>275</v>
-      </c>
-      <c r="D49" s="188" t="s">
-        <v>276</v>
-      </c>
-      <c r="E49" s="83" t="s">
-        <v>277</v>
-      </c>
-      <c r="F49" s="128" t="s">
-        <v>27</v>
-      </c>
-      <c r="G49" s="128" t="s">
-        <v>43</v>
-      </c>
-      <c r="H49" s="128" t="s">
-        <v>29</v>
-      </c>
-      <c r="I49" s="130" t="s">
-        <v>61</v>
-      </c>
-      <c r="J49" s="130" t="s">
-        <v>30</v>
-      </c>
-      <c r="K49" s="131" t="s">
-        <v>278</v>
-      </c>
-      <c r="L49" s="130"/>
-    </row>
-    <row r="50" spans="1:12" ht="32" x14ac:dyDescent="0.2">
-      <c r="A50" s="122" t="s">
-        <v>279</v>
-      </c>
-      <c r="B50" s="35" t="s">
-        <v>280</v>
-      </c>
-      <c r="C50" s="122" t="s">
-        <v>281</v>
-      </c>
-      <c r="D50" s="133" t="s">
-        <v>25</v>
-      </c>
-      <c r="E50" s="133" t="s">
-        <v>282</v>
-      </c>
-      <c r="F50" s="125" t="s">
-        <v>27</v>
-      </c>
-      <c r="G50" s="125" t="s">
-        <v>75</v>
-      </c>
-      <c r="H50" s="125" t="s">
-        <v>93</v>
-      </c>
-      <c r="I50" s="107" t="s">
-        <v>61</v>
-      </c>
-      <c r="J50" s="107" t="s">
-        <v>62</v>
-      </c>
-      <c r="K50" s="106" t="s">
-        <v>283</v>
-      </c>
-      <c r="L50" s="107"/>
-    </row>
-    <row r="51" spans="1:12" ht="32" x14ac:dyDescent="0.2">
-      <c r="A51" s="126" t="s">
-        <v>284</v>
-      </c>
-      <c r="B51" s="74" t="s">
-        <v>285</v>
-      </c>
-      <c r="C51" s="126" t="s">
-        <v>286</v>
-      </c>
-      <c r="D51" s="127" t="s">
-        <v>25</v>
-      </c>
-      <c r="E51" s="74" t="s">
-        <v>287</v>
-      </c>
-      <c r="F51" s="128" t="s">
-        <v>27</v>
-      </c>
-      <c r="G51" s="128" t="s">
-        <v>75</v>
-      </c>
-      <c r="H51" s="128" t="s">
-        <v>29</v>
-      </c>
-      <c r="I51" s="130" t="s">
-        <v>19</v>
-      </c>
-      <c r="J51" s="130" t="s">
-        <v>76</v>
-      </c>
-      <c r="K51" s="131" t="s">
-        <v>288</v>
-      </c>
-      <c r="L51" s="130"/>
-    </row>
-    <row r="52" spans="1:12" ht="84.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="122" t="s">
-        <v>289</v>
-      </c>
-      <c r="B52" s="35" t="s">
-        <v>290</v>
-      </c>
-      <c r="C52" s="122" t="s">
-        <v>291</v>
-      </c>
-      <c r="D52" s="133" t="s">
-        <v>25</v>
-      </c>
-      <c r="E52" s="133"/>
-      <c r="F52" s="125" t="s">
-        <v>27</v>
-      </c>
-      <c r="G52" s="125" t="s">
-        <v>292</v>
-      </c>
-      <c r="H52" s="125" t="s">
-        <v>29</v>
-      </c>
-      <c r="I52" s="107" t="s">
-        <v>19</v>
-      </c>
-      <c r="J52" s="107" t="s">
-        <v>76</v>
-      </c>
-      <c r="K52" s="106"/>
-      <c r="L52" s="107"/>
-    </row>
-    <row r="53" spans="1:12" s="119" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="147"/>
-      <c r="B53" s="148"/>
-      <c r="C53" s="147"/>
-      <c r="D53" s="149"/>
-      <c r="E53" s="149"/>
-      <c r="F53" s="150"/>
-      <c r="G53" s="150"/>
-      <c r="H53" s="150"/>
-      <c r="I53" s="151"/>
-      <c r="J53" s="151"/>
-      <c r="K53" s="152"/>
-      <c r="L53" s="151"/>
+      <c r="O48" s="32" t="s">
+        <v>648</v>
+      </c>
+      <c r="P48" s="32" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q48" s="32" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" s="119" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="147"/>
+      <c r="B49" s="148"/>
+      <c r="C49" s="147"/>
+      <c r="D49" s="149"/>
+      <c r="E49" s="149"/>
+      <c r="F49" s="150"/>
+      <c r="G49" s="150"/>
+      <c r="H49" s="150"/>
+      <c r="I49" s="151"/>
+      <c r="J49" s="151"/>
+      <c r="K49" s="152"/>
+      <c r="L49" s="151"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J53" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J53">
-    <sortCondition ref="A2:A53"/>
+  <autoFilter ref="A1:J49" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J49">
+    <sortCondition ref="A2:A49"/>
   </sortState>
-  <mergeCells count="11">
-    <mergeCell ref="A14:A18"/>
-    <mergeCell ref="B14:B18"/>
-    <mergeCell ref="C14:C18"/>
-    <mergeCell ref="F14:F18"/>
-    <mergeCell ref="E14:E18"/>
-    <mergeCell ref="L14:L18"/>
-    <mergeCell ref="K14:K18"/>
-    <mergeCell ref="G14:G18"/>
-    <mergeCell ref="H14:H18"/>
-    <mergeCell ref="I14:I18"/>
-    <mergeCell ref="J14:J18"/>
-  </mergeCells>
-  <conditionalFormatting sqref="F2:F14 F19:F53">
+  <conditionalFormatting sqref="F2:F49">
     <cfRule type="cellIs" dxfId="170" priority="8" operator="equal">
       <formula>"Not added"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H14 H19:H53">
+  <conditionalFormatting sqref="H2:H49">
     <cfRule type="cellIs" dxfId="169" priority="17" operator="greaterThan">
       <formula>"reviewd"</formula>
     </cfRule>
@@ -17518,7 +18241,7 @@
       <formula>"needs review"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H1:I1 F1:F14 F19:F53">
+  <conditionalFormatting sqref="H1:I1 F1:F49">
     <cfRule type="cellIs" dxfId="167" priority="19" operator="equal">
       <formula>"Optional"</formula>
     </cfRule>
@@ -17532,7 +18255,7 @@
       <formula>"Conditional"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J14 J19:J53">
+  <conditionalFormatting sqref="J2:J49">
     <cfRule type="containsText" dxfId="163" priority="5" operator="containsText" text="Health and NL">
       <formula>NOT(ISERROR(SEARCH("Health and NL",J2)))</formula>
     </cfRule>
@@ -17561,41 +18284,37 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1" xr:uid="{7D4DA44D-79A1-46A0-A570-1C5C4461BB54}">
       <formula1>"Mandatory, Recommended, Optional, Conditional"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H47:H53 H14 H28:H38 H19:H26 H2:H12" xr:uid="{9762E750-ADF5-4984-93BF-D8ED80389E8E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H43:H49 H24:H34 H14:H22 H2:H12" xr:uid="{9762E750-ADF5-4984-93BF-D8ED80389E8E}">
       <formula1>"0..n, 0..1, 1, 1..n"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J1 J48 J52:J53" xr:uid="{D74C1692-73CE-477E-BF57-68FEA17E3FE5}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J49:J51 J53 J19:J47 J2:J14" xr:uid="{B80CEB2B-1BEF-4952-992A-5359B9DD2C11}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J1 J44 J48:J49" xr:uid="{D74C1692-73CE-477E-BF57-68FEA17E3FE5}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J45:J47 J49 J2:J43" xr:uid="{B80CEB2B-1BEF-4952-992A-5359B9DD2C11}">
       <formula1>"DCAT-AP v3, HealthDCAT-AP, DCAT-AP NL, HRI v1, Health and NL"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I19:I1048576 K54:K1048576 I2:I14" xr:uid="{96DDE4B1-378F-48ED-B590-490B6967CC12}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K50:K1048576 I2:I1048576" xr:uid="{96DDE4B1-378F-48ED-B590-490B6967CC12}">
       <formula1>"Identical to v1, Adapted from v1, new"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F19:F53 F2:F14" xr:uid="{584B70CE-0B19-4CA2-8DA1-B7818B2A385E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F49" xr:uid="{584B70CE-0B19-4CA2-8DA1-B7818B2A385E}">
       <formula1>"Mandatory, Recommended, Optional, Conditional, Not added"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J54:J1048576" xr:uid="{1E5E2E20-49B0-42CC-AEB2-F591D86C2104}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J50:J1048576" xr:uid="{1E5E2E20-49B0-42CC-AEB2-F591D86C2104}">
       <formula1>"DCAT-AP v3, HealthDCAT-AP, DCAT-AP NL, HRI v1"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="D49" r:id="rId1" xr:uid="{91138281-081C-4FCB-A57E-72AD63591E46}"/>
-    <hyperlink ref="D44" r:id="rId2" xr:uid="{F8D55E3A-6834-452E-87A5-486C6DC2AB9C}"/>
-    <hyperlink ref="D47" r:id="rId3" xr:uid="{865E93AD-51B7-46E5-8BC3-1DADF5F6B30B}"/>
-    <hyperlink ref="D25" r:id="rId4" xr:uid="{44AB3AA7-A33B-4284-8A50-B160BBE78CCD}"/>
+    <hyperlink ref="D45" r:id="rId1" xr:uid="{91138281-081C-4FCB-A57E-72AD63591E46}"/>
+    <hyperlink ref="D40" r:id="rId2" xr:uid="{F8D55E3A-6834-452E-87A5-486C6DC2AB9C}"/>
+    <hyperlink ref="D43" r:id="rId3" xr:uid="{865E93AD-51B7-46E5-8BC3-1DADF5F6B30B}"/>
+    <hyperlink ref="D21" r:id="rId4" xr:uid="{44AB3AA7-A33B-4284-8A50-B160BBE78CCD}"/>
     <hyperlink ref="D2" r:id="rId5" xr:uid="{09FF204A-6D13-47DD-815F-9332A177A210}"/>
-    <hyperlink ref="D33" r:id="rId6" xr:uid="{438AEAA3-68CD-40FB-B06F-D8337C050F13}"/>
+    <hyperlink ref="D29" r:id="rId6" xr:uid="{438AEAA3-68CD-40FB-B06F-D8337C050F13}"/>
     <hyperlink ref="D13" r:id="rId7" xr:uid="{34DA509B-48BE-49A4-9202-31C368FF1E15}"/>
     <hyperlink ref="D14" r:id="rId8" xr:uid="{49A76848-F344-47A3-B292-6477CBA598F6}"/>
-    <hyperlink ref="D15" r:id="rId9" xr:uid="{49797FF1-9BCE-4245-9B0E-8123D217DB10}"/>
-    <hyperlink ref="D16" r:id="rId10" xr:uid="{92E48F67-CD82-4057-983D-B57CAF999167}"/>
-    <hyperlink ref="D17" r:id="rId11" xr:uid="{B343B042-A5A8-4EE9-938E-0760AFFAA83C}"/>
-    <hyperlink ref="D18" r:id="rId12" xr:uid="{7BDB6C8C-2D36-4A45-B0A4-8F5BA0B9E485}"/>
-    <hyperlink ref="D26" r:id="rId13" location="vocab-legal-basis" xr:uid="{9EEE329D-0E5D-4286-9533-8A6AB1929736}"/>
-    <hyperlink ref="D36" r:id="rId14" location="vocab-purposes" xr:uid="{0AFDD853-55E1-48FA-8AC6-4D2598057364}"/>
+    <hyperlink ref="D22" r:id="rId9" location="vocab-legal-basis" xr:uid="{9EEE329D-0E5D-4286-9533-8A6AB1929736}"/>
+    <hyperlink ref="D32" r:id="rId10" location="vocab-purposes" xr:uid="{0AFDD853-55E1-48FA-8AC6-4D2598057364}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="8" fitToHeight="0" orientation="landscape" r:id="rId15"/>
+  <pageSetup paperSize="8" fitToHeight="0" orientation="landscape" r:id="rId11"/>
 </worksheet>
 </file>
 
@@ -17875,13 +18594,13 @@
       <c r="L7" s="130"/>
     </row>
     <row r="8" spans="1:12" ht="32" x14ac:dyDescent="0.2">
-      <c r="A8" s="220" t="s">
+      <c r="A8" s="221" t="s">
         <v>95</v>
       </c>
       <c r="B8" s="223" t="s">
         <v>96</v>
       </c>
-      <c r="C8" s="220" t="s">
+      <c r="C8" s="221" t="s">
         <v>97</v>
       </c>
       <c r="D8" s="154" t="s">
@@ -17890,87 +18609,87 @@
       <c r="E8" s="222" t="s">
         <v>307</v>
       </c>
-      <c r="F8" s="219" t="s">
+      <c r="F8" s="220" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="219" t="s">
+      <c r="G8" s="220" t="s">
         <v>100</v>
       </c>
-      <c r="H8" s="219" t="s">
+      <c r="H8" s="220" t="s">
         <v>29</v>
       </c>
-      <c r="I8" s="217" t="s">
+      <c r="I8" s="219" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="217" t="s">
+      <c r="J8" s="219" t="s">
         <v>30</v>
       </c>
       <c r="K8" s="138"/>
-      <c r="L8" s="217"/>
+      <c r="L8" s="219"/>
     </row>
     <row r="9" spans="1:12" ht="32" x14ac:dyDescent="0.2">
-      <c r="A9" s="220"/>
+      <c r="A9" s="221"/>
       <c r="B9" s="223"/>
-      <c r="C9" s="220"/>
+      <c r="C9" s="221"/>
       <c r="D9" s="155" t="s">
         <v>101</v>
       </c>
       <c r="E9" s="222"/>
-      <c r="F9" s="219"/>
-      <c r="G9" s="219"/>
-      <c r="H9" s="219"/>
-      <c r="I9" s="217"/>
-      <c r="J9" s="217"/>
+      <c r="F9" s="220"/>
+      <c r="G9" s="220"/>
+      <c r="H9" s="220"/>
+      <c r="I9" s="219"/>
+      <c r="J9" s="219"/>
       <c r="K9" s="138"/>
-      <c r="L9" s="217"/>
+      <c r="L9" s="219"/>
     </row>
     <row r="10" spans="1:12" ht="32" x14ac:dyDescent="0.2">
-      <c r="A10" s="220"/>
+      <c r="A10" s="221"/>
       <c r="B10" s="223"/>
-      <c r="C10" s="220"/>
+      <c r="C10" s="221"/>
       <c r="D10" s="155" t="s">
         <v>102</v>
       </c>
       <c r="E10" s="222"/>
-      <c r="F10" s="219"/>
-      <c r="G10" s="219"/>
-      <c r="H10" s="219"/>
-      <c r="I10" s="217"/>
-      <c r="J10" s="217"/>
+      <c r="F10" s="220"/>
+      <c r="G10" s="220"/>
+      <c r="H10" s="220"/>
+      <c r="I10" s="219"/>
+      <c r="J10" s="219"/>
       <c r="K10" s="138"/>
-      <c r="L10" s="217"/>
+      <c r="L10" s="219"/>
     </row>
     <row r="11" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="220"/>
+      <c r="A11" s="221"/>
       <c r="B11" s="223"/>
-      <c r="C11" s="220"/>
+      <c r="C11" s="221"/>
       <c r="D11" s="155" t="s">
         <v>103</v>
       </c>
       <c r="E11" s="222"/>
-      <c r="F11" s="219"/>
-      <c r="G11" s="219"/>
-      <c r="H11" s="219"/>
-      <c r="I11" s="217"/>
-      <c r="J11" s="217"/>
+      <c r="F11" s="220"/>
+      <c r="G11" s="220"/>
+      <c r="H11" s="220"/>
+      <c r="I11" s="219"/>
+      <c r="J11" s="219"/>
       <c r="K11" s="156"/>
-      <c r="L11" s="217"/>
+      <c r="L11" s="219"/>
     </row>
     <row r="12" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="220"/>
+      <c r="A12" s="221"/>
       <c r="B12" s="223"/>
-      <c r="C12" s="220"/>
+      <c r="C12" s="221"/>
       <c r="D12" s="155" t="s">
         <v>104</v>
       </c>
       <c r="E12" s="222"/>
-      <c r="F12" s="219"/>
-      <c r="G12" s="219"/>
-      <c r="H12" s="219"/>
-      <c r="I12" s="217"/>
-      <c r="J12" s="217"/>
+      <c r="F12" s="220"/>
+      <c r="G12" s="220"/>
+      <c r="H12" s="220"/>
+      <c r="I12" s="219"/>
+      <c r="J12" s="219"/>
       <c r="K12" s="138"/>
-      <c r="L12" s="217"/>
+      <c r="L12" s="219"/>
     </row>
     <row r="13" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A13" s="126" t="s">

</xml_diff>

<commit_message>
feat: adds a lot of functions to clean up shacls
</commit_message>
<xml_diff>
--- a/inputs/Health-RI-Metadata_CoreGenericHealth_v2-0-0.xlsx
+++ b/inputs/Health-RI-Metadata_CoreGenericHealth_v2-0-0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexanderharms/Documents/Projects/Metadata automation/metadata-automation/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFD012DD-7667-514C-AB18-4C2AE0906268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{193AB2A4-C193-3549-B69C-34F73A7121B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36000" yWindow="-4920" windowWidth="34360" windowHeight="28300" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37900" yWindow="-2640" windowWidth="34420" windowHeight="28300" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="14" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2124" uniqueCount="737">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2447" uniqueCount="759">
   <si>
     <t>Property label</t>
   </si>
@@ -2468,9 +2468,6 @@
     <t>hri:Dataset</t>
   </si>
   <si>
-    <t>dash:EnumSelectEditor</t>
-  </si>
-  <si>
     <t>dash:BlankNodeEditor</t>
   </si>
   <si>
@@ -2538,6 +2535,75 @@
   </si>
   <si>
     <t>hri:Kind,hri:Agent,hri:PeriodOfTime</t>
+  </si>
+  <si>
+    <t>Pattern</t>
+  </si>
+  <si>
+    <t>Default value</t>
+  </si>
+  <si>
+    <t>http://data.europa.eu/eli/reg/2025/327/oj</t>
+  </si>
+  <si>
+    <t>^mailto:.+@.+\..+$</t>
+  </si>
+  <si>
+    <t>^\d{4}-\d{2}-\d{2}T\d{2}:\d{2}:\d{2}(\.\d{1,3})?(Z|[+-]\d{2}:\d{2})$</t>
+  </si>
+  <si>
+    <t>Distribution</t>
+  </si>
+  <si>
+    <t>hri:Distribution</t>
+  </si>
+  <si>
+    <t>DatasetSeries</t>
+  </si>
+  <si>
+    <t>hri:DatasetSeries</t>
+  </si>
+  <si>
+    <t>DataService</t>
+  </si>
+  <si>
+    <t>hri:DataService</t>
+  </si>
+  <si>
+    <t>hri:Kind,hri:Agent,hri:Identifier</t>
+  </si>
+  <si>
+    <t>adms_Identifier</t>
+  </si>
+  <si>
+    <t>PeriodOfTime</t>
+  </si>
+  <si>
+    <t>Attribution</t>
+  </si>
+  <si>
+    <t>Relationship</t>
+  </si>
+  <si>
+    <t>hri:Relationship</t>
+  </si>
+  <si>
+    <t>QualityCertificate</t>
+  </si>
+  <si>
+    <t>Checksum</t>
+  </si>
+  <si>
+    <t>hri:Checksum</t>
+  </si>
+  <si>
+    <t>Resource</t>
+  </si>
+  <si>
+    <t>hri:Resource</t>
+  </si>
+  <si>
+    <t>dcat:Resource</t>
   </si>
 </sst>
 </file>
@@ -3603,6 +3669,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3611,10 +3692,22 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3622,33 +3715,6 @@
     </xf>
     <xf numFmtId="49" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -7299,11 +7365,11 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:L57"/>
+  <dimension ref="A1:T57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N19" sqref="N19"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q24" sqref="Q24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7311,19 +7377,21 @@
     <col min="1" max="1" width="19.1640625" style="9" customWidth="1"/>
     <col min="2" max="2" width="42.6640625" style="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.5" style="8" customWidth="1"/>
-    <col min="5" max="5" width="57.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.1640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="24" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.83203125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="18.5" style="2" customWidth="1"/>
-    <col min="10" max="10" width="17.5" style="2" customWidth="1"/>
+    <col min="4" max="4" width="23.5" style="8" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="57.6640625" style="8" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="22.1640625" style="2" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="24" style="2" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="11.83203125" style="2" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="18.5" style="2" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="17.5" style="2" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="39.33203125" style="2" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="20.33203125" style="2" customWidth="1"/>
-    <col min="13" max="16384" width="9.1640625" style="2"/>
+    <col min="12" max="12" width="20.33203125" style="2" hidden="1" customWidth="1"/>
+    <col min="13" max="14" width="9.1640625" style="2"/>
+    <col min="15" max="20" width="16.6640625" style="2" customWidth="1"/>
+    <col min="21" max="16384" width="9.1640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="202" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" s="202" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A1" s="89" t="s">
         <v>0</v>
       </c>
@@ -7360,8 +7428,32 @@
       <c r="L1" s="106" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="M1" s="216" t="s">
+        <v>638</v>
+      </c>
+      <c r="N1" s="216" t="s">
+        <v>639</v>
+      </c>
+      <c r="O1" s="216" t="s">
+        <v>640</v>
+      </c>
+      <c r="P1" s="216" t="s">
+        <v>641</v>
+      </c>
+      <c r="Q1" s="216" t="s">
+        <v>642</v>
+      </c>
+      <c r="R1" s="216" t="s">
+        <v>643</v>
+      </c>
+      <c r="S1" s="216" t="s">
+        <v>736</v>
+      </c>
+      <c r="T1" s="216" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="120" t="s">
         <v>387</v>
       </c>
@@ -7397,7 +7489,7 @@
       </c>
       <c r="L2" s="105"/>
     </row>
-    <row r="3" spans="1:12" ht="64" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A3" s="124" t="s">
         <v>392</v>
       </c>
@@ -7432,8 +7524,17 @@
         <v>396</v>
       </c>
       <c r="L3" s="128"/>
-    </row>
-    <row r="4" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="O3" s="2" t="s">
+        <v>648</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="130" t="s">
         <v>32</v>
       </c>
@@ -7468,8 +7569,17 @@
         <v>38</v>
       </c>
       <c r="L4" s="105"/>
-    </row>
-    <row r="5" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+      <c r="O4" s="2" t="s">
+        <v>648</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="48" x14ac:dyDescent="0.2">
       <c r="A5" s="124" t="s">
         <v>398</v>
       </c>
@@ -7504,8 +7614,17 @@
         <v>403</v>
       </c>
       <c r="L5" s="128"/>
-    </row>
-    <row r="6" spans="1:12" ht="64" x14ac:dyDescent="0.2">
+      <c r="O5" s="2" t="s">
+        <v>649</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>715</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="120" t="s">
         <v>404</v>
       </c>
@@ -7540,8 +7659,17 @@
         <v>409</v>
       </c>
       <c r="L6" s="105"/>
-    </row>
-    <row r="7" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+      <c r="O6" s="2" t="s">
+        <v>714</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="48" x14ac:dyDescent="0.2">
       <c r="A7" s="124" t="s">
         <v>410</v>
       </c>
@@ -7576,8 +7704,17 @@
         <v>416</v>
       </c>
       <c r="L7" s="128"/>
-    </row>
-    <row r="8" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+      <c r="O7" s="2" t="s">
+        <v>649</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>715</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" ht="48" x14ac:dyDescent="0.2">
       <c r="A8" s="120" t="s">
         <v>71</v>
       </c>
@@ -7612,8 +7749,17 @@
         <v>418</v>
       </c>
       <c r="L8" s="105"/>
-    </row>
-    <row r="9" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="O8" s="2" t="s">
+        <v>649</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>715</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="124" t="s">
         <v>82</v>
       </c>
@@ -7648,8 +7794,17 @@
         <v>420</v>
       </c>
       <c r="L9" s="128"/>
-    </row>
-    <row r="10" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+      <c r="O9" s="2" t="s">
+        <v>648</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" ht="48" x14ac:dyDescent="0.2">
       <c r="A10" s="120" t="s">
         <v>421</v>
       </c>
@@ -7684,8 +7839,17 @@
         <v>425</v>
       </c>
       <c r="L10" s="105"/>
-    </row>
-    <row r="11" spans="1:12" ht="80" x14ac:dyDescent="0.2">
+      <c r="O10" s="2" t="s">
+        <v>648</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" ht="80" x14ac:dyDescent="0.2">
       <c r="A11" s="124" t="s">
         <v>426</v>
       </c>
@@ -7720,8 +7884,17 @@
         <v>432</v>
       </c>
       <c r="L11" s="128"/>
-    </row>
-    <row r="12" spans="1:12" ht="99" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O11" s="2" t="s">
+        <v>648</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q11" s="2" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" ht="99" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="120" t="s">
         <v>137</v>
       </c>
@@ -7756,8 +7929,17 @@
         <v>434</v>
       </c>
       <c r="L12" s="105"/>
-    </row>
-    <row r="13" spans="1:12" ht="80" x14ac:dyDescent="0.2">
+      <c r="O12" s="2" t="s">
+        <v>648</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q12" s="2" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" ht="80" x14ac:dyDescent="0.2">
       <c r="A13" s="124" t="s">
         <v>435</v>
       </c>
@@ -7792,8 +7974,17 @@
         <v>438</v>
       </c>
       <c r="L13" s="128"/>
-    </row>
-    <row r="14" spans="1:12" ht="80" x14ac:dyDescent="0.2">
+      <c r="O13" s="2" t="s">
+        <v>648</v>
+      </c>
+      <c r="P13" s="2" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q13" s="2" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" ht="80" x14ac:dyDescent="0.2">
       <c r="A14" s="120" t="s">
         <v>439</v>
       </c>
@@ -7828,8 +8019,17 @@
         <v>441</v>
       </c>
       <c r="L14" s="105"/>
-    </row>
-    <row r="15" spans="1:12" ht="112" x14ac:dyDescent="0.2">
+      <c r="O14" s="2" t="s">
+        <v>648</v>
+      </c>
+      <c r="P14" s="2" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q14" s="2" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" ht="112" x14ac:dyDescent="0.2">
       <c r="A15" s="124" t="s">
         <v>442</v>
       </c>
@@ -7864,8 +8064,17 @@
         <v>446</v>
       </c>
       <c r="L15" s="128"/>
-    </row>
-    <row r="16" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="O15" s="2" t="s">
+        <v>648</v>
+      </c>
+      <c r="P15" s="2" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q15" s="2" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="120" t="s">
         <v>162</v>
       </c>
@@ -7898,8 +8107,20 @@
         <v>447</v>
       </c>
       <c r="L16" s="105"/>
-    </row>
-    <row r="17" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+      <c r="O16" s="2" t="s">
+        <v>649</v>
+      </c>
+      <c r="P16" s="2" t="s">
+        <v>716</v>
+      </c>
+      <c r="Q16" s="2" t="s">
+        <v>720</v>
+      </c>
+      <c r="S16" s="2" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" ht="48" x14ac:dyDescent="0.2">
       <c r="A17" s="124" t="s">
         <v>448</v>
       </c>
@@ -7934,8 +8155,17 @@
         <v>452</v>
       </c>
       <c r="L17" s="128"/>
-    </row>
-    <row r="18" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="O17" s="2" t="s">
+        <v>648</v>
+      </c>
+      <c r="P17" s="2" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q17" s="2" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="120" t="s">
         <v>225</v>
       </c>
@@ -7970,8 +8200,20 @@
         <v>454</v>
       </c>
       <c r="L18" s="105"/>
-    </row>
-    <row r="19" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="O18" s="2" t="s">
+        <v>649</v>
+      </c>
+      <c r="P18" s="2" t="s">
+        <v>716</v>
+      </c>
+      <c r="Q18" s="2" t="s">
+        <v>720</v>
+      </c>
+      <c r="S18" s="2" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="124" t="s">
         <v>230</v>
       </c>
@@ -8002,8 +8244,17 @@
       </c>
       <c r="K19" s="102"/>
       <c r="L19" s="128"/>
-    </row>
-    <row r="20" spans="1:12" ht="144" x14ac:dyDescent="0.2">
+      <c r="O19" s="2" t="s">
+        <v>714</v>
+      </c>
+      <c r="P19" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="Q19" s="2" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" ht="144" x14ac:dyDescent="0.2">
       <c r="A20" s="120" t="s">
         <v>325</v>
       </c>
@@ -8038,8 +8289,17 @@
         <v>457</v>
       </c>
       <c r="L20" s="105"/>
-    </row>
-    <row r="21" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+      <c r="O20" s="2" t="s">
+        <v>648</v>
+      </c>
+      <c r="P20" s="2" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q20" s="2" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" ht="48" x14ac:dyDescent="0.2">
       <c r="A21" s="124" t="s">
         <v>246</v>
       </c>
@@ -8074,8 +8334,17 @@
         <v>460</v>
       </c>
       <c r="L21" s="128"/>
-    </row>
-    <row r="22" spans="1:12" ht="64" x14ac:dyDescent="0.2">
+      <c r="O21" s="2" t="s">
+        <v>648</v>
+      </c>
+      <c r="P21" s="2" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q21" s="2" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" ht="64" x14ac:dyDescent="0.2">
       <c r="A22" s="120" t="s">
         <v>257</v>
       </c>
@@ -8108,8 +8377,17 @@
       </c>
       <c r="K22" s="103"/>
       <c r="L22" s="105"/>
-    </row>
-    <row r="23" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="O22" s="2" t="s">
+        <v>649</v>
+      </c>
+      <c r="P22" s="2" t="s">
+        <v>715</v>
+      </c>
+      <c r="Q22" s="2" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="124" t="s">
         <v>269</v>
       </c>
@@ -8144,8 +8422,17 @@
         <v>463</v>
       </c>
       <c r="L23" s="128"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O23" s="2" t="s">
+        <v>649</v>
+      </c>
+      <c r="P23" s="2" t="s">
+        <v>715</v>
+      </c>
+      <c r="Q23" s="2" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24" s="23"/>
       <c r="B24" s="8"/>
       <c r="C24" s="23"/>
@@ -8157,7 +8444,7 @@
       <c r="K24" s="98"/>
       <c r="L24" s="32"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" s="23"/>
       <c r="B25" s="8"/>
       <c r="C25" s="29"/>
@@ -8169,7 +8456,7 @@
       <c r="K25" s="96"/>
       <c r="L25" s="32"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A26" s="23"/>
       <c r="B26" s="8"/>
       <c r="C26" s="23"/>
@@ -8180,7 +8467,7 @@
       <c r="H26" s="24"/>
       <c r="K26" s="98"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A27" s="23"/>
       <c r="B27" s="8"/>
       <c r="D27" s="25"/>
@@ -8190,7 +8477,7 @@
       <c r="H27" s="24"/>
       <c r="K27" s="96"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A28" s="23"/>
       <c r="B28" s="8"/>
       <c r="C28" s="23"/>
@@ -8201,7 +8488,7 @@
       <c r="H28" s="24"/>
       <c r="K28" s="96"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A29" s="23"/>
       <c r="B29" s="8"/>
       <c r="C29" s="23"/>
@@ -8211,7 +8498,7 @@
       <c r="H29" s="24"/>
       <c r="K29" s="96"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A30" s="23"/>
       <c r="B30" s="8"/>
       <c r="C30" s="23"/>
@@ -8222,7 +8509,7 @@
       <c r="H30" s="24"/>
       <c r="K30" s="96"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A31" s="23"/>
       <c r="B31" s="8"/>
       <c r="C31" s="29"/>
@@ -8233,7 +8520,7 @@
       <c r="H31" s="24"/>
       <c r="K31" s="96"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A32" s="23"/>
       <c r="B32" s="8"/>
       <c r="C32" s="23"/>
@@ -8565,11 +8852,11 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:L55"/>
+  <dimension ref="A1:T55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
+      <selection pane="bottomLeft" activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8577,19 +8864,21 @@
     <col min="1" max="1" width="22.6640625" style="41" customWidth="1"/>
     <col min="2" max="2" width="43.5" style="41" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.33203125" style="41" customWidth="1"/>
-    <col min="4" max="4" width="24" style="34" customWidth="1"/>
-    <col min="5" max="5" width="76.6640625" style="41" customWidth="1"/>
-    <col min="6" max="6" width="16.5" style="32" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.1640625" style="32" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.83203125" style="32" customWidth="1"/>
-    <col min="9" max="9" width="16.5" style="32" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.6640625" style="32" customWidth="1"/>
+    <col min="4" max="4" width="24" style="34" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="76.6640625" style="41" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5" style="32" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="20.1640625" style="32" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="11.83203125" style="32" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5" style="32" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="18.6640625" style="32" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="39.33203125" style="2" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="20.5" style="32" customWidth="1"/>
-    <col min="13" max="16384" width="9.1640625" style="32"/>
+    <col min="12" max="12" width="20.5" style="32" hidden="1" customWidth="1"/>
+    <col min="13" max="14" width="9.1640625" style="32"/>
+    <col min="15" max="20" width="22.5" style="32" customWidth="1"/>
+    <col min="21" max="16384" width="9.1640625" style="32"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="200" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" s="200" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A1" s="89" t="s">
         <v>0</v>
       </c>
@@ -8626,8 +8915,32 @@
       <c r="L1" s="106" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M1" s="216" t="s">
+        <v>638</v>
+      </c>
+      <c r="N1" s="216" t="s">
+        <v>639</v>
+      </c>
+      <c r="O1" s="216" t="s">
+        <v>640</v>
+      </c>
+      <c r="P1" s="216" t="s">
+        <v>641</v>
+      </c>
+      <c r="Q1" s="216" t="s">
+        <v>642</v>
+      </c>
+      <c r="R1" s="216" t="s">
+        <v>643</v>
+      </c>
+      <c r="S1" s="216" t="s">
+        <v>736</v>
+      </c>
+      <c r="T1" s="216" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="192" t="s">
         <v>32</v>
       </c>
@@ -8662,8 +8975,17 @@
         <v>465</v>
       </c>
       <c r="L2" s="128"/>
-    </row>
-    <row r="3" spans="1:12" ht="64" x14ac:dyDescent="0.2">
+      <c r="O2" s="32" t="s">
+        <v>648</v>
+      </c>
+      <c r="P2" s="32" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q2" s="32" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A3" s="120" t="s">
         <v>56</v>
       </c>
@@ -8698,8 +9020,17 @@
         <v>467</v>
       </c>
       <c r="L3" s="105"/>
-    </row>
-    <row r="4" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="O3" s="32" t="s">
+        <v>714</v>
+      </c>
+      <c r="P3" s="32" t="s">
+        <v>713</v>
+      </c>
+      <c r="Q3" s="32" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="124" t="s">
         <v>71</v>
       </c>
@@ -8734,8 +9065,17 @@
         <v>469</v>
       </c>
       <c r="L4" s="128"/>
-    </row>
-    <row r="5" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="O4" s="32" t="s">
+        <v>649</v>
+      </c>
+      <c r="P4" s="32" t="s">
+        <v>715</v>
+      </c>
+      <c r="Q4" s="32" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="120" t="s">
         <v>88</v>
       </c>
@@ -8768,108 +9108,126 @@
       </c>
       <c r="K5" s="103"/>
       <c r="L5" s="105"/>
-    </row>
-    <row r="6" spans="1:12" ht="32" x14ac:dyDescent="0.2">
-      <c r="A6" s="225" t="s">
+      <c r="O5" s="32" t="s">
+        <v>648</v>
+      </c>
+      <c r="P5" s="32" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q5" s="32" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+      <c r="A6" s="228" t="s">
         <v>95</v>
       </c>
-      <c r="B6" s="226" t="s">
+      <c r="B6" s="229" t="s">
         <v>96</v>
       </c>
-      <c r="C6" s="225" t="s">
+      <c r="C6" s="228" t="s">
         <v>97</v>
       </c>
       <c r="D6" s="138" t="s">
         <v>98</v>
       </c>
-      <c r="E6" s="227" t="s">
+      <c r="E6" s="230" t="s">
         <v>99</v>
       </c>
-      <c r="F6" s="224" t="s">
+      <c r="F6" s="227" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="224" t="s">
+      <c r="G6" s="227" t="s">
         <v>100</v>
       </c>
-      <c r="H6" s="224" t="s">
+      <c r="H6" s="227" t="s">
         <v>29</v>
       </c>
-      <c r="I6" s="222" t="s">
+      <c r="I6" s="231" t="s">
         <v>19</v>
       </c>
-      <c r="J6" s="217" t="s">
+      <c r="J6" s="222" t="s">
         <v>30</v>
       </c>
-      <c r="K6" s="223" t="s">
+      <c r="K6" s="232" t="s">
         <v>471</v>
       </c>
-      <c r="L6" s="222"/>
-    </row>
-    <row r="7" spans="1:12" ht="32" x14ac:dyDescent="0.2">
-      <c r="A7" s="225"/>
-      <c r="B7" s="226"/>
-      <c r="C7" s="225"/>
+      <c r="L6" s="231"/>
+      <c r="O6" s="32" t="s">
+        <v>648</v>
+      </c>
+      <c r="P6" s="32" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q6" s="32" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+      <c r="A7" s="228"/>
+      <c r="B7" s="229"/>
+      <c r="C7" s="228"/>
       <c r="D7" s="139" t="s">
         <v>101</v>
       </c>
-      <c r="E7" s="227"/>
-      <c r="F7" s="224"/>
-      <c r="G7" s="224"/>
-      <c r="H7" s="224"/>
-      <c r="I7" s="222"/>
-      <c r="J7" s="217"/>
-      <c r="K7" s="223"/>
-      <c r="L7" s="222"/>
-    </row>
-    <row r="8" spans="1:12" ht="32" x14ac:dyDescent="0.2">
-      <c r="A8" s="225"/>
-      <c r="B8" s="226"/>
-      <c r="C8" s="225"/>
+      <c r="E7" s="230"/>
+      <c r="F7" s="227"/>
+      <c r="G7" s="227"/>
+      <c r="H7" s="227"/>
+      <c r="I7" s="231"/>
+      <c r="J7" s="222"/>
+      <c r="K7" s="232"/>
+      <c r="L7" s="231"/>
+    </row>
+    <row r="8" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+      <c r="A8" s="228"/>
+      <c r="B8" s="229"/>
+      <c r="C8" s="228"/>
       <c r="D8" s="139" t="s">
         <v>102</v>
       </c>
-      <c r="E8" s="227"/>
-      <c r="F8" s="224"/>
-      <c r="G8" s="224"/>
-      <c r="H8" s="224"/>
-      <c r="I8" s="222"/>
-      <c r="J8" s="217"/>
-      <c r="K8" s="223"/>
-      <c r="L8" s="222"/>
-    </row>
-    <row r="9" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="225"/>
-      <c r="B9" s="226"/>
-      <c r="C9" s="225"/>
+      <c r="E8" s="230"/>
+      <c r="F8" s="227"/>
+      <c r="G8" s="227"/>
+      <c r="H8" s="227"/>
+      <c r="I8" s="231"/>
+      <c r="J8" s="222"/>
+      <c r="K8" s="232"/>
+      <c r="L8" s="231"/>
+    </row>
+    <row r="9" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="228"/>
+      <c r="B9" s="229"/>
+      <c r="C9" s="228"/>
       <c r="D9" s="139" t="s">
         <v>103</v>
       </c>
-      <c r="E9" s="227"/>
-      <c r="F9" s="224"/>
-      <c r="G9" s="224"/>
-      <c r="H9" s="224"/>
-      <c r="I9" s="222"/>
-      <c r="J9" s="217"/>
-      <c r="K9" s="223"/>
-      <c r="L9" s="222"/>
-    </row>
-    <row r="10" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="225"/>
-      <c r="B10" s="226"/>
-      <c r="C10" s="225"/>
+      <c r="E9" s="230"/>
+      <c r="F9" s="227"/>
+      <c r="G9" s="227"/>
+      <c r="H9" s="227"/>
+      <c r="I9" s="231"/>
+      <c r="J9" s="222"/>
+      <c r="K9" s="232"/>
+      <c r="L9" s="231"/>
+    </row>
+    <row r="10" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="228"/>
+      <c r="B10" s="229"/>
+      <c r="C10" s="228"/>
       <c r="D10" s="139" t="s">
         <v>104</v>
       </c>
-      <c r="E10" s="227"/>
-      <c r="F10" s="224"/>
-      <c r="G10" s="224"/>
-      <c r="H10" s="224"/>
-      <c r="I10" s="222"/>
-      <c r="J10" s="217"/>
-      <c r="K10" s="223"/>
-      <c r="L10" s="222"/>
-    </row>
-    <row r="11" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="E10" s="230"/>
+      <c r="F10" s="227"/>
+      <c r="G10" s="227"/>
+      <c r="H10" s="227"/>
+      <c r="I10" s="231"/>
+      <c r="J10" s="222"/>
+      <c r="K10" s="232"/>
+      <c r="L10" s="231"/>
+    </row>
+    <row r="11" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="120" t="s">
         <v>162</v>
       </c>
@@ -8904,8 +9262,20 @@
         <v>469</v>
       </c>
       <c r="L11" s="105"/>
-    </row>
-    <row r="12" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="O11" s="32" t="s">
+        <v>649</v>
+      </c>
+      <c r="P11" s="32" t="s">
+        <v>716</v>
+      </c>
+      <c r="Q11" s="32" t="s">
+        <v>720</v>
+      </c>
+      <c r="S11" s="32" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="124" t="s">
         <v>197</v>
       </c>
@@ -8940,8 +9310,17 @@
         <v>474</v>
       </c>
       <c r="L12" s="128"/>
-    </row>
-    <row r="13" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="O12" s="32" t="s">
+        <v>714</v>
+      </c>
+      <c r="P12" s="32" t="s">
+        <v>713</v>
+      </c>
+      <c r="Q12" s="32" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="120" t="s">
         <v>225</v>
       </c>
@@ -8976,8 +9355,20 @@
         <v>476</v>
       </c>
       <c r="L13" s="105"/>
-    </row>
-    <row r="14" spans="1:12" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O13" s="32" t="s">
+        <v>649</v>
+      </c>
+      <c r="P13" s="32" t="s">
+        <v>716</v>
+      </c>
+      <c r="Q13" s="32" t="s">
+        <v>720</v>
+      </c>
+      <c r="S13" s="32" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="124" t="s">
         <v>252</v>
       </c>
@@ -9012,8 +9403,17 @@
         <v>478</v>
       </c>
       <c r="L14" s="128"/>
-    </row>
-    <row r="15" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="O14" s="32" t="s">
+        <v>714</v>
+      </c>
+      <c r="P14" s="32" t="s">
+        <v>713</v>
+      </c>
+      <c r="Q14" s="32" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="120" t="s">
         <v>269</v>
       </c>
@@ -9048,8 +9448,17 @@
         <v>269</v>
       </c>
       <c r="L15" s="105"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O15" s="32" t="s">
+        <v>649</v>
+      </c>
+      <c r="P15" s="32" t="s">
+        <v>715</v>
+      </c>
+      <c r="Q15" s="32" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="K16" s="32"/>
     </row>
     <row r="17" spans="11:11" x14ac:dyDescent="0.2">
@@ -9172,17 +9581,17 @@
   </sheetData>
   <autoFilter ref="A1:L15" xr:uid="{FBE7E653-2382-46E4-9C76-9C694EDC9195}"/>
   <mergeCells count="11">
+    <mergeCell ref="L6:L10"/>
+    <mergeCell ref="K6:K10"/>
+    <mergeCell ref="H6:H10"/>
+    <mergeCell ref="I6:I10"/>
+    <mergeCell ref="J6:J10"/>
     <mergeCell ref="G6:G10"/>
     <mergeCell ref="A6:A10"/>
     <mergeCell ref="B6:B10"/>
     <mergeCell ref="C6:C10"/>
     <mergeCell ref="E6:E10"/>
     <mergeCell ref="F6:F10"/>
-    <mergeCell ref="L6:L10"/>
-    <mergeCell ref="K6:K10"/>
-    <mergeCell ref="H6:H10"/>
-    <mergeCell ref="I6:I10"/>
-    <mergeCell ref="J6:J10"/>
   </mergeCells>
   <conditionalFormatting sqref="F2:F6 F11:F15">
     <cfRule type="cellIs" dxfId="127" priority="7" operator="equal">
@@ -9272,11 +9681,11 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:L57"/>
+  <dimension ref="A1:T57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomLeft" activeCell="S18" sqref="S18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9284,18 +9693,19 @@
     <col min="1" max="1" width="22.33203125" style="19" customWidth="1"/>
     <col min="2" max="2" width="33.33203125" style="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.33203125" style="19" customWidth="1"/>
-    <col min="4" max="4" width="21.83203125" style="110" customWidth="1"/>
-    <col min="5" max="5" width="67.6640625" style="19" customWidth="1"/>
-    <col min="6" max="6" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.33203125" customWidth="1"/>
-    <col min="8" max="8" width="16.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.33203125" customWidth="1"/>
+    <col min="4" max="4" width="21.83203125" style="110" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="67.6640625" style="19" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="22.1640625" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="25.33203125" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="19.6640625" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="20.33203125" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="33.33203125" style="2" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="25.5" customWidth="1"/>
+    <col min="12" max="12" width="25.5" hidden="1" customWidth="1"/>
+    <col min="15" max="20" width="17.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="203" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" s="203" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A1" s="89" t="s">
         <v>0</v>
       </c>
@@ -9332,8 +9742,32 @@
       <c r="L1" s="106" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="84" x14ac:dyDescent="0.2">
+      <c r="M1" s="216" t="s">
+        <v>638</v>
+      </c>
+      <c r="N1" s="216" t="s">
+        <v>639</v>
+      </c>
+      <c r="O1" s="216" t="s">
+        <v>640</v>
+      </c>
+      <c r="P1" s="216" t="s">
+        <v>641</v>
+      </c>
+      <c r="Q1" s="216" t="s">
+        <v>642</v>
+      </c>
+      <c r="R1" s="216" t="s">
+        <v>643</v>
+      </c>
+      <c r="S1" s="216" t="s">
+        <v>736</v>
+      </c>
+      <c r="T1" s="216" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="84" x14ac:dyDescent="0.2">
       <c r="A2" s="130" t="s">
         <v>12</v>
       </c>
@@ -9368,8 +9802,17 @@
         <v>481</v>
       </c>
       <c r="L2" s="187"/>
-    </row>
-    <row r="3" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="O2" t="s">
+        <v>648</v>
+      </c>
+      <c r="P2" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="124" t="s">
         <v>32</v>
       </c>
@@ -9400,8 +9843,17 @@
       </c>
       <c r="K3" s="104"/>
       <c r="L3" s="128"/>
-    </row>
-    <row r="4" spans="1:12" ht="92.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O3" t="s">
+        <v>648</v>
+      </c>
+      <c r="P3" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="92.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="120" t="s">
         <v>482</v>
       </c>
@@ -9434,8 +9886,17 @@
       </c>
       <c r="K4" s="105"/>
       <c r="L4" s="105"/>
-    </row>
-    <row r="5" spans="1:12" ht="80" x14ac:dyDescent="0.2">
+      <c r="O4" t="s">
+        <v>648</v>
+      </c>
+      <c r="P4" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="80" x14ac:dyDescent="0.2">
       <c r="A5" s="192" t="s">
         <v>56</v>
       </c>
@@ -9468,8 +9929,17 @@
       </c>
       <c r="K5" s="104"/>
       <c r="L5" s="128"/>
-    </row>
-    <row r="6" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+      <c r="O5" t="s">
+        <v>714</v>
+      </c>
+      <c r="P5" t="s">
+        <v>713</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" s="120" t="s">
         <v>64</v>
       </c>
@@ -9502,8 +9972,17 @@
       </c>
       <c r="K6" s="104"/>
       <c r="L6" s="105"/>
-    </row>
-    <row r="7" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="O6" t="s">
+        <v>714</v>
+      </c>
+      <c r="P6" t="s">
+        <v>713</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="124" t="s">
         <v>325</v>
       </c>
@@ -9534,8 +10013,17 @@
       </c>
       <c r="K7" s="105"/>
       <c r="L7" s="128"/>
-    </row>
-    <row r="8" spans="1:12" ht="42" x14ac:dyDescent="0.2">
+      <c r="O7" t="s">
+        <v>648</v>
+      </c>
+      <c r="P7" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" ht="42" x14ac:dyDescent="0.2">
       <c r="A8" s="130" t="s">
         <v>71</v>
       </c>
@@ -9570,8 +10058,17 @@
         <v>487</v>
       </c>
       <c r="L8" s="105"/>
-    </row>
-    <row r="9" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+      <c r="O8" t="s">
+        <v>649</v>
+      </c>
+      <c r="P8" t="s">
+        <v>651</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" ht="48" x14ac:dyDescent="0.2">
       <c r="A9" s="124" t="s">
         <v>488</v>
       </c>
@@ -9606,8 +10103,17 @@
         <v>491</v>
       </c>
       <c r="L9" s="128"/>
-    </row>
-    <row r="10" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+      <c r="O9" t="s">
+        <v>648</v>
+      </c>
+      <c r="P9" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" ht="48" x14ac:dyDescent="0.2">
       <c r="A10" s="120" t="s">
         <v>492</v>
       </c>
@@ -9642,8 +10148,17 @@
         <v>496</v>
       </c>
       <c r="L10" s="105"/>
-    </row>
-    <row r="11" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+      <c r="O10" t="s">
+        <v>648</v>
+      </c>
+      <c r="P10" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" ht="48" x14ac:dyDescent="0.2">
       <c r="A11" s="124" t="s">
         <v>426</v>
       </c>
@@ -9674,8 +10189,17 @@
       </c>
       <c r="K11" s="105"/>
       <c r="L11" s="128"/>
-    </row>
-    <row r="12" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="O11" t="s">
+        <v>648</v>
+      </c>
+      <c r="P11" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="120" t="s">
         <v>497</v>
       </c>
@@ -9706,8 +10230,17 @@
       </c>
       <c r="K12" s="104"/>
       <c r="L12" s="105"/>
-    </row>
-    <row r="13" spans="1:12" ht="64" x14ac:dyDescent="0.2">
+      <c r="O12" t="s">
+        <v>648</v>
+      </c>
+      <c r="P12" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A13" s="192" t="s">
         <v>116</v>
       </c>
@@ -9740,8 +10273,17 @@
       </c>
       <c r="K13" s="104"/>
       <c r="L13" s="128"/>
-    </row>
-    <row r="14" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="O13" t="s">
+        <v>649</v>
+      </c>
+      <c r="P13" t="s">
+        <v>651</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="120" t="s">
         <v>132</v>
       </c>
@@ -9772,8 +10314,17 @@
       </c>
       <c r="K14" s="104"/>
       <c r="L14" s="105"/>
-    </row>
-    <row r="15" spans="1:12" ht="64" x14ac:dyDescent="0.2">
+      <c r="O14" t="s">
+        <v>649</v>
+      </c>
+      <c r="P14" t="s">
+        <v>651</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A15" s="124" t="s">
         <v>501</v>
       </c>
@@ -9806,8 +10357,17 @@
       </c>
       <c r="K15" s="104"/>
       <c r="L15" s="128"/>
-    </row>
-    <row r="16" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+      <c r="O15" t="s">
+        <v>648</v>
+      </c>
+      <c r="P15" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" ht="48" x14ac:dyDescent="0.2">
       <c r="A16" s="120" t="s">
         <v>137</v>
       </c>
@@ -9840,8 +10400,17 @@
       </c>
       <c r="K16" s="104"/>
       <c r="L16" s="105"/>
-    </row>
-    <row r="17" spans="1:12" ht="64" x14ac:dyDescent="0.2">
+      <c r="O16" t="s">
+        <v>648</v>
+      </c>
+      <c r="P16" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" ht="64" x14ac:dyDescent="0.2">
       <c r="A17" s="124" t="s">
         <v>317</v>
       </c>
@@ -9876,8 +10445,17 @@
         <v>507</v>
       </c>
       <c r="L17" s="128"/>
-    </row>
-    <row r="18" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+      <c r="O17" t="s">
+        <v>648</v>
+      </c>
+      <c r="P17" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" ht="48" x14ac:dyDescent="0.2">
       <c r="A18" s="120" t="s">
         <v>162</v>
       </c>
@@ -9910,8 +10488,20 @@
       </c>
       <c r="K18" s="104"/>
       <c r="L18" s="105"/>
-    </row>
-    <row r="19" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="O18" t="s">
+        <v>649</v>
+      </c>
+      <c r="P18" t="s">
+        <v>716</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>720</v>
+      </c>
+      <c r="S18" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="124" t="s">
         <v>179</v>
       </c>
@@ -9942,8 +10532,17 @@
       </c>
       <c r="K19" s="104"/>
       <c r="L19" s="128"/>
-    </row>
-    <row r="20" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+      <c r="O19" t="s">
+        <v>714</v>
+      </c>
+      <c r="P19" t="s">
+        <v>713</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" ht="48" x14ac:dyDescent="0.2">
       <c r="A20" s="120" t="s">
         <v>197</v>
       </c>
@@ -9976,8 +10575,17 @@
       </c>
       <c r="K20" s="105"/>
       <c r="L20" s="105"/>
-    </row>
-    <row r="21" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+      <c r="O20" t="s">
+        <v>714</v>
+      </c>
+      <c r="P20" t="s">
+        <v>713</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" ht="48" x14ac:dyDescent="0.2">
       <c r="A21" s="124" t="s">
         <v>510</v>
       </c>
@@ -10012,8 +10620,17 @@
         <v>514</v>
       </c>
       <c r="L21" s="128"/>
-    </row>
-    <row r="22" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+      <c r="O21" t="s">
+        <v>648</v>
+      </c>
+      <c r="P21" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" ht="48" x14ac:dyDescent="0.2">
       <c r="A22" s="120" t="s">
         <v>263</v>
       </c>
@@ -10046,8 +10663,17 @@
       </c>
       <c r="K22" s="104"/>
       <c r="L22" s="105"/>
-    </row>
-    <row r="23" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="O22" t="s">
+        <v>648</v>
+      </c>
+      <c r="P22" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="124" t="s">
         <v>269</v>
       </c>
@@ -10083,7 +10709,7 @@
       </c>
       <c r="L23" s="196"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24" s="23"/>
       <c r="B24" s="8"/>
       <c r="C24" s="23"/>
@@ -10096,7 +10722,7 @@
       <c r="J24" s="2"/>
       <c r="K24" s="98"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" s="23"/>
       <c r="B25" s="8"/>
       <c r="C25" s="29"/>
@@ -10109,7 +10735,7 @@
       <c r="J25" s="2"/>
       <c r="K25" s="96"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A26" s="23"/>
       <c r="B26" s="8"/>
       <c r="C26" s="23"/>
@@ -10122,7 +10748,7 @@
       <c r="J26" s="2"/>
       <c r="K26" s="98"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A27" s="23"/>
       <c r="B27" s="8"/>
       <c r="C27" s="9"/>
@@ -10135,7 +10761,7 @@
       <c r="J27" s="2"/>
       <c r="K27" s="96"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A28" s="23"/>
       <c r="B28" s="8"/>
       <c r="C28" s="23"/>
@@ -10148,7 +10774,7 @@
       <c r="J28" s="2"/>
       <c r="K28" s="96"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A29" s="23"/>
       <c r="B29" s="8"/>
       <c r="C29" s="23"/>
@@ -10161,7 +10787,7 @@
       <c r="J29" s="2"/>
       <c r="K29" s="96"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A30" s="23"/>
       <c r="B30" s="8"/>
       <c r="C30" s="23"/>
@@ -10174,7 +10800,7 @@
       <c r="J30" s="2"/>
       <c r="K30" s="96"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A31" s="23"/>
       <c r="B31" s="8"/>
       <c r="C31" s="29"/>
@@ -10187,7 +10813,7 @@
       <c r="J31" s="2"/>
       <c r="K31" s="96"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A32" s="23"/>
       <c r="B32" s="8"/>
       <c r="C32" s="23"/>
@@ -10563,19 +11189,23 @@
   <sheetPr>
     <tabColor theme="4" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R3" sqref="R3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.33203125" customWidth="1"/>
     <col min="2" max="2" width="33.33203125" customWidth="1"/>
-    <col min="3" max="10" width="22.33203125" customWidth="1"/>
-    <col min="11" max="11" width="22.33203125" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" customWidth="1"/>
+    <col min="4" max="11" width="22.33203125" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="0" hidden="1" customWidth="1"/>
+    <col min="15" max="20" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="204" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" s="204" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A1" s="89" t="s">
         <v>0</v>
       </c>
@@ -10612,8 +11242,32 @@
       <c r="L1" s="106" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="80" x14ac:dyDescent="0.2">
+      <c r="M1" s="216" t="s">
+        <v>638</v>
+      </c>
+      <c r="N1" s="216" t="s">
+        <v>639</v>
+      </c>
+      <c r="O1" s="216" t="s">
+        <v>640</v>
+      </c>
+      <c r="P1" s="216" t="s">
+        <v>641</v>
+      </c>
+      <c r="Q1" s="216" t="s">
+        <v>642</v>
+      </c>
+      <c r="R1" s="216" t="s">
+        <v>643</v>
+      </c>
+      <c r="S1" s="216" t="s">
+        <v>736</v>
+      </c>
+      <c r="T1" s="216" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="80" x14ac:dyDescent="0.2">
       <c r="A2" s="197" t="s">
         <v>518</v>
       </c>
@@ -10646,8 +11300,17 @@
       </c>
       <c r="K2" s="157"/>
       <c r="L2" s="187"/>
-    </row>
-    <row r="3" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="O2" t="s">
+        <v>649</v>
+      </c>
+      <c r="P2" t="s">
+        <v>715</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="68" t="s">
         <v>523</v>
       </c>
@@ -10678,6 +11341,15 @@
       </c>
       <c r="K3" s="168"/>
       <c r="L3" s="196"/>
+      <c r="O3" t="s">
+        <v>649</v>
+      </c>
+      <c r="P3" t="s">
+        <v>715</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>655</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="F2:F3">
@@ -10737,11 +11409,11 @@
   <sheetPr>
     <tabColor theme="4" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:L52"/>
+  <dimension ref="A1:T52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10760,7 +11432,7 @@
     <col min="12" max="16384" width="9.1640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="64" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A1" s="89" t="s">
         <v>0</v>
       </c>
@@ -10797,8 +11469,32 @@
       <c r="L1" s="106" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M1" s="216" t="s">
+        <v>638</v>
+      </c>
+      <c r="N1" s="216" t="s">
+        <v>639</v>
+      </c>
+      <c r="O1" s="216" t="s">
+        <v>640</v>
+      </c>
+      <c r="P1" s="216" t="s">
+        <v>641</v>
+      </c>
+      <c r="Q1" s="216" t="s">
+        <v>642</v>
+      </c>
+      <c r="R1" s="216" t="s">
+        <v>643</v>
+      </c>
+      <c r="S1" s="216" t="s">
+        <v>736</v>
+      </c>
+      <c r="T1" s="216" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="58" t="s">
         <v>526</v>
       </c>
@@ -10827,8 +11523,20 @@
       <c r="J2" s="47" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="O2" s="2" t="s">
+        <v>649</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>716</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>720</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="48" t="s">
         <v>529</v>
       </c>
@@ -10859,8 +11567,20 @@
       </c>
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O3" s="2" t="s">
+        <v>649</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>716</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>720</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="13"/>
       <c r="B4" s="8"/>
       <c r="C4" s="13"/>
@@ -10870,7 +11590,7 @@
       <c r="G4" s="3"/>
       <c r="H4" s="4"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" s="13"/>
       <c r="B5" s="8"/>
       <c r="C5" s="13"/>
@@ -10880,7 +11600,7 @@
       <c r="G5" s="3"/>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="13"/>
       <c r="B6" s="8"/>
       <c r="C6" s="13"/>
@@ -10890,7 +11610,7 @@
       <c r="G6" s="3"/>
       <c r="H6" s="4"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="13"/>
       <c r="B7" s="8"/>
       <c r="C7" s="21"/>
@@ -10900,7 +11620,7 @@
       <c r="G7" s="3"/>
       <c r="H7" s="4"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" s="13"/>
       <c r="B8" s="8"/>
       <c r="C8" s="13"/>
@@ -10910,7 +11630,7 @@
       <c r="G8" s="3"/>
       <c r="H8" s="4"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" s="13"/>
       <c r="B9" s="11"/>
       <c r="C9" s="13"/>
@@ -10919,7 +11639,7 @@
       <c r="F9" s="3"/>
       <c r="H9" s="4"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" s="13"/>
       <c r="B10" s="8"/>
       <c r="C10" s="21"/>
@@ -10929,7 +11649,7 @@
       <c r="G10" s="12"/>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" s="13"/>
       <c r="B11" s="8"/>
       <c r="C11" s="13"/>
@@ -10939,7 +11659,7 @@
       <c r="G11" s="3"/>
       <c r="H11" s="4"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" s="13"/>
       <c r="B12" s="8"/>
       <c r="C12" s="13"/>
@@ -10949,7 +11669,7 @@
       <c r="G12" s="3"/>
       <c r="H12" s="4"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" s="13"/>
       <c r="B13" s="8"/>
       <c r="C13" s="13"/>
@@ -10959,7 +11679,7 @@
       <c r="G13" s="3"/>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" s="13"/>
       <c r="B14" s="8"/>
       <c r="C14" s="13"/>
@@ -10969,7 +11689,7 @@
       <c r="G14" s="3"/>
       <c r="H14" s="4"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" s="13"/>
       <c r="B15" s="8"/>
       <c r="C15" s="13"/>
@@ -10978,7 +11698,7 @@
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" s="13"/>
       <c r="B16" s="11"/>
       <c r="D16" s="17"/>
@@ -11442,9 +12162,11 @@
   <sheetPr>
     <tabColor theme="4" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -11458,7 +12180,7 @@
     <col min="12" max="16384" width="9.1640625" style="84"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" ht="48" x14ac:dyDescent="0.2">
       <c r="A1" s="89" t="s">
         <v>0</v>
       </c>
@@ -11495,8 +12217,32 @@
       <c r="L1" s="106" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+      <c r="M1" s="216" t="s">
+        <v>638</v>
+      </c>
+      <c r="N1" s="216" t="s">
+        <v>639</v>
+      </c>
+      <c r="O1" s="216" t="s">
+        <v>640</v>
+      </c>
+      <c r="P1" s="216" t="s">
+        <v>641</v>
+      </c>
+      <c r="Q1" s="216" t="s">
+        <v>642</v>
+      </c>
+      <c r="R1" s="216" t="s">
+        <v>643</v>
+      </c>
+      <c r="S1" s="216" t="s">
+        <v>736</v>
+      </c>
+      <c r="T1" s="216" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="84" t="s">
         <v>532</v>
       </c>
@@ -11528,8 +12274,17 @@
         <v>76</v>
       </c>
       <c r="K2" s="2"/>
-    </row>
-    <row r="3" spans="1:12" ht="96" x14ac:dyDescent="0.2">
+      <c r="O2" s="84" t="s">
+        <v>714</v>
+      </c>
+      <c r="P2" s="84" t="s">
+        <v>713</v>
+      </c>
+      <c r="Q2" s="84" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="96" x14ac:dyDescent="0.2">
       <c r="A3" s="48" t="s">
         <v>536</v>
       </c>
@@ -11562,6 +12317,15 @@
       </c>
       <c r="K3" s="5"/>
       <c r="L3" s="119"/>
+      <c r="O3" s="84" t="s">
+        <v>717</v>
+      </c>
+      <c r="P3" s="84" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q3" s="84" t="s">
+        <v>608</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="F2:F3">
@@ -11624,9 +12388,11 @@
   <sheetPr>
     <tabColor theme="4" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -11636,7 +12402,7 @@
     <col min="11" max="11" width="21.5" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" ht="48" x14ac:dyDescent="0.2">
       <c r="A1" s="89" t="s">
         <v>0</v>
       </c>
@@ -11673,8 +12439,32 @@
       <c r="L1" s="106" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="160" x14ac:dyDescent="0.2">
+      <c r="M1" s="216" t="s">
+        <v>638</v>
+      </c>
+      <c r="N1" s="216" t="s">
+        <v>639</v>
+      </c>
+      <c r="O1" s="216" t="s">
+        <v>640</v>
+      </c>
+      <c r="P1" s="216" t="s">
+        <v>641</v>
+      </c>
+      <c r="Q1" s="216" t="s">
+        <v>642</v>
+      </c>
+      <c r="R1" s="216" t="s">
+        <v>643</v>
+      </c>
+      <c r="S1" s="216" t="s">
+        <v>736</v>
+      </c>
+      <c r="T1" s="216" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="160" x14ac:dyDescent="0.2">
       <c r="A2" s="84" t="s">
         <v>541</v>
       </c>
@@ -11706,8 +12496,17 @@
         <v>76</v>
       </c>
       <c r="K2" s="2"/>
-    </row>
-    <row r="3" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+      <c r="O2" t="s">
+        <v>648</v>
+      </c>
+      <c r="P2" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="48" t="s">
         <v>544</v>
       </c>
@@ -11740,6 +12539,15 @@
       </c>
       <c r="K3" s="5"/>
       <c r="L3" s="111"/>
+      <c r="O3" t="s">
+        <v>648</v>
+      </c>
+      <c r="P3" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>608</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="F2:F3">
@@ -11799,10 +12607,10 @@
   <sheetPr>
     <tabColor theme="4" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11813,7 +12621,7 @@
     <col min="11" max="11" width="20.1640625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" ht="48" x14ac:dyDescent="0.2">
       <c r="A1" s="89" t="s">
         <v>0</v>
       </c>
@@ -11850,8 +12658,32 @@
       <c r="L1" s="106" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="112" x14ac:dyDescent="0.2">
+      <c r="M1" s="216" t="s">
+        <v>638</v>
+      </c>
+      <c r="N1" s="216" t="s">
+        <v>639</v>
+      </c>
+      <c r="O1" s="216" t="s">
+        <v>640</v>
+      </c>
+      <c r="P1" s="216" t="s">
+        <v>641</v>
+      </c>
+      <c r="Q1" s="216" t="s">
+        <v>642</v>
+      </c>
+      <c r="R1" s="216" t="s">
+        <v>643</v>
+      </c>
+      <c r="S1" s="216" t="s">
+        <v>736</v>
+      </c>
+      <c r="T1" s="216" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="112" x14ac:dyDescent="0.2">
       <c r="A2" s="84" t="s">
         <v>548</v>
       </c>
@@ -11883,8 +12715,17 @@
         <v>76</v>
       </c>
       <c r="K2" s="2"/>
-    </row>
-    <row r="3" spans="1:12" ht="64" x14ac:dyDescent="0.2">
+      <c r="O2" t="s">
+        <v>648</v>
+      </c>
+      <c r="P2" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A3" s="48" t="s">
         <v>552</v>
       </c>
@@ -11917,6 +12758,15 @@
       </c>
       <c r="K3" s="5"/>
       <c r="L3" s="111"/>
+      <c r="O3" t="s">
+        <v>648</v>
+      </c>
+      <c r="P3" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>608</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="F2:F3">
@@ -11995,7 +12845,7 @@
     <col min="11" max="16384" width="9.1640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A1" s="62" t="s">
         <v>0</v>
       </c>
@@ -12686,11 +13536,11 @@
   <sheetPr>
     <tabColor theme="4" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:L52"/>
+  <dimension ref="A1:T52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12706,7 +13556,7 @@
     <col min="12" max="16384" width="9.1640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="89" t="s">
         <v>0</v>
       </c>
@@ -12743,8 +13593,32 @@
       <c r="L1" s="106" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="64" x14ac:dyDescent="0.2">
+      <c r="M1" s="216" t="s">
+        <v>638</v>
+      </c>
+      <c r="N1" s="216" t="s">
+        <v>639</v>
+      </c>
+      <c r="O1" s="216" t="s">
+        <v>640</v>
+      </c>
+      <c r="P1" s="216" t="s">
+        <v>641</v>
+      </c>
+      <c r="Q1" s="216" t="s">
+        <v>642</v>
+      </c>
+      <c r="R1" s="216" t="s">
+        <v>643</v>
+      </c>
+      <c r="S1" s="216" t="s">
+        <v>736</v>
+      </c>
+      <c r="T1" s="216" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A2" s="44" t="s">
         <v>596</v>
       </c>
@@ -12775,8 +13649,17 @@
       <c r="J2" s="47" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O2" s="2" t="s">
+        <v>648</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="49" t="s">
         <v>602</v>
       </c>
@@ -12807,8 +13690,17 @@
       </c>
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O3" s="2" t="s">
+        <v>649</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>651</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="13"/>
       <c r="B4" s="8"/>
       <c r="C4" s="13"/>
@@ -12818,7 +13710,7 @@
       <c r="G4" s="3"/>
       <c r="H4" s="4"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" s="13"/>
       <c r="B5" s="8"/>
       <c r="C5" s="13"/>
@@ -12828,7 +13720,7 @@
       <c r="G5" s="3"/>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="13"/>
       <c r="B6" s="8"/>
       <c r="C6" s="13"/>
@@ -12838,7 +13730,7 @@
       <c r="G6" s="3"/>
       <c r="H6" s="4"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="13"/>
       <c r="B7" s="8"/>
       <c r="C7" s="21"/>
@@ -12848,7 +13740,7 @@
       <c r="G7" s="3"/>
       <c r="H7" s="4"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" s="13"/>
       <c r="B8" s="8"/>
       <c r="C8" s="13"/>
@@ -12858,7 +13750,7 @@
       <c r="G8" s="3"/>
       <c r="H8" s="4"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" s="13"/>
       <c r="B9" s="11"/>
       <c r="C9" s="13"/>
@@ -12867,7 +13759,7 @@
       <c r="F9" s="3"/>
       <c r="H9" s="4"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" s="13"/>
       <c r="B10" s="8"/>
       <c r="C10" s="21"/>
@@ -12877,7 +13769,7 @@
       <c r="G10" s="12"/>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" s="13"/>
       <c r="B11" s="8"/>
       <c r="C11" s="13"/>
@@ -12887,7 +13779,7 @@
       <c r="G11" s="3"/>
       <c r="H11" s="4"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" s="13"/>
       <c r="B12" s="8"/>
       <c r="C12" s="13"/>
@@ -12897,7 +13789,7 @@
       <c r="G12" s="3"/>
       <c r="H12" s="4"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" s="13"/>
       <c r="B13" s="8"/>
       <c r="C13" s="13"/>
@@ -12907,7 +13799,7 @@
       <c r="G13" s="3"/>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" s="13"/>
       <c r="B14" s="8"/>
       <c r="C14" s="13"/>
@@ -12917,7 +13809,7 @@
       <c r="G14" s="3"/>
       <c r="H14" s="4"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" s="13"/>
       <c r="B15" s="8"/>
       <c r="C15" s="13"/>
@@ -12926,7 +13818,7 @@
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" s="13"/>
       <c r="B16" s="11"/>
       <c r="D16" s="17"/>
@@ -13678,26 +14570,26 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B32" s="215" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>728</v>
+      </c>
+      <c r="B33" s="215" t="s">
         <v>729</v>
-      </c>
-      <c r="B33" s="215" t="s">
-        <v>730</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
+        <v>731</v>
+      </c>
+      <c r="B34" t="s">
         <v>732</v>
-      </c>
-      <c r="B34" t="s">
-        <v>733</v>
       </c>
     </row>
   </sheetData>
@@ -13741,17 +14633,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD28D2AD-F644-014B-AA60-BBFA3B19D155}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="13.83203125" customWidth="1"/>
     <col min="3" max="3" width="15.83203125" customWidth="1"/>
-    <col min="4" max="4" width="26.6640625" style="232" customWidth="1"/>
+    <col min="4" max="4" width="26.6640625" style="221" customWidth="1"/>
     <col min="6" max="6" width="20.33203125" customWidth="1"/>
     <col min="7" max="7" width="12.5" customWidth="1"/>
     <col min="8" max="8" width="18.33203125" customWidth="1"/>
@@ -13767,7 +14659,7 @@
       <c r="C1" t="s">
         <v>612</v>
       </c>
-      <c r="D1" s="232" t="s">
+      <c r="D1" s="221" t="s">
         <v>672</v>
       </c>
       <c r="E1" t="s">
@@ -13824,8 +14716,8 @@
       <c r="B4" t="s">
         <v>712</v>
       </c>
-      <c r="D4" s="232" t="s">
-        <v>722</v>
+      <c r="D4" s="221" t="s">
+        <v>721</v>
       </c>
       <c r="H4" t="s">
         <v>109</v>
@@ -13833,16 +14725,138 @@
     </row>
     <row r="5" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>733</v>
+      </c>
+      <c r="B5" t="s">
         <v>734</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" s="221" t="s">
         <v>735</v>
-      </c>
-      <c r="D5" s="232" t="s">
-        <v>736</v>
       </c>
       <c r="H5" t="s">
         <v>297</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>741</v>
+      </c>
+      <c r="B6" t="s">
+        <v>742</v>
+      </c>
+      <c r="D6" s="221" t="s">
+        <v>726</v>
+      </c>
+      <c r="H6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>743</v>
+      </c>
+      <c r="B7" t="s">
+        <v>744</v>
+      </c>
+      <c r="D7" s="221" t="s">
+        <v>735</v>
+      </c>
+      <c r="H7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>745</v>
+      </c>
+      <c r="B8" t="s">
+        <v>746</v>
+      </c>
+      <c r="D8" s="221" t="s">
+        <v>747</v>
+      </c>
+      <c r="H8" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>748</v>
+      </c>
+      <c r="B9" t="s">
+        <v>722</v>
+      </c>
+      <c r="H9" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>749</v>
+      </c>
+      <c r="B10" t="s">
+        <v>726</v>
+      </c>
+      <c r="H10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>750</v>
+      </c>
+      <c r="B11" t="s">
+        <v>723</v>
+      </c>
+      <c r="D11" s="221" t="s">
+        <v>708</v>
+      </c>
+      <c r="H11" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>751</v>
+      </c>
+      <c r="B12" t="s">
+        <v>752</v>
+      </c>
+      <c r="H12" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>753</v>
+      </c>
+      <c r="B13" t="s">
+        <v>725</v>
+      </c>
+      <c r="H13" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>754</v>
+      </c>
+      <c r="B14" t="s">
+        <v>755</v>
+      </c>
+      <c r="H14" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>756</v>
+      </c>
+      <c r="B15" t="s">
+        <v>757</v>
+      </c>
+      <c r="H15" t="s">
+        <v>758</v>
       </c>
     </row>
   </sheetData>
@@ -13859,11 +14873,11 @@
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="A1:R57"/>
+  <dimension ref="A1:T57"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M1" sqref="M1:R1"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13880,11 +14894,11 @@
     <col min="10" max="10" width="19" style="135" customWidth="1"/>
     <col min="11" max="11" width="39.33203125" style="157" customWidth="1"/>
     <col min="12" max="12" width="26.6640625" style="135" customWidth="1"/>
-    <col min="13" max="18" width="16" style="135" customWidth="1"/>
-    <col min="19" max="16384" width="8.83203125" style="135"/>
+    <col min="13" max="20" width="16" style="135" customWidth="1"/>
+    <col min="21" max="16384" width="8.83203125" style="135"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="202" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" s="202" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A1" s="89" t="s">
         <v>0</v>
       </c>
@@ -13939,8 +14953,14 @@
       <c r="R1" s="216" t="s">
         <v>643</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+      <c r="S1" s="216" t="s">
+        <v>736</v>
+      </c>
+      <c r="T1" s="216" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="64" t="s">
         <v>339</v>
       </c>
@@ -13990,7 +15010,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="96" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" ht="96" x14ac:dyDescent="0.2">
       <c r="A3" s="68" t="s">
         <v>342</v>
       </c>
@@ -14043,8 +15063,11 @@
       <c r="R3" s="135" t="s">
         <v>652</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" ht="112" x14ac:dyDescent="0.2">
+      <c r="S3" s="135" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="112" x14ac:dyDescent="0.2">
       <c r="A4" s="64" t="s">
         <v>116</v>
       </c>
@@ -14098,7 +15121,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="48" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" ht="48" x14ac:dyDescent="0.2">
       <c r="A5" s="166" t="s">
         <v>352</v>
       </c>
@@ -14152,7 +15175,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="80" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" ht="80" x14ac:dyDescent="0.2">
       <c r="A6" s="169" t="s">
         <v>357</v>
       </c>
@@ -14204,7 +15227,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="128" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" ht="128" x14ac:dyDescent="0.2">
       <c r="A7" s="124" t="s">
         <v>361</v>
       </c>
@@ -14256,7 +15279,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="64" t="s">
         <v>273</v>
       </c>
@@ -14310,7 +15333,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="48" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" ht="48" x14ac:dyDescent="0.2">
       <c r="A9" s="166" t="s">
         <v>368</v>
       </c>
@@ -14364,7 +15387,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" s="175"/>
       <c r="B10" s="176"/>
       <c r="C10" s="175"/>
@@ -14377,7 +15400,7 @@
       <c r="J10" s="157"/>
       <c r="K10" s="96"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" s="175"/>
       <c r="B11" s="176"/>
       <c r="D11" s="177"/>
@@ -14389,7 +15412,7 @@
       <c r="J11" s="157"/>
       <c r="K11" s="97"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" s="175"/>
       <c r="B12" s="176"/>
       <c r="C12" s="175"/>
@@ -14402,7 +15425,7 @@
       <c r="J12" s="157"/>
       <c r="K12" s="96"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" s="175"/>
       <c r="B13" s="176"/>
       <c r="C13" s="175"/>
@@ -14415,7 +15438,7 @@
       <c r="J13" s="157"/>
       <c r="K13" s="96"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" s="175"/>
       <c r="B14" s="176"/>
       <c r="C14" s="175"/>
@@ -14428,7 +15451,7 @@
       <c r="J14" s="157"/>
       <c r="K14" s="96"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" s="175"/>
       <c r="B15" s="176"/>
       <c r="C15" s="180"/>
@@ -14441,7 +15464,7 @@
       <c r="J15" s="157"/>
       <c r="K15" s="96"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" s="175"/>
       <c r="B16" s="176"/>
       <c r="C16" s="175"/>
@@ -15038,11 +16061,11 @@
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="A1:R56"/>
+  <dimension ref="A1:T56"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="L1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O1" sqref="O1:Q1"/>
+      <selection pane="bottomLeft" activeCell="S4" sqref="S4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15064,11 +16087,11 @@
     <col min="15" max="15" width="14" style="84" customWidth="1"/>
     <col min="16" max="16" width="22" style="84" customWidth="1"/>
     <col min="17" max="17" width="13.1640625" style="84" customWidth="1"/>
-    <col min="18" max="18" width="14.33203125" style="84" customWidth="1"/>
-    <col min="19" max="16384" width="8.83203125" style="84"/>
+    <col min="18" max="20" width="14.33203125" style="84" customWidth="1"/>
+    <col min="21" max="16384" width="8.83203125" style="84"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="202" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" s="202" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A1" s="89" t="s">
         <v>0</v>
       </c>
@@ -15123,8 +16146,14 @@
       <c r="R1" s="216" t="s">
         <v>643</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" ht="64.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S1" s="216" t="s">
+        <v>736</v>
+      </c>
+      <c r="T1" s="216" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="64.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="64" t="s">
         <v>371</v>
       </c>
@@ -15178,7 +16207,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="112" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" ht="112" x14ac:dyDescent="0.2">
       <c r="A3" s="68" t="s">
         <v>376</v>
       </c>
@@ -15231,8 +16260,11 @@
       <c r="R3" s="84" t="s">
         <v>653</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+      <c r="S3" s="84" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="64" t="s">
         <v>381</v>
       </c>
@@ -15286,7 +16318,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" s="23"/>
       <c r="B5" s="8"/>
       <c r="C5" s="23"/>
@@ -15299,7 +16331,7 @@
       <c r="J5" s="2"/>
       <c r="K5" s="84"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="23"/>
       <c r="B6" s="8"/>
       <c r="C6" s="29"/>
@@ -15312,7 +16344,7 @@
       <c r="J6" s="2"/>
       <c r="K6" s="84"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="23"/>
       <c r="B7" s="8"/>
       <c r="C7" s="23"/>
@@ -15325,7 +16357,7 @@
       <c r="J7" s="2"/>
       <c r="K7" s="84"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" s="23"/>
       <c r="B8" s="8"/>
       <c r="D8" s="23"/>
@@ -15337,7 +16369,7 @@
       <c r="J8" s="2"/>
       <c r="K8" s="84"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" s="23"/>
       <c r="B9" s="8"/>
       <c r="C9" s="23"/>
@@ -15350,7 +16382,7 @@
       <c r="J9" s="2"/>
       <c r="K9" s="96"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" s="23"/>
       <c r="B10" s="8"/>
       <c r="C10" s="23"/>
@@ -15363,7 +16395,7 @@
       <c r="J10" s="2"/>
       <c r="K10" s="97"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" s="23"/>
       <c r="B11" s="8"/>
       <c r="C11" s="23"/>
@@ -15376,7 +16408,7 @@
       <c r="J11" s="2"/>
       <c r="K11" s="96"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" s="23"/>
       <c r="B12" s="8"/>
       <c r="C12" s="29"/>
@@ -15389,7 +16421,7 @@
       <c r="J12" s="2"/>
       <c r="K12" s="96"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" s="23"/>
       <c r="B13" s="8"/>
       <c r="C13" s="23"/>
@@ -15402,7 +16434,7 @@
       <c r="J13" s="2"/>
       <c r="K13" s="96"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" s="23"/>
       <c r="B14" s="8"/>
       <c r="D14" s="23"/>
@@ -15414,7 +16446,7 @@
       <c r="J14" s="2"/>
       <c r="K14" s="96"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" s="23"/>
       <c r="B15" s="8"/>
       <c r="C15" s="23"/>
@@ -15427,7 +16459,7 @@
       <c r="J15" s="2"/>
       <c r="K15" s="96"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" s="23"/>
       <c r="B16" s="8"/>
       <c r="C16" s="23"/>
@@ -16090,11 +17122,11 @@
     <tabColor rgb="FFC00000"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R49"/>
+  <dimension ref="A1:T49"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M1" sqref="M1:R1"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16116,10 +17148,13 @@
     <col min="15" max="15" width="18.83203125" style="32" customWidth="1"/>
     <col min="16" max="16" width="21.33203125" style="32" customWidth="1"/>
     <col min="17" max="17" width="22" style="32" customWidth="1"/>
-    <col min="18" max="16384" width="9.1640625" style="32"/>
+    <col min="18" max="18" width="9.1640625" style="32"/>
+    <col min="19" max="19" width="18.1640625" style="32" customWidth="1"/>
+    <col min="20" max="20" width="16" style="32" customWidth="1"/>
+    <col min="21" max="16384" width="9.1640625" style="32"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="200" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" s="200" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A1" s="91" t="s">
         <v>0</v>
       </c>
@@ -16174,8 +17209,14 @@
       <c r="R1" s="216" t="s">
         <v>643</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" ht="209.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S1" s="216" t="s">
+        <v>736</v>
+      </c>
+      <c r="T1" s="216" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="209.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="120" t="s">
         <v>12</v>
       </c>
@@ -16214,13 +17255,13 @@
         <v>648</v>
       </c>
       <c r="P2" s="32" t="s">
-        <v>713</v>
+        <v>650</v>
       </c>
       <c r="Q2" s="32" t="s">
         <v>608</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="80" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" ht="80" x14ac:dyDescent="0.2">
       <c r="A3" s="124" t="s">
         <v>22</v>
       </c>
@@ -16265,7 +17306,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="4" spans="1:18" s="116" customFormat="1" ht="144" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" s="116" customFormat="1" ht="144" x14ac:dyDescent="0.2">
       <c r="A4" s="130" t="s">
         <v>32</v>
       </c>
@@ -16309,8 +17350,11 @@
       <c r="Q4" s="116" t="s">
         <v>608</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" ht="64" x14ac:dyDescent="0.2">
+      <c r="T4" s="116" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A5" s="124" t="s">
         <v>39</v>
       </c>
@@ -16355,7 +17399,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="120" t="s">
         <v>45</v>
       </c>
@@ -16400,7 +17444,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="48" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" ht="48" x14ac:dyDescent="0.2">
       <c r="A7" s="124" t="s">
         <v>51</v>
       </c>
@@ -16445,7 +17489,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="123.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" ht="123.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="120" t="s">
         <v>56</v>
       </c>
@@ -16484,13 +17528,13 @@
         <v>648</v>
       </c>
       <c r="P8" s="32" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="Q8" s="32" t="s">
         <v>710</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="64" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A9" s="124" t="s">
         <v>64</v>
       </c>
@@ -16526,16 +17570,16 @@
       </c>
       <c r="L9" s="128"/>
       <c r="O9" s="32" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="P9" s="32" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="Q9" s="32" t="s">
         <v>708</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="64" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A10" s="120" t="s">
         <v>71</v>
       </c>
@@ -16574,13 +17618,13 @@
         <v>649</v>
       </c>
       <c r="P10" s="32" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="Q10" s="32" t="s">
         <v>655</v>
       </c>
     </row>
-    <row r="11" spans="1:18" s="208" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" s="208" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="124" t="s">
         <v>78</v>
       </c>
@@ -16623,7 +17667,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="120" t="s">
         <v>82</v>
       </c>
@@ -16668,7 +17712,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="124" t="s">
         <v>88</v>
       </c>
@@ -16713,39 +17757,39 @@
         <v>608</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="228" t="s">
+    <row r="14" spans="1:20" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="217" t="s">
         <v>95</v>
       </c>
-      <c r="B14" s="229" t="s">
+      <c r="B14" s="218" t="s">
         <v>96</v>
       </c>
-      <c r="C14" s="228" t="s">
+      <c r="C14" s="217" t="s">
         <v>97</v>
       </c>
       <c r="D14" s="152" t="s">
         <v>98</v>
       </c>
-      <c r="E14" s="230" t="s">
+      <c r="E14" s="219" t="s">
         <v>99</v>
       </c>
-      <c r="F14" s="228" t="s">
+      <c r="F14" s="217" t="s">
         <v>27</v>
       </c>
-      <c r="G14" s="228" t="s">
+      <c r="G14" s="217" t="s">
         <v>100</v>
       </c>
-      <c r="H14" s="228" t="s">
+      <c r="H14" s="217" t="s">
         <v>29</v>
       </c>
-      <c r="I14" s="231" t="s">
+      <c r="I14" s="220" t="s">
         <v>19</v>
       </c>
-      <c r="J14" s="231" t="s">
+      <c r="J14" s="220" t="s">
         <v>30</v>
       </c>
       <c r="K14" s="156"/>
-      <c r="L14" s="231"/>
+      <c r="L14" s="220"/>
       <c r="O14" s="32" t="s">
         <v>648</v>
       </c>
@@ -16756,7 +17800,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="124" t="s">
         <v>105</v>
       </c>
@@ -16801,7 +17845,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="96" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" ht="96" x14ac:dyDescent="0.2">
       <c r="A16" s="120" t="s">
         <v>111</v>
       </c>
@@ -16846,7 +17890,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="96" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:19" ht="96" x14ac:dyDescent="0.2">
       <c r="A17" s="124" t="s">
         <v>116</v>
       </c>
@@ -16885,13 +17929,13 @@
         <v>649</v>
       </c>
       <c r="P17" s="32" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="Q17" s="32" t="s">
         <v>655</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="120" t="s">
         <v>121</v>
       </c>
@@ -16934,7 +17978,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="19" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:19" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="124" t="s">
         <v>126</v>
       </c>
@@ -16979,7 +18023,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="20" spans="1:17" ht="48" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:19" ht="48" x14ac:dyDescent="0.2">
       <c r="A20" s="120" t="s">
         <v>132</v>
       </c>
@@ -17018,13 +18062,13 @@
         <v>649</v>
       </c>
       <c r="P20" s="32" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="Q20" s="32" t="s">
         <v>655</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="48" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:19" ht="48" x14ac:dyDescent="0.2">
       <c r="A21" s="124" t="s">
         <v>137</v>
       </c>
@@ -17069,7 +18113,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="128" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:19" ht="128" x14ac:dyDescent="0.2">
       <c r="A22" s="120" t="s">
         <v>144</v>
       </c>
@@ -17114,7 +18158,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:19" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="124" t="s">
         <v>151</v>
       </c>
@@ -17153,13 +18197,13 @@
         <v>649</v>
       </c>
       <c r="P23" s="32" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="Q23" s="32" t="s">
-        <v>719</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="120" t="s">
         <v>157</v>
       </c>
@@ -17198,13 +18242,13 @@
         <v>649</v>
       </c>
       <c r="P24" s="32" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="Q24" s="32" t="s">
-        <v>719</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" ht="48" x14ac:dyDescent="0.2">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" ht="48" x14ac:dyDescent="0.2">
       <c r="A25" s="124" t="s">
         <v>162</v>
       </c>
@@ -17243,13 +18287,16 @@
         <v>649</v>
       </c>
       <c r="P25" s="32" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="Q25" s="32" t="s">
-        <v>721</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+        <v>720</v>
+      </c>
+      <c r="S25" s="32" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="120" t="s">
         <v>168</v>
       </c>
@@ -17288,13 +18335,13 @@
         <v>649</v>
       </c>
       <c r="P26" s="32" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="Q26" s="32" t="s">
-        <v>719</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="124" t="s">
         <v>174</v>
       </c>
@@ -17333,13 +18380,13 @@
         <v>649</v>
       </c>
       <c r="P27" s="32" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="Q27" s="32" t="s">
-        <v>719</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" ht="48" x14ac:dyDescent="0.2">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" ht="64" x14ac:dyDescent="0.2">
       <c r="A28" s="120" t="s">
         <v>179</v>
       </c>
@@ -17375,16 +18422,16 @@
       </c>
       <c r="L28" s="105"/>
       <c r="O28" s="32" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="P28" s="32" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="Q28" s="32" t="s">
-        <v>723</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" ht="64" x14ac:dyDescent="0.2">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" ht="64" x14ac:dyDescent="0.2">
       <c r="A29" s="124" t="s">
         <v>185</v>
       </c>
@@ -17420,7 +18467,7 @@
       </c>
       <c r="L29" s="128"/>
       <c r="O29" s="32" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="P29" s="32" t="s">
         <v>650</v>
@@ -17429,7 +18476,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="30" spans="1:17" ht="48" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:19" ht="48" x14ac:dyDescent="0.2">
       <c r="A30" s="120" t="s">
         <v>192</v>
       </c>
@@ -17468,13 +18515,13 @@
         <v>649</v>
       </c>
       <c r="P30" s="32" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="Q30" s="32" t="s">
         <v>655</v>
       </c>
     </row>
-    <row r="31" spans="1:17" ht="112" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:19" ht="112" x14ac:dyDescent="0.2">
       <c r="A31" s="124" t="s">
         <v>197</v>
       </c>
@@ -17510,16 +18557,16 @@
       </c>
       <c r="L31" s="128"/>
       <c r="O31" s="32" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="P31" s="32" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="Q31" s="32" t="s">
         <v>708</v>
       </c>
     </row>
-    <row r="32" spans="1:17" ht="48" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:19" ht="48" x14ac:dyDescent="0.2">
       <c r="A32" s="120" t="s">
         <v>202</v>
       </c>
@@ -17555,7 +18602,7 @@
       </c>
       <c r="L32" s="105"/>
       <c r="O32" s="32" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="P32" s="32" t="s">
         <v>650</v>
@@ -17564,7 +18611,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="33" spans="1:17" ht="192" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:19" ht="192" x14ac:dyDescent="0.2">
       <c r="A33" s="124" t="s">
         <v>209</v>
       </c>
@@ -17598,16 +18645,16 @@
       <c r="K33" s="129"/>
       <c r="L33" s="128"/>
       <c r="O33" s="32" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="P33" s="32" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="Q33" s="32" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17" ht="48" x14ac:dyDescent="0.2">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" ht="48" x14ac:dyDescent="0.2">
       <c r="A34" s="120" t="s">
         <v>214</v>
       </c>
@@ -17643,16 +18690,16 @@
       </c>
       <c r="L34" s="105"/>
       <c r="O34" s="32" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="P34" s="32" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="Q34" s="32" t="s">
-        <v>725</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" ht="48" x14ac:dyDescent="0.2">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" ht="48" x14ac:dyDescent="0.2">
       <c r="A35" s="124" t="s">
         <v>220</v>
       </c>
@@ -17686,16 +18733,16 @@
       <c r="K35" s="129"/>
       <c r="L35" s="128"/>
       <c r="O35" s="32" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="P35" s="32" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="Q35" s="32" t="s">
-        <v>726</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" ht="32" x14ac:dyDescent="0.2">
       <c r="A36" s="120" t="s">
         <v>225</v>
       </c>
@@ -17734,13 +18781,16 @@
         <v>649</v>
       </c>
       <c r="P36" s="32" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="Q36" s="32" t="s">
-        <v>721</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+        <v>720</v>
+      </c>
+      <c r="S36" s="32" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" ht="32" x14ac:dyDescent="0.2">
       <c r="A37" s="124" t="s">
         <v>230</v>
       </c>
@@ -17776,16 +18826,16 @@
       </c>
       <c r="L37" s="128"/>
       <c r="O37" s="32" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="P37" s="32" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="Q37" s="32" t="s">
-        <v>727</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" ht="64" x14ac:dyDescent="0.2">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" ht="64" x14ac:dyDescent="0.2">
       <c r="A38" s="120" t="s">
         <v>236</v>
       </c>
@@ -17830,7 +18880,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="39" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:19" ht="32" x14ac:dyDescent="0.2">
       <c r="A39" s="124" t="s">
         <v>241</v>
       </c>
@@ -17875,7 +18925,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="40" spans="1:17" ht="64" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:19" ht="64" x14ac:dyDescent="0.2">
       <c r="A40" s="120" t="s">
         <v>246</v>
       </c>
@@ -17920,7 +18970,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="41" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:19" ht="32" x14ac:dyDescent="0.2">
       <c r="A41" s="124" t="s">
         <v>252</v>
       </c>
@@ -17956,16 +19006,16 @@
       </c>
       <c r="L41" s="128"/>
       <c r="O41" s="32" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="P41" s="32" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="Q41" s="32" t="s">
-        <v>727</v>
-      </c>
-    </row>
-    <row r="42" spans="1:17" ht="48" x14ac:dyDescent="0.2">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" ht="64" x14ac:dyDescent="0.2">
       <c r="A42" s="120" t="s">
         <v>257</v>
       </c>
@@ -18004,13 +19054,13 @@
         <v>649</v>
       </c>
       <c r="P42" s="32" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="Q42" s="32" t="s">
-        <v>720</v>
-      </c>
-    </row>
-    <row r="43" spans="1:17" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="124" t="s">
         <v>263</v>
       </c>
@@ -18055,7 +19105,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="44" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:19" ht="32" x14ac:dyDescent="0.2">
       <c r="A44" s="120" t="s">
         <v>269</v>
       </c>
@@ -18094,13 +19144,13 @@
         <v>649</v>
       </c>
       <c r="P44" s="32" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="Q44" s="32" t="s">
         <v>655</v>
       </c>
     </row>
-    <row r="45" spans="1:17" ht="64" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:19" ht="64" x14ac:dyDescent="0.2">
       <c r="A45" s="124" t="s">
         <v>273</v>
       </c>
@@ -18145,7 +19195,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="46" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:19" ht="32" x14ac:dyDescent="0.2">
       <c r="A46" s="120" t="s">
         <v>279</v>
       </c>
@@ -18184,13 +19234,13 @@
         <v>649</v>
       </c>
       <c r="P46" s="32" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="Q46" s="32" t="s">
         <v>655</v>
       </c>
     </row>
-    <row r="47" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:19" ht="32" x14ac:dyDescent="0.2">
       <c r="A47" s="124" t="s">
         <v>284</v>
       </c>
@@ -18229,13 +19279,13 @@
         <v>649</v>
       </c>
       <c r="P47" s="32" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="Q47" s="32" t="s">
         <v>655</v>
       </c>
     </row>
-    <row r="48" spans="1:17" ht="84.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:19" ht="84.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="120" t="s">
         <v>289</v>
       </c>
@@ -18390,35 +19440,35 @@
   <sheetPr>
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="A1:R60"/>
+  <dimension ref="A1:T60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q23" sqref="Q23"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20" style="41" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.6640625" style="41" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="25.6640625" style="41" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="25.6640625" style="34" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="54.5" style="41" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="22.1640625" style="32" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="24" style="32" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" style="32" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="16.1640625" style="32" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="16" style="32" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="23.6640625" style="32" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="26.5" style="32" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="40.6640625" style="41" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" style="41" customWidth="1"/>
+    <col min="4" max="4" width="25.6640625" style="34" customWidth="1"/>
+    <col min="5" max="5" width="54.5" style="41" customWidth="1"/>
+    <col min="6" max="6" width="22.1640625" style="32" customWidth="1"/>
+    <col min="7" max="7" width="24" style="32" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" style="32" customWidth="1"/>
+    <col min="9" max="9" width="16.1640625" style="32" customWidth="1"/>
+    <col min="10" max="10" width="16" style="32" customWidth="1"/>
+    <col min="11" max="11" width="23.6640625" style="32" customWidth="1"/>
+    <col min="12" max="12" width="26.5" style="32" customWidth="1"/>
     <col min="13" max="14" width="9.1640625" style="32"/>
     <col min="15" max="16" width="20.83203125" style="32" customWidth="1"/>
     <col min="17" max="17" width="16.33203125" style="32" customWidth="1"/>
-    <col min="18" max="18" width="14.6640625" style="32" customWidth="1"/>
-    <col min="19" max="16384" width="9.1640625" style="32"/>
+    <col min="18" max="20" width="14.6640625" style="32" customWidth="1"/>
+    <col min="21" max="16384" width="9.1640625" style="32"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="200" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" s="200" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A1" s="89" t="s">
         <v>0</v>
       </c>
@@ -18473,8 +19523,14 @@
       <c r="R1" s="216" t="s">
         <v>643</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="S1" s="216" t="s">
+        <v>736</v>
+      </c>
+      <c r="T1" s="216" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="130" t="s">
         <v>32</v>
       </c>
@@ -18517,7 +19573,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="48" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="124" t="s">
         <v>293</v>
       </c>
@@ -18560,7 +19616,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="95.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" ht="95.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="130" t="s">
         <v>56</v>
       </c>
@@ -18596,16 +19652,16 @@
       </c>
       <c r="L4" s="105"/>
       <c r="O4" s="32" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="P4" s="32" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="Q4" s="32" t="s">
         <v>710</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="48" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" ht="48" x14ac:dyDescent="0.2">
       <c r="A5" s="124" t="s">
         <v>64</v>
       </c>
@@ -18639,16 +19695,16 @@
       </c>
       <c r="L5" s="128"/>
       <c r="O5" s="32" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="P5" s="32" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="Q5" s="32" t="s">
         <v>708</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="48" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" s="120" t="s">
         <v>302</v>
       </c>
@@ -18671,7 +19727,7 @@
         <v>109</v>
       </c>
       <c r="H6" s="132" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="I6" s="105" t="s">
         <v>69</v>
@@ -18682,7 +19738,7 @@
       <c r="K6" s="136"/>
       <c r="L6" s="105"/>
     </row>
-    <row r="7" spans="1:18" ht="32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="124" t="s">
         <v>71</v>
       </c>
@@ -18727,39 +19783,39 @@
         <v>655</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="32" x14ac:dyDescent="0.2">
-      <c r="A8" s="219" t="s">
+    <row r="8" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+      <c r="A8" s="224" t="s">
         <v>95</v>
       </c>
-      <c r="B8" s="221" t="s">
+      <c r="B8" s="225" t="s">
         <v>96</v>
       </c>
-      <c r="C8" s="219" t="s">
+      <c r="C8" s="224" t="s">
         <v>97</v>
       </c>
       <c r="D8" s="152" t="s">
         <v>98</v>
       </c>
-      <c r="E8" s="220" t="s">
+      <c r="E8" s="226" t="s">
         <v>307</v>
       </c>
-      <c r="F8" s="218" t="s">
+      <c r="F8" s="223" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="218" t="s">
+      <c r="G8" s="223" t="s">
         <v>100</v>
       </c>
-      <c r="H8" s="218" t="s">
+      <c r="H8" s="223" t="s">
         <v>29</v>
       </c>
-      <c r="I8" s="217" t="s">
+      <c r="I8" s="222" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="217" t="s">
+      <c r="J8" s="222" t="s">
         <v>30</v>
       </c>
       <c r="K8" s="136"/>
-      <c r="L8" s="217"/>
+      <c r="L8" s="222"/>
       <c r="O8" s="32" t="s">
         <v>648</v>
       </c>
@@ -18770,71 +19826,71 @@
         <v>608</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="32" x14ac:dyDescent="0.2">
-      <c r="A9" s="219"/>
-      <c r="B9" s="221"/>
-      <c r="C9" s="219"/>
+    <row r="9" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+      <c r="A9" s="224"/>
+      <c r="B9" s="225"/>
+      <c r="C9" s="224"/>
       <c r="D9" s="153" t="s">
         <v>101</v>
       </c>
-      <c r="E9" s="220"/>
-      <c r="F9" s="218"/>
-      <c r="G9" s="218"/>
-      <c r="H9" s="218"/>
-      <c r="I9" s="217"/>
-      <c r="J9" s="217"/>
+      <c r="E9" s="226"/>
+      <c r="F9" s="223"/>
+      <c r="G9" s="223"/>
+      <c r="H9" s="223"/>
+      <c r="I9" s="222"/>
+      <c r="J9" s="222"/>
       <c r="K9" s="136"/>
-      <c r="L9" s="217"/>
-    </row>
-    <row r="10" spans="1:18" ht="32" x14ac:dyDescent="0.2">
-      <c r="A10" s="219"/>
-      <c r="B10" s="221"/>
-      <c r="C10" s="219"/>
+      <c r="L9" s="222"/>
+    </row>
+    <row r="10" spans="1:20" ht="32" x14ac:dyDescent="0.2">
+      <c r="A10" s="224"/>
+      <c r="B10" s="225"/>
+      <c r="C10" s="224"/>
       <c r="D10" s="153" t="s">
         <v>102</v>
       </c>
-      <c r="E10" s="220"/>
-      <c r="F10" s="218"/>
-      <c r="G10" s="218"/>
-      <c r="H10" s="218"/>
-      <c r="I10" s="217"/>
-      <c r="J10" s="217"/>
+      <c r="E10" s="226"/>
+      <c r="F10" s="223"/>
+      <c r="G10" s="223"/>
+      <c r="H10" s="223"/>
+      <c r="I10" s="222"/>
+      <c r="J10" s="222"/>
       <c r="K10" s="136"/>
-      <c r="L10" s="217"/>
-    </row>
-    <row r="11" spans="1:18" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="219"/>
-      <c r="B11" s="221"/>
-      <c r="C11" s="219"/>
+      <c r="L10" s="222"/>
+    </row>
+    <row r="11" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="224"/>
+      <c r="B11" s="225"/>
+      <c r="C11" s="224"/>
       <c r="D11" s="153" t="s">
         <v>103</v>
       </c>
-      <c r="E11" s="220"/>
-      <c r="F11" s="218"/>
-      <c r="G11" s="218"/>
-      <c r="H11" s="218"/>
-      <c r="I11" s="217"/>
-      <c r="J11" s="217"/>
+      <c r="E11" s="226"/>
+      <c r="F11" s="223"/>
+      <c r="G11" s="223"/>
+      <c r="H11" s="223"/>
+      <c r="I11" s="222"/>
+      <c r="J11" s="222"/>
       <c r="K11" s="154"/>
-      <c r="L11" s="217"/>
-    </row>
-    <row r="12" spans="1:18" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="219"/>
-      <c r="B12" s="221"/>
-      <c r="C12" s="219"/>
+      <c r="L11" s="222"/>
+    </row>
+    <row r="12" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="224"/>
+      <c r="B12" s="225"/>
+      <c r="C12" s="224"/>
       <c r="D12" s="153" t="s">
         <v>104</v>
       </c>
-      <c r="E12" s="220"/>
-      <c r="F12" s="218"/>
-      <c r="G12" s="218"/>
-      <c r="H12" s="218"/>
-      <c r="I12" s="217"/>
-      <c r="J12" s="217"/>
+      <c r="E12" s="226"/>
+      <c r="F12" s="223"/>
+      <c r="G12" s="223"/>
+      <c r="H12" s="223"/>
+      <c r="I12" s="222"/>
+      <c r="J12" s="222"/>
       <c r="K12" s="136"/>
-      <c r="L12" s="217"/>
-    </row>
-    <row r="13" spans="1:18" ht="48" x14ac:dyDescent="0.2">
+      <c r="L12" s="222"/>
+    </row>
+    <row r="13" spans="1:20" ht="48" x14ac:dyDescent="0.2">
       <c r="A13" s="124" t="s">
         <v>308</v>
       </c>
@@ -18877,7 +19933,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="120" t="s">
         <v>312</v>
       </c>
@@ -18920,7 +19976,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="64" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A15" s="124" t="s">
         <v>137</v>
       </c>
@@ -18965,7 +20021,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="48" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" ht="48" x14ac:dyDescent="0.2">
       <c r="A16" s="120" t="s">
         <v>317</v>
       </c>
@@ -19010,7 +20066,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="124" t="s">
         <v>162</v>
       </c>
@@ -19047,13 +20103,16 @@
         <v>649</v>
       </c>
       <c r="P17" s="32" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="Q17" s="32" t="s">
-        <v>721</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" ht="48" x14ac:dyDescent="0.2">
+        <v>720</v>
+      </c>
+      <c r="S17" s="32" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" ht="48" x14ac:dyDescent="0.2">
       <c r="A18" s="120" t="s">
         <v>197</v>
       </c>
@@ -19089,16 +20148,16 @@
       </c>
       <c r="L18" s="105"/>
       <c r="O18" s="32" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="P18" s="32" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="Q18" s="32" t="s">
         <v>708</v>
       </c>
     </row>
-    <row r="19" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="124" t="s">
         <v>225</v>
       </c>
@@ -19135,13 +20194,16 @@
         <v>649</v>
       </c>
       <c r="P19" s="32" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="Q19" s="32" t="s">
-        <v>721</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" ht="48" x14ac:dyDescent="0.2">
+        <v>720</v>
+      </c>
+      <c r="S19" s="32" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" ht="48" x14ac:dyDescent="0.2">
       <c r="A20" s="120" t="s">
         <v>325</v>
       </c>
@@ -19184,7 +20246,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="64" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:19" ht="64" x14ac:dyDescent="0.2">
       <c r="A21" s="124" t="s">
         <v>329</v>
       </c>
@@ -19227,7 +20289,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="120" t="s">
         <v>252</v>
       </c>
@@ -19261,16 +20323,16 @@
       </c>
       <c r="L22" s="105"/>
       <c r="O22" s="32" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="P22" s="32" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="Q22" s="32" t="s">
-        <v>727</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" ht="48" x14ac:dyDescent="0.2">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" ht="64" x14ac:dyDescent="0.2">
       <c r="A23" s="124" t="s">
         <v>334</v>
       </c>
@@ -19313,7 +20375,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="32" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:19" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="120" t="s">
         <v>269</v>
       </c>
@@ -19348,8 +20410,17 @@
         <v>269</v>
       </c>
       <c r="L24" s="105"/>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="O24" s="32" t="s">
+        <v>649</v>
+      </c>
+      <c r="P24" s="32" t="s">
+        <v>715</v>
+      </c>
+      <c r="Q24" s="32" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" s="33"/>
       <c r="B25" s="34"/>
       <c r="C25" s="33"/>
@@ -19360,7 +20431,7 @@
       <c r="H25" s="37"/>
       <c r="K25" s="94"/>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A26" s="33"/>
       <c r="B26" s="34"/>
       <c r="C26" s="33"/>
@@ -19371,7 +20442,7 @@
       <c r="H26" s="37"/>
       <c r="K26" s="93"/>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A27" s="33"/>
       <c r="B27" s="34"/>
       <c r="C27" s="33"/>
@@ -19382,7 +20453,7 @@
       <c r="H27" s="37"/>
       <c r="K27" s="93"/>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A28" s="33"/>
       <c r="B28" s="34"/>
       <c r="C28" s="33"/>
@@ -19393,7 +20464,7 @@
       <c r="H28" s="37"/>
       <c r="K28" s="93"/>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A29" s="33"/>
       <c r="B29" s="34"/>
       <c r="C29" s="33"/>
@@ -19404,7 +20475,7 @@
       <c r="H29" s="37"/>
       <c r="K29" s="93"/>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A30" s="33"/>
       <c r="B30" s="34"/>
       <c r="D30" s="38"/>
@@ -19414,7 +20485,7 @@
       <c r="H30" s="37"/>
       <c r="K30" s="93"/>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A31" s="33"/>
       <c r="B31" s="34"/>
       <c r="C31" s="33"/>
@@ -19425,7 +20496,7 @@
       <c r="H31" s="37"/>
       <c r="K31" s="93"/>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A32" s="33"/>
       <c r="B32" s="34"/>
       <c r="C32" s="33"/>
@@ -19832,6 +20903,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Status xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e">Draft</Status>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="221af607-abea-4d5e-830c-567dcc03c0ec" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000B1A1CF98C819F4881BB4349588D0C85" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ff8ef391852eaca4511043a54bffd4a2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cfc87205-1831-4b6c-a7b4-76d40079a43e" xmlns:ns3="221af607-abea-4d5e-830c-567dcc03c0ec" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="201dd8b781da46d5daa37e3355db44fe" ns2:_="" ns3:_="">
     <xsd:import namespace="cfc87205-1831-4b6c-a7b4-76d40079a43e"/>
@@ -20074,28 +21166,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Status xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e">Draft</Status>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="221af607-abea-4d5e-830c-567dcc03c0ec" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1A00443-9B7C-473F-A198-CBEB23A0BCC5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16D2CAB5-B21B-4A93-9D82-49FE3E36CF14}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="cfc87205-1831-4b6c-a7b4-76d40079a43e"/>
+    <ds:schemaRef ds:uri="221af607-abea-4d5e-830c-567dcc03c0ec"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19A23828-4FF7-4569-837D-B1B2C775409F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -20112,23 +21202,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16D2CAB5-B21B-4A93-9D82-49FE3E36CF14}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="cfc87205-1831-4b6c-a7b4-76d40079a43e"/>
-    <ds:schemaRef ds:uri="221af607-abea-4d5e-830c-567dcc03c0ec"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1A00443-9B7C-473F-A198-CBEB23A0BCC5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
docs: updates README.md and adds Turtle and YAML files
</commit_message>
<xml_diff>
--- a/inputs/Health-RI-Metadata_CoreGenericHealth_v2-0-0.xlsx
+++ b/inputs/Health-RI-Metadata_CoreGenericHealth_v2-0-0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexanderharms/Documents/Projects/Metadata automation/metadata-automation/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{193AB2A4-C193-3549-B69C-34F73A7121B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A1AE139-1F91-4E45-8393-26606798704B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37900" yWindow="-2640" windowWidth="34420" windowHeight="28300" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="80" yWindow="880" windowWidth="34420" windowHeight="20720" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="14" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2447" uniqueCount="759">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2449" uniqueCount="759">
   <si>
     <t>Property label</t>
   </si>
@@ -3699,6 +3699,12 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3709,12 +3715,6 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3723,36 +3723,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="199">
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="4" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -3775,11 +3745,41 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3885,11 +3885,11 @@
     </dxf>
     <dxf>
       <font>
-        <color theme="1"/>
+        <color rgb="FF9C5700"/>
       </font>
       <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="4" tint="0.59999389629810485"/>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3905,51 +3905,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color theme="1"/>
       </font>
       <fill>
         <patternFill patternType="solid">
           <bgColor theme="4" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4008,8 +3968,58 @@
         <color rgb="FF9C5700"/>
       </font>
       <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4035,11 +4045,31 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4065,51 +4095,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color theme="1"/>
       </font>
       <fill>
         <patternFill patternType="solid">
           <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="4" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4155,11 +4145,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color rgb="FF9C5700"/>
       </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+        <patternFill patternType="solid">
+          <bgColor theme="7" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4175,11 +4165,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C5700"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.79998168889431442"/>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4195,6 +4185,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
@@ -4205,11 +4205,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C5700"/>
+        <color theme="1"/>
       </font>
       <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
+        <patternFill patternType="solid">
+          <bgColor theme="4" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
     </dxf>
@@ -9119,40 +9119,40 @@
       </c>
     </row>
     <row r="6" spans="1:20" ht="32" x14ac:dyDescent="0.2">
-      <c r="A6" s="228" t="s">
+      <c r="A6" s="230" t="s">
         <v>95</v>
       </c>
-      <c r="B6" s="229" t="s">
+      <c r="B6" s="231" t="s">
         <v>96</v>
       </c>
-      <c r="C6" s="228" t="s">
+      <c r="C6" s="230" t="s">
         <v>97</v>
       </c>
       <c r="D6" s="138" t="s">
         <v>98</v>
       </c>
-      <c r="E6" s="230" t="s">
+      <c r="E6" s="232" t="s">
         <v>99</v>
       </c>
-      <c r="F6" s="227" t="s">
+      <c r="F6" s="229" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="227" t="s">
+      <c r="G6" s="229" t="s">
         <v>100</v>
       </c>
-      <c r="H6" s="227" t="s">
+      <c r="H6" s="229" t="s">
         <v>29</v>
       </c>
-      <c r="I6" s="231" t="s">
+      <c r="I6" s="227" t="s">
         <v>19</v>
       </c>
       <c r="J6" s="222" t="s">
         <v>30</v>
       </c>
-      <c r="K6" s="232" t="s">
+      <c r="K6" s="228" t="s">
         <v>471</v>
       </c>
-      <c r="L6" s="231"/>
+      <c r="L6" s="227"/>
       <c r="O6" s="32" t="s">
         <v>648</v>
       </c>
@@ -9164,68 +9164,68 @@
       </c>
     </row>
     <row r="7" spans="1:20" ht="32" x14ac:dyDescent="0.2">
-      <c r="A7" s="228"/>
-      <c r="B7" s="229"/>
-      <c r="C7" s="228"/>
+      <c r="A7" s="230"/>
+      <c r="B7" s="231"/>
+      <c r="C7" s="230"/>
       <c r="D7" s="139" t="s">
         <v>101</v>
       </c>
-      <c r="E7" s="230"/>
-      <c r="F7" s="227"/>
-      <c r="G7" s="227"/>
-      <c r="H7" s="227"/>
-      <c r="I7" s="231"/>
+      <c r="E7" s="232"/>
+      <c r="F7" s="229"/>
+      <c r="G7" s="229"/>
+      <c r="H7" s="229"/>
+      <c r="I7" s="227"/>
       <c r="J7" s="222"/>
-      <c r="K7" s="232"/>
-      <c r="L7" s="231"/>
+      <c r="K7" s="228"/>
+      <c r="L7" s="227"/>
     </row>
     <row r="8" spans="1:20" ht="32" x14ac:dyDescent="0.2">
-      <c r="A8" s="228"/>
-      <c r="B8" s="229"/>
-      <c r="C8" s="228"/>
+      <c r="A8" s="230"/>
+      <c r="B8" s="231"/>
+      <c r="C8" s="230"/>
       <c r="D8" s="139" t="s">
         <v>102</v>
       </c>
-      <c r="E8" s="230"/>
-      <c r="F8" s="227"/>
-      <c r="G8" s="227"/>
-      <c r="H8" s="227"/>
-      <c r="I8" s="231"/>
+      <c r="E8" s="232"/>
+      <c r="F8" s="229"/>
+      <c r="G8" s="229"/>
+      <c r="H8" s="229"/>
+      <c r="I8" s="227"/>
       <c r="J8" s="222"/>
-      <c r="K8" s="232"/>
-      <c r="L8" s="231"/>
+      <c r="K8" s="228"/>
+      <c r="L8" s="227"/>
     </row>
     <row r="9" spans="1:20" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="228"/>
-      <c r="B9" s="229"/>
-      <c r="C9" s="228"/>
+      <c r="A9" s="230"/>
+      <c r="B9" s="231"/>
+      <c r="C9" s="230"/>
       <c r="D9" s="139" t="s">
         <v>103</v>
       </c>
-      <c r="E9" s="230"/>
-      <c r="F9" s="227"/>
-      <c r="G9" s="227"/>
-      <c r="H9" s="227"/>
-      <c r="I9" s="231"/>
+      <c r="E9" s="232"/>
+      <c r="F9" s="229"/>
+      <c r="G9" s="229"/>
+      <c r="H9" s="229"/>
+      <c r="I9" s="227"/>
       <c r="J9" s="222"/>
-      <c r="K9" s="232"/>
-      <c r="L9" s="231"/>
+      <c r="K9" s="228"/>
+      <c r="L9" s="227"/>
     </row>
     <row r="10" spans="1:20" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="228"/>
-      <c r="B10" s="229"/>
-      <c r="C10" s="228"/>
+      <c r="A10" s="230"/>
+      <c r="B10" s="231"/>
+      <c r="C10" s="230"/>
       <c r="D10" s="139" t="s">
         <v>104</v>
       </c>
-      <c r="E10" s="230"/>
-      <c r="F10" s="227"/>
-      <c r="G10" s="227"/>
-      <c r="H10" s="227"/>
-      <c r="I10" s="231"/>
+      <c r="E10" s="232"/>
+      <c r="F10" s="229"/>
+      <c r="G10" s="229"/>
+      <c r="H10" s="229"/>
+      <c r="I10" s="227"/>
       <c r="J10" s="222"/>
-      <c r="K10" s="232"/>
-      <c r="L10" s="231"/>
+      <c r="K10" s="228"/>
+      <c r="L10" s="227"/>
     </row>
     <row r="11" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="120" t="s">
@@ -9581,17 +9581,17 @@
   </sheetData>
   <autoFilter ref="A1:L15" xr:uid="{FBE7E653-2382-46E4-9C76-9C694EDC9195}"/>
   <mergeCells count="11">
-    <mergeCell ref="L6:L10"/>
-    <mergeCell ref="K6:K10"/>
-    <mergeCell ref="H6:H10"/>
-    <mergeCell ref="I6:I10"/>
-    <mergeCell ref="J6:J10"/>
     <mergeCell ref="G6:G10"/>
     <mergeCell ref="A6:A10"/>
     <mergeCell ref="B6:B10"/>
     <mergeCell ref="C6:C10"/>
     <mergeCell ref="E6:E10"/>
     <mergeCell ref="F6:F10"/>
+    <mergeCell ref="L6:L10"/>
+    <mergeCell ref="K6:K10"/>
+    <mergeCell ref="H6:H10"/>
+    <mergeCell ref="I6:I10"/>
+    <mergeCell ref="J6:J10"/>
   </mergeCells>
   <conditionalFormatting sqref="F2:F6 F11:F15">
     <cfRule type="cellIs" dxfId="127" priority="7" operator="equal">
@@ -13419,42 +13419,42 @@
     <cfRule type="cellIs" dxfId="49" priority="41" operator="equal">
       <formula>"Optional"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="42" operator="equal">
-      <formula>"Recommended"</formula>
+    <cfRule type="cellIs" dxfId="48" priority="44" operator="equal">
+      <formula>"Conditional"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="47" priority="43" operator="equal">
       <formula>"Mandatory"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="44" operator="equal">
-      <formula>"Conditional"</formula>
+    <cfRule type="cellIs" dxfId="46" priority="42" operator="equal">
+      <formula>"Recommended"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D26:E28">
-    <cfRule type="cellIs" dxfId="45" priority="45" operator="equal">
-      <formula>"Optional"</formula>
+    <cfRule type="cellIs" dxfId="45" priority="48" operator="equal">
+      <formula>"Conditional"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="47" operator="equal">
+      <formula>"Mandatory"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="43" priority="46" operator="equal">
       <formula>"Recommended"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="47" operator="equal">
-      <formula>"Mandatory"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="48" operator="equal">
-      <formula>"Conditional"</formula>
+    <cfRule type="cellIs" dxfId="42" priority="45" operator="equal">
+      <formula>"Optional"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="cellIs" dxfId="41" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="54" operator="equal">
+      <formula>"Conditional"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="51" operator="equal">
       <formula>"Optional"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="52" operator="equal">
       <formula>"Recommended"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="53" operator="equal">
       <formula>"Mandatory"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="54" operator="equal">
-      <formula>"Conditional"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F7 E8">
@@ -13463,28 +13463,28 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9:F38">
-    <cfRule type="cellIs" dxfId="36" priority="33" operator="equal">
-      <formula>"Not added"</formula>
+    <cfRule type="cellIs" dxfId="36" priority="38" operator="equal">
+      <formula>"Mandatory"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="36" operator="equal">
-      <formula>"Optional"</formula>
+    <cfRule type="cellIs" dxfId="35" priority="39" operator="equal">
+      <formula>"Conditional"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="34" priority="37" operator="equal">
       <formula>"Recommended"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="38" operator="equal">
-      <formula>"Mandatory"</formula>
+    <cfRule type="cellIs" dxfId="33" priority="36" operator="equal">
+      <formula>"Optional"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="39" operator="equal">
-      <formula>"Conditional"</formula>
+    <cfRule type="cellIs" dxfId="32" priority="33" operator="equal">
+      <formula>"Not added"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H11">
-    <cfRule type="cellIs" dxfId="31" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="31" priority="10" operator="equal">
+      <formula>"needs review"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="9" operator="greaterThan">
       <formula>"reviewd"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="10" operator="equal">
-      <formula>"needs review"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H14:H27 H36:H38">
@@ -13496,17 +13496,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:I1 F1:F7">
-    <cfRule type="cellIs" dxfId="27" priority="15" operator="equal">
-      <formula>"Optional"</formula>
+    <cfRule type="cellIs" dxfId="27" priority="18" operator="equal">
+      <formula>"Conditional"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="17" operator="equal">
+      <formula>"Mandatory"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="16" operator="equal">
       <formula>"Recommended"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="17" operator="equal">
-      <formula>"Mandatory"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="18" operator="equal">
-      <formula>"Conditional"</formula>
+    <cfRule type="cellIs" dxfId="24" priority="15" operator="equal">
+      <formula>"Optional"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="6">
@@ -14204,14 +14204,14 @@
     <cfRule type="cellIs" dxfId="19" priority="25" operator="equal">
       <formula>"Optional"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="26" operator="equal">
-      <formula>"Recommended"</formula>
+    <cfRule type="cellIs" dxfId="18" priority="28" operator="equal">
+      <formula>"Conditional"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="17" priority="27" operator="equal">
       <formula>"Mandatory"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="28" operator="equal">
-      <formula>"Conditional"</formula>
+    <cfRule type="cellIs" dxfId="16" priority="26" operator="equal">
+      <formula>"Recommended"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E3">
@@ -14251,25 +14251,25 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:H9 H11:H15 H17:H25 H27:H41 H50:H52">
-    <cfRule type="cellIs" dxfId="5" priority="29" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="30" operator="equal">
+      <formula>"needs review"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="29" operator="greaterThan">
       <formula>"reviewd"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="30" operator="equal">
-      <formula>"needs review"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:I1 F1:F52">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
-      <formula>"Optional"</formula>
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+      <formula>"Conditional"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>"Mandatory"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Recommended"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
-      <formula>"Mandatory"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
-      <formula>"Conditional"</formula>
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"Optional"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="6">
@@ -14312,10 +14312,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F1189FF-E617-AB44-8E2D-7CBBF26DD393}">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14590,6 +14590,14 @@
       </c>
       <c r="B34" t="s">
         <v>732</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>680</v>
+      </c>
+      <c r="B35" t="s">
+        <v>695</v>
       </c>
     </row>
   </sheetData>
@@ -17124,8 +17132,8 @@
   </sheetPr>
   <dimension ref="A1:T49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
@@ -19442,7 +19450,7 @@
   </sheetPr>
   <dimension ref="A1:T60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
@@ -20903,15 +20911,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Status xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e">Draft</Status>
@@ -20921,6 +20920,15 @@
     <TaxCatchAll xmlns="221af607-abea-4d5e-830c-567dcc03c0ec" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -21167,20 +21175,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1A00443-9B7C-473F-A198-CBEB23A0BCC5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16D2CAB5-B21B-4A93-9D82-49FE3E36CF14}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="cfc87205-1831-4b6c-a7b4-76d40079a43e"/>
     <ds:schemaRef ds:uri="221af607-abea-4d5e-830c-567dcc03c0ec"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1A00443-9B7C-473F-A198-CBEB23A0BCC5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>